<commit_message>
alteração da documentação e da ATA com as novas etapas da semana
</commit_message>
<xml_diff>
--- a/ATAs_de_Reuniao/Sprint 2/Semana 2609/Grupo4_ATA_Semana2609.xlsx
+++ b/ATAs_de_Reuniao/Sprint 2/Semana 2609/Grupo4_ATA_Semana2609.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f4fd29038e46714d/Área de Trabalho/SPTECH/Pesquisa e Inovação/Sprint-SPTECH/ATAs_de_Reuniao/Sprint 2/Semana 2609/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miguel\Desktop\sptech\Sprint2\git\Repositorio Sprint2\Sprint-SPTECH\ATAs_de_Reuniao\Sprint 2\Semana 2609\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="255" documentId="13_ncr:1_{57DF1821-0962-4C64-A1D3-54AC52FF73A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6FEB66BA-B53B-4D4C-9C03-C73910CE1D52}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2714820C-4E85-45A7-800F-E6FEBFBC856C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" firstSheet="1" activeTab="1" xr2:uid="{D70EAD62-B489-48DA-AED6-4403B2320B59}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{D70EAD62-B489-48DA-AED6-4403B2320B59}"/>
   </bookViews>
   <sheets>
     <sheet name="BANCO DE DADOS" sheetId="2" state="hidden" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="66">
   <si>
     <t>NOME</t>
   </si>
@@ -150,9 +150,6 @@
     <t xml:space="preserve">DESCRIÇÕES </t>
   </si>
   <si>
-    <t>Foi discutido sobre a organização e atribuição das tarefas pedentes do projeto, decidindo quem as faria. Essa reunião teve como objetivo rever o trabalho já feito pelo grupo anterior.</t>
-  </si>
-  <si>
     <t>Foi discutido sobre a alteração de data de prazos de entrega, junto da discussão, organização e preparo para a apresentação de TI no dia 25/09.</t>
   </si>
   <si>
@@ -232,6 +229,18 @@
   </si>
   <si>
     <t>DIAGRAMA DE NEGÓCIO</t>
+  </si>
+  <si>
+    <t>0210/2024</t>
+  </si>
+  <si>
+    <t>DIAGRAM DE NEGÓCIO</t>
+  </si>
+  <si>
+    <t>INSTALAR MYSQL NA VM LOCAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fechamos a primeira semana (Sprint 2A) com a Sprint Review. Iniciamos a Sprint 2B - foi decidido o Product Owner e Scrum Master, definimos novos objetivo e prazos para o andamento do projeto.  </t>
   </si>
 </sst>
 </file>
@@ -879,6 +888,33 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -930,33 +966,6 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="8" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="8" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="8" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="8" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="8" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="8" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1291,6 +1300,142 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2922,142 +3067,6 @@
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -3072,179 +3081,179 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}" name="Tabela1" displayName="Tabela1" ref="A4:D12" totalsRowShown="0" headerRowDxfId="124" dataDxfId="123" tableBorderDxfId="122">
-  <autoFilter ref="A4:D12" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}" name="Tabela1" displayName="Tabela1" ref="A4:D15" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38" tableBorderDxfId="37">
+  <autoFilter ref="A4:D15" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{304AA193-8246-42D6-B1C9-59B7CDC154B3}" name="O QUE FAZER" dataDxfId="121"/>
-    <tableColumn id="2" xr3:uid="{78AA6BC8-76A1-4FBB-8FD3-BCC5150E3A32}" name="PRAZOS DE ENTREGA" dataDxfId="120"/>
-    <tableColumn id="3" xr3:uid="{2F5C5138-DE27-4C39-AB08-9838AABC1D77}" name="RESPONSAVEL" dataDxfId="119"/>
-    <tableColumn id="4" xr3:uid="{D7517C3D-D3B1-4731-934F-9B5B368C5317}" name="SITUAÇÃO" dataDxfId="118"/>
+    <tableColumn id="1" xr3:uid="{304AA193-8246-42D6-B1C9-59B7CDC154B3}" name="O QUE FAZER" dataDxfId="36"/>
+    <tableColumn id="2" xr3:uid="{78AA6BC8-76A1-4FBB-8FD3-BCC5150E3A32}" name="PRAZOS DE ENTREGA" dataDxfId="35"/>
+    <tableColumn id="3" xr3:uid="{2F5C5138-DE27-4C39-AB08-9838AABC1D77}" name="RESPONSAVEL" dataDxfId="34"/>
+    <tableColumn id="4" xr3:uid="{D7517C3D-D3B1-4731-934F-9B5B368C5317}" name="SITUAÇÃO" dataDxfId="33"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{5A356893-9A8B-4B13-8C28-51E182146249}" name="Tabela257911" displayName="Tabela257911" ref="A20:C26" totalsRowShown="0" headerRowDxfId="65" dataDxfId="64" tableBorderDxfId="63">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{5A356893-9A8B-4B13-8C28-51E182146249}" name="Tabela257911" displayName="Tabela257911" ref="A20:C26" totalsRowShown="0" headerRowDxfId="72" dataDxfId="71" tableBorderDxfId="70">
   <autoFilter ref="A20:C26" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{139E8E28-282E-4954-A42E-FF13F888D8CB}" name="NOME" dataDxfId="62"/>
-    <tableColumn id="2" xr3:uid="{2D2F98D9-24BC-48E1-977F-50AADAAFFCD7}" name="PARTICIPAÇÃO" dataDxfId="61"/>
-    <tableColumn id="3" xr3:uid="{ECE86497-A781-4678-B780-5FE8694A399F}" name="JUSTIFICATIVA" dataDxfId="60"/>
+    <tableColumn id="1" xr3:uid="{139E8E28-282E-4954-A42E-FF13F888D8CB}" name="NOME" dataDxfId="69"/>
+    <tableColumn id="2" xr3:uid="{2D2F98D9-24BC-48E1-977F-50AADAAFFCD7}" name="PARTICIPAÇÃO" dataDxfId="68"/>
+    <tableColumn id="3" xr3:uid="{ECE86497-A781-4678-B780-5FE8694A399F}" name="JUSTIFICATIVA" dataDxfId="67"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{2886C088-B6C9-41EE-96FE-A8E0AA69BC21}" name="Tabela14681012" displayName="Tabela14681012" ref="A4:D11" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58" tableBorderDxfId="57">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{2886C088-B6C9-41EE-96FE-A8E0AA69BC21}" name="Tabela14681012" displayName="Tabela14681012" ref="A4:D11" totalsRowShown="0" headerRowDxfId="66" dataDxfId="65" tableBorderDxfId="64">
   <autoFilter ref="A4:D11" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{6BA21BAE-9078-42C7-822B-52A293391852}" name="O QUE FAZER" dataDxfId="56"/>
-    <tableColumn id="2" xr3:uid="{F8A78184-BA68-4990-9C19-32D05CA74AA6}" name="PRAZOS DE ENTREGA" dataDxfId="55"/>
-    <tableColumn id="3" xr3:uid="{3E9EBBE9-2298-4066-AADB-C4F83F09344A}" name="RESPONSAVEL" dataDxfId="54"/>
-    <tableColumn id="4" xr3:uid="{8377538D-9891-4CF2-87F8-DD620412251C}" name="SITUAÇÃO" dataDxfId="53"/>
+    <tableColumn id="1" xr3:uid="{6BA21BAE-9078-42C7-822B-52A293391852}" name="O QUE FAZER" dataDxfId="63"/>
+    <tableColumn id="2" xr3:uid="{F8A78184-BA68-4990-9C19-32D05CA74AA6}" name="PRAZOS DE ENTREGA" dataDxfId="62"/>
+    <tableColumn id="3" xr3:uid="{3E9EBBE9-2298-4066-AADB-C4F83F09344A}" name="RESPONSAVEL" dataDxfId="61"/>
+    <tableColumn id="4" xr3:uid="{8377538D-9891-4CF2-87F8-DD620412251C}" name="SITUAÇÃO" dataDxfId="60"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{DE61209C-5FFF-4AB7-A88E-0738F2BE2FD2}" name="Tabela25791113" displayName="Tabela25791113" ref="A20:C26" totalsRowShown="0" headerRowDxfId="52" dataDxfId="51" tableBorderDxfId="50">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{DE61209C-5FFF-4AB7-A88E-0738F2BE2FD2}" name="Tabela25791113" displayName="Tabela25791113" ref="A20:C26" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58" tableBorderDxfId="57">
   <autoFilter ref="A20:C26" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{58AE96D9-C80D-4487-A8FD-25CA95399084}" name="NOME" dataDxfId="49"/>
-    <tableColumn id="2" xr3:uid="{DA2DAD6E-8AC8-4A3C-A3D5-3586B85EFCC9}" name="PARTICIPAÇÃO" dataDxfId="48"/>
-    <tableColumn id="3" xr3:uid="{DE52FF26-9E09-4FB8-B756-26BD1C24F803}" name="JUSTIFICATIVA" dataDxfId="47"/>
+    <tableColumn id="1" xr3:uid="{58AE96D9-C80D-4487-A8FD-25CA95399084}" name="NOME" dataDxfId="56"/>
+    <tableColumn id="2" xr3:uid="{DA2DAD6E-8AC8-4A3C-A3D5-3586B85EFCC9}" name="PARTICIPAÇÃO" dataDxfId="55"/>
+    <tableColumn id="3" xr3:uid="{DE52FF26-9E09-4FB8-B756-26BD1C24F803}" name="JUSTIFICATIVA" dataDxfId="54"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{5D051227-CD21-44B9-B384-BB058BE2415C}" name="Tabela1468101214" displayName="Tabela1468101214" ref="A7:D11" totalsRowShown="0" headerRowDxfId="46" dataDxfId="45" tableBorderDxfId="44">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{5D051227-CD21-44B9-B384-BB058BE2415C}" name="Tabela1468101214" displayName="Tabela1468101214" ref="A7:D11" totalsRowShown="0" headerRowDxfId="53" dataDxfId="52" tableBorderDxfId="51">
   <autoFilter ref="A7:D11" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{60DF006F-DEC1-44B4-B650-77AA681BD053}" name="O QUE FAZER" dataDxfId="43"/>
-    <tableColumn id="2" xr3:uid="{B1C8A4D2-1A12-4627-B02D-C93638B8E22A}" name="PRAZOS DE ENTREGA" dataDxfId="42"/>
-    <tableColumn id="3" xr3:uid="{F9358C8C-A26D-4EC1-88FC-FC7F9E7F7126}" name="RESPONSAVEL" dataDxfId="41"/>
-    <tableColumn id="4" xr3:uid="{4EFF508D-FF9C-4340-8D19-B4DDBABBA711}" name="SITUAÇÃO" dataDxfId="40"/>
+    <tableColumn id="1" xr3:uid="{60DF006F-DEC1-44B4-B650-77AA681BD053}" name="O QUE FAZER" dataDxfId="50"/>
+    <tableColumn id="2" xr3:uid="{B1C8A4D2-1A12-4627-B02D-C93638B8E22A}" name="PRAZOS DE ENTREGA" dataDxfId="49"/>
+    <tableColumn id="3" xr3:uid="{F9358C8C-A26D-4EC1-88FC-FC7F9E7F7126}" name="RESPONSAVEL" dataDxfId="48"/>
+    <tableColumn id="4" xr3:uid="{4EFF508D-FF9C-4340-8D19-B4DDBABBA711}" name="SITUAÇÃO" dataDxfId="47"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{3230F418-B85A-4611-A179-37FFDCA32F80}" name="Tabela146810121418" displayName="Tabela146810121418" ref="F7:I17" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38" tableBorderDxfId="37">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{3230F418-B85A-4611-A179-37FFDCA32F80}" name="Tabela146810121418" displayName="Tabela146810121418" ref="F7:I17" totalsRowShown="0" headerRowDxfId="46" dataDxfId="45" tableBorderDxfId="44">
   <autoFilter ref="F7:I17" xr:uid="{3230F418-B85A-4611-A179-37FFDCA32F80}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="F8:I17">
     <sortCondition ref="H7:H17"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{8C9AFF73-6E6E-4E4C-A377-C37849BB14F7}" name="O QUE FAZER" dataDxfId="36"/>
-    <tableColumn id="2" xr3:uid="{591F032C-5225-4191-A54B-DEF3830ED570}" name="PRAZOS DE ENTREGA" dataDxfId="35"/>
-    <tableColumn id="3" xr3:uid="{E796F4BB-4BEF-4028-8B36-D1E4B9650852}" name="RESPONSAVEL" dataDxfId="34"/>
-    <tableColumn id="4" xr3:uid="{D6A8EF5F-93E1-4C3A-A560-545F459C0602}" name="SITUAÇÃO" dataDxfId="33"/>
+    <tableColumn id="1" xr3:uid="{8C9AFF73-6E6E-4E4C-A377-C37849BB14F7}" name="O QUE FAZER" dataDxfId="43"/>
+    <tableColumn id="2" xr3:uid="{591F032C-5225-4191-A54B-DEF3830ED570}" name="PRAZOS DE ENTREGA" dataDxfId="42"/>
+    <tableColumn id="3" xr3:uid="{E796F4BB-4BEF-4028-8B36-D1E4B9650852}" name="RESPONSAVEL" dataDxfId="41"/>
+    <tableColumn id="4" xr3:uid="{D6A8EF5F-93E1-4C3A-A560-545F459C0602}" name="SITUAÇÃO" dataDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}" name="Tabela2" displayName="Tabela2" ref="A21:C27" totalsRowShown="0" headerRowDxfId="117" dataDxfId="116" tableBorderDxfId="115">
-  <autoFilter ref="A21:C27" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}" name="Tabela2" displayName="Tabela2" ref="A24:C30" totalsRowShown="0" headerRowDxfId="124" dataDxfId="123" tableBorderDxfId="122">
+  <autoFilter ref="A24:C30" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{EE178185-CFC7-4789-A834-552542FE9234}" name="NOME" dataDxfId="114"/>
-    <tableColumn id="2" xr3:uid="{441E3B93-F7D3-4DEA-9A31-B2AAF98FF93F}" name="PARTICIPAÇÃO" dataDxfId="113"/>
-    <tableColumn id="3" xr3:uid="{63718DE3-E919-4841-AE71-A3377F141C19}" name="JUSTIFICATIVA" dataDxfId="112"/>
+    <tableColumn id="1" xr3:uid="{EE178185-CFC7-4789-A834-552542FE9234}" name="NOME" dataDxfId="121"/>
+    <tableColumn id="2" xr3:uid="{441E3B93-F7D3-4DEA-9A31-B2AAF98FF93F}" name="PARTICIPAÇÃO" dataDxfId="120"/>
+    <tableColumn id="3" xr3:uid="{63718DE3-E919-4841-AE71-A3377F141C19}" name="JUSTIFICATIVA" dataDxfId="119"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4F95CA63-C4C7-4EB6-955D-ED05E38937E0}" name="Tabela14" displayName="Tabela14" ref="A4:D12" totalsRowShown="0" headerRowDxfId="111" dataDxfId="110" tableBorderDxfId="109">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4F95CA63-C4C7-4EB6-955D-ED05E38937E0}" name="Tabela14" displayName="Tabela14" ref="A4:D12" totalsRowShown="0" headerRowDxfId="118" dataDxfId="117" tableBorderDxfId="116">
   <autoFilter ref="A4:D12" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{A7FACD00-2B31-4019-A56E-65C773E3AA49}" name="O QUE FAZER" dataDxfId="108"/>
-    <tableColumn id="2" xr3:uid="{9BDA6AAE-D8A7-451F-BDDB-C505248F0ED2}" name="PRAZOS DE ENTREGA" dataDxfId="107"/>
-    <tableColumn id="3" xr3:uid="{687F7861-FC98-4254-AEF3-B5108163FD30}" name="RESPONSAVEL" dataDxfId="106"/>
-    <tableColumn id="4" xr3:uid="{4CE5089F-14AC-4902-9804-474D2482620F}" name="SITUAÇÃO" dataDxfId="105"/>
+    <tableColumn id="1" xr3:uid="{A7FACD00-2B31-4019-A56E-65C773E3AA49}" name="O QUE FAZER" dataDxfId="115"/>
+    <tableColumn id="2" xr3:uid="{9BDA6AAE-D8A7-451F-BDDB-C505248F0ED2}" name="PRAZOS DE ENTREGA" dataDxfId="114"/>
+    <tableColumn id="3" xr3:uid="{687F7861-FC98-4254-AEF3-B5108163FD30}" name="RESPONSAVEL" dataDxfId="113"/>
+    <tableColumn id="4" xr3:uid="{4CE5089F-14AC-4902-9804-474D2482620F}" name="SITUAÇÃO" dataDxfId="112"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{233261E1-B78E-4980-89B4-ECD8BA87118E}" name="Tabela25" displayName="Tabela25" ref="A21:C27" totalsRowShown="0" headerRowDxfId="104" dataDxfId="103" tableBorderDxfId="102">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{233261E1-B78E-4980-89B4-ECD8BA87118E}" name="Tabela25" displayName="Tabela25" ref="A21:C27" totalsRowShown="0" headerRowDxfId="111" dataDxfId="110" tableBorderDxfId="109">
   <autoFilter ref="A21:C27" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{BEAC01C6-9DF6-4F3E-AE22-4F43300E8D20}" name="NOME" dataDxfId="101"/>
-    <tableColumn id="2" xr3:uid="{22B38C5A-614F-40A6-9C22-AF72FFB3E3B6}" name="PARTICIPAÇÃO" dataDxfId="100"/>
-    <tableColumn id="3" xr3:uid="{571C9057-2775-4114-AC19-407CD64A10AE}" name="JUSTIFICATIVA" dataDxfId="99"/>
+    <tableColumn id="1" xr3:uid="{BEAC01C6-9DF6-4F3E-AE22-4F43300E8D20}" name="NOME" dataDxfId="108"/>
+    <tableColumn id="2" xr3:uid="{22B38C5A-614F-40A6-9C22-AF72FFB3E3B6}" name="PARTICIPAÇÃO" dataDxfId="107"/>
+    <tableColumn id="3" xr3:uid="{571C9057-2775-4114-AC19-407CD64A10AE}" name="JUSTIFICATIVA" dataDxfId="106"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{0D24B965-B4D0-472F-8B6D-931251406FD0}" name="Tabela146" displayName="Tabela146" ref="A4:D11" totalsRowShown="0" headerRowDxfId="98" dataDxfId="97" tableBorderDxfId="96">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{0D24B965-B4D0-472F-8B6D-931251406FD0}" name="Tabela146" displayName="Tabela146" ref="A4:D11" totalsRowShown="0" headerRowDxfId="105" dataDxfId="104" tableBorderDxfId="103">
   <autoFilter ref="A4:D11" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{4DB758E7-A5B8-4A9F-BCA4-563D8A6C3B6B}" name="O QUE FAZER" dataDxfId="95"/>
-    <tableColumn id="2" xr3:uid="{7EF6621B-1CC5-4635-882A-1B8E78882552}" name="PRAZOS DE ENTREGA" dataDxfId="94"/>
-    <tableColumn id="3" xr3:uid="{9F41E9D9-BCC0-44A3-9CEA-7746D12A0832}" name="RESPONSAVEL" dataDxfId="93"/>
-    <tableColumn id="4" xr3:uid="{C11A8EA2-A0AA-4B12-9B04-E8A9ADB179F1}" name="SITUAÇÃO" dataDxfId="92"/>
+    <tableColumn id="1" xr3:uid="{4DB758E7-A5B8-4A9F-BCA4-563D8A6C3B6B}" name="O QUE FAZER" dataDxfId="102"/>
+    <tableColumn id="2" xr3:uid="{7EF6621B-1CC5-4635-882A-1B8E78882552}" name="PRAZOS DE ENTREGA" dataDxfId="101"/>
+    <tableColumn id="3" xr3:uid="{9F41E9D9-BCC0-44A3-9CEA-7746D12A0832}" name="RESPONSAVEL" dataDxfId="100"/>
+    <tableColumn id="4" xr3:uid="{C11A8EA2-A0AA-4B12-9B04-E8A9ADB179F1}" name="SITUAÇÃO" dataDxfId="99"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{42551E1E-5CD7-4F6A-843E-1CBF547215BB}" name="Tabela257" displayName="Tabela257" ref="A20:C26" totalsRowShown="0" headerRowDxfId="91" dataDxfId="90" tableBorderDxfId="89">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{42551E1E-5CD7-4F6A-843E-1CBF547215BB}" name="Tabela257" displayName="Tabela257" ref="A20:C26" totalsRowShown="0" headerRowDxfId="98" dataDxfId="97" tableBorderDxfId="96">
   <autoFilter ref="A20:C26" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{8E8C9FBB-2737-4F1B-8662-DC7B8E05FE39}" name="NOME" dataDxfId="88"/>
-    <tableColumn id="2" xr3:uid="{5E83EC73-7E41-45E0-AF4D-68FC709F651A}" name="PARTICIPAÇÃO" dataDxfId="87"/>
-    <tableColumn id="3" xr3:uid="{87E32803-B844-4BA6-BF0A-17270B237D48}" name="JUSTIFICATIVA" dataDxfId="86"/>
+    <tableColumn id="1" xr3:uid="{8E8C9FBB-2737-4F1B-8662-DC7B8E05FE39}" name="NOME" dataDxfId="95"/>
+    <tableColumn id="2" xr3:uid="{5E83EC73-7E41-45E0-AF4D-68FC709F651A}" name="PARTICIPAÇÃO" dataDxfId="94"/>
+    <tableColumn id="3" xr3:uid="{87E32803-B844-4BA6-BF0A-17270B237D48}" name="JUSTIFICATIVA" dataDxfId="93"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{2973F3F9-B8D9-4E9E-BA21-0F7855C23630}" name="Tabela1468" displayName="Tabela1468" ref="A4:D11" totalsRowShown="0" headerRowDxfId="85" dataDxfId="84" tableBorderDxfId="83">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{2973F3F9-B8D9-4E9E-BA21-0F7855C23630}" name="Tabela1468" displayName="Tabela1468" ref="A4:D11" totalsRowShown="0" headerRowDxfId="92" dataDxfId="91" tableBorderDxfId="90">
   <autoFilter ref="A4:D11" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{11646B81-A121-4FA2-893E-362D3A1A52F0}" name="O QUE FAZER" dataDxfId="82"/>
-    <tableColumn id="2" xr3:uid="{4833C381-32BB-4B40-AD0C-A01805D370D5}" name="PRAZOS DE ENTREGA" dataDxfId="81"/>
-    <tableColumn id="3" xr3:uid="{B9FED99E-7EE5-453D-998F-758D676F139A}" name="RESPONSAVEL" dataDxfId="80"/>
-    <tableColumn id="4" xr3:uid="{C9B39C91-0344-4E7A-847B-74EBED4B2F53}" name="SITUAÇÃO" dataDxfId="79"/>
+    <tableColumn id="1" xr3:uid="{11646B81-A121-4FA2-893E-362D3A1A52F0}" name="O QUE FAZER" dataDxfId="89"/>
+    <tableColumn id="2" xr3:uid="{4833C381-32BB-4B40-AD0C-A01805D370D5}" name="PRAZOS DE ENTREGA" dataDxfId="88"/>
+    <tableColumn id="3" xr3:uid="{B9FED99E-7EE5-453D-998F-758D676F139A}" name="RESPONSAVEL" dataDxfId="87"/>
+    <tableColumn id="4" xr3:uid="{C9B39C91-0344-4E7A-847B-74EBED4B2F53}" name="SITUAÇÃO" dataDxfId="86"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{3C9D5C14-8487-4611-B27F-7F4ABC950782}" name="Tabela2579" displayName="Tabela2579" ref="A20:C26" totalsRowShown="0" headerRowDxfId="78" dataDxfId="77" tableBorderDxfId="76">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{3C9D5C14-8487-4611-B27F-7F4ABC950782}" name="Tabela2579" displayName="Tabela2579" ref="A20:C26" totalsRowShown="0" headerRowDxfId="85" dataDxfId="84" tableBorderDxfId="83">
   <autoFilter ref="A20:C26" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{66272961-D89D-4DD2-807F-D10CF138519D}" name="NOME" dataDxfId="75"/>
-    <tableColumn id="2" xr3:uid="{9700B9DF-18DC-4FF9-B87F-CA8E809DFE18}" name="PARTICIPAÇÃO" dataDxfId="74"/>
-    <tableColumn id="3" xr3:uid="{336A4CF9-2C48-4740-BBCF-05EBC653EB59}" name="JUSTIFICATIVA" dataDxfId="73"/>
+    <tableColumn id="1" xr3:uid="{66272961-D89D-4DD2-807F-D10CF138519D}" name="NOME" dataDxfId="82"/>
+    <tableColumn id="2" xr3:uid="{9700B9DF-18DC-4FF9-B87F-CA8E809DFE18}" name="PARTICIPAÇÃO" dataDxfId="81"/>
+    <tableColumn id="3" xr3:uid="{336A4CF9-2C48-4740-BBCF-05EBC653EB59}" name="JUSTIFICATIVA" dataDxfId="80"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{4239FFAB-7F81-4D5D-933C-45DFBF3605AD}" name="Tabela146810" displayName="Tabela146810" ref="A4:D11" totalsRowShown="0" headerRowDxfId="72" dataDxfId="71" tableBorderDxfId="70">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{4239FFAB-7F81-4D5D-933C-45DFBF3605AD}" name="Tabela146810" displayName="Tabela146810" ref="A4:D11" totalsRowShown="0" headerRowDxfId="79" dataDxfId="78" tableBorderDxfId="77">
   <autoFilter ref="A4:D11" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{04C4A5A4-6229-4505-8F11-B7E824AC1473}" name="O QUE FAZER" dataDxfId="69"/>
-    <tableColumn id="2" xr3:uid="{E21C73CF-DFCA-4323-8C97-CBB757FA2560}" name="PRAZOS DE ENTREGA" dataDxfId="68"/>
-    <tableColumn id="3" xr3:uid="{9A31040F-148F-42BE-8FBC-5FCB2398EFB4}" name="RESPONSAVEL" dataDxfId="67"/>
-    <tableColumn id="4" xr3:uid="{4756F678-1E57-4686-8D68-E8BB92990CAB}" name="SITUAÇÃO" dataDxfId="66"/>
+    <tableColumn id="1" xr3:uid="{04C4A5A4-6229-4505-8F11-B7E824AC1473}" name="O QUE FAZER" dataDxfId="76"/>
+    <tableColumn id="2" xr3:uid="{E21C73CF-DFCA-4323-8C97-CBB757FA2560}" name="PRAZOS DE ENTREGA" dataDxfId="75"/>
+    <tableColumn id="3" xr3:uid="{9A31040F-148F-42BE-8FBC-5FCB2398EFB4}" name="RESPONSAVEL" dataDxfId="74"/>
+    <tableColumn id="4" xr3:uid="{4756F678-1E57-4686-8D68-E8BB92990CAB}" name="SITUAÇÃO" dataDxfId="73"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3573,12 +3582,12 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="18.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -3589,7 +3598,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -3600,7 +3609,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>18</v>
       </c>
@@ -3612,23 +3621,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{440FA3E8-7F0D-4287-A3E8-76B61D68049B}">
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.453125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.08984375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.453125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.453125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.08984375" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.90625" style="1"/>
+    <col min="1" max="1" width="34.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>24</v>
       </c>
@@ -3636,8 +3645,8 @@
       <c r="C1" s="25"/>
       <c r="D1" s="26"/>
     </row>
-    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="24" t="s">
         <v>2</v>
       </c>
@@ -3649,7 +3658,7 @@
       <c r="H3"/>
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -3667,12 +3676,12 @@
       <c r="H4"/>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="B5" s="6">
-        <v>45556</v>
+        <v>45567</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>8</v>
@@ -3685,242 +3694,285 @@
       <c r="H5"/>
       <c r="I5"/>
     </row>
-    <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6" s="6">
-        <v>45555</v>
+        <v>32</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>62</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="6">
-        <v>45554</v>
+        <v>49</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>62</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="6">
-        <v>45559</v>
+      <c r="B8" s="6" t="s">
+        <v>62</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9" s="6">
-        <v>45555</v>
+        <v>48</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>62</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="6">
-        <v>45559</v>
+        <v>30</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>62</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" s="6">
-        <v>45555</v>
+        <v>46</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>62</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="5"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-    </row>
-    <row r="13" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="14" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="24" t="s">
+    <row r="12" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="5"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+    </row>
+    <row r="16" spans="1:9" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="1:4" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="25"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="26"/>
-    </row>
-    <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="B15" s="31"/>
-      <c r="C15" s="31"/>
-      <c r="D15" s="32"/>
-    </row>
-    <row r="16" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="33"/>
-      <c r="B16" s="34"/>
-      <c r="C16" s="34"/>
-      <c r="D16" s="35"/>
-    </row>
-    <row r="17" spans="1:4" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="33"/>
-      <c r="B17" s="34"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="35"/>
-    </row>
-    <row r="18" spans="1:4" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="36"/>
-      <c r="B18" s="37"/>
-      <c r="C18" s="37"/>
-      <c r="D18" s="38"/>
-    </row>
-    <row r="19" spans="1:4" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="20" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="27" t="s">
+      <c r="B17" s="25"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="26"/>
+    </row>
+    <row r="18" spans="1:4" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="B18" s="31"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="32"/>
+    </row>
+    <row r="19" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="33"/>
+      <c r="B19" s="34"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="35"/>
+    </row>
+    <row r="20" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="33"/>
+      <c r="B20" s="34"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="35"/>
+    </row>
+    <row r="21" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="36"/>
+      <c r="B21" s="37"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="38"/>
+    </row>
+    <row r="22" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="28"/>
-      <c r="C20" s="29"/>
-      <c r="D20" s="12" t="s">
+      <c r="B23" s="28"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="10" t="s">
+    <row r="24" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B24" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C24" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D21" s="4">
+      <c r="D24" s="4">
         <v>45561</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="2" t="s">
+    <row r="25" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22" s="5"/>
-      <c r="D22" s="12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23" s="5"/>
-      <c r="D23" s="7">
-        <v>0.68819444444444444</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C24" s="5"/>
-      <c r="D24" s="12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C25" s="5"/>
-      <c r="D25" s="8">
-        <v>0.69930555555555551</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D25" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C26" s="5"/>
-      <c r="D26" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D26" s="7">
+        <v>0.68819444444444444</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C27" s="5"/>
-      <c r="D27" s="3">
-        <f>IF(D25="","",D25-D23)</f>
+      <c r="D27" s="12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C28" s="5"/>
+      <c r="D28" s="8">
+        <v>0.69930555555555551</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" s="5"/>
+      <c r="D29" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C30" s="5"/>
+      <c r="D30" s="3">
+        <f>IF(D28="","",D28-D26)</f>
         <v>1.1111111111111072E-2</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A22:C27">
-    <sortCondition ref="A21:A27"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A25:C30">
+    <sortCondition ref="A24:A30"/>
   </sortState>
   <mergeCells count="5">
     <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="A14:D14"/>
-    <mergeCell ref="A15:D18"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A18:D21"/>
     <mergeCell ref="A1:D1"/>
   </mergeCells>
-  <conditionalFormatting sqref="B22:B27">
+  <phoneticPr fontId="6" type="noConversion"/>
+  <conditionalFormatting sqref="B25:B30">
     <cfRule type="cellIs" dxfId="32" priority="4" operator="equal">
       <formula>"AUSENTE"</formula>
     </cfRule>
@@ -3928,7 +3980,7 @@
       <formula>"PRESENTE"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D5:D11">
+  <conditionalFormatting sqref="D5:D14">
     <cfRule type="cellIs" dxfId="30" priority="1" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
@@ -3940,8 +3992,8 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C12" xr:uid="{3324AE11-71AC-4AA1-B23A-F31A79FB27A6}">
-      <formula1>$A$22:$A$27</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C15" xr:uid="{3324AE11-71AC-4AA1-B23A-F31A79FB27A6}">
+      <formula1>$A$25:$A$30</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -3957,13 +4009,13 @@
           <x14:formula1>
             <xm:f>'BANCO DE DADOS'!$A$1:$A$2</xm:f>
           </x14:formula1>
-          <xm:sqref>B22:B27</xm:sqref>
+          <xm:sqref>B25:B30</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{084CBBA6-F302-47EA-9F18-F0E3EAEF0A1E}">
           <x14:formula1>
             <xm:f>'BANCO DE DADOS'!$B$1:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>D5:D12</xm:sqref>
+          <xm:sqref>D5:D15</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3979,17 +4031,17 @@
       <selection activeCell="E16" activeCellId="1" sqref="E27 E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.453125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.08984375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.453125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.453125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.08984375" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.90625" style="1"/>
+    <col min="1" max="1" width="34.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>24</v>
       </c>
@@ -3997,8 +4049,8 @@
       <c r="C1" s="25"/>
       <c r="D1" s="26"/>
     </row>
-    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="24" t="s">
         <v>2</v>
       </c>
@@ -4010,7 +4062,7 @@
       <c r="H3"/>
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -4028,7 +4080,7 @@
       <c r="H4"/>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>27</v>
       </c>
@@ -4046,7 +4098,7 @@
       <c r="H5"/>
       <c r="I5"/>
     </row>
-    <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>28</v>
       </c>
@@ -4060,7 +4112,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>29</v>
       </c>
@@ -4074,7 +4126,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>30</v>
       </c>
@@ -4088,7 +4140,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>31</v>
       </c>
@@ -4102,7 +4154,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>32</v>
       </c>
@@ -4116,7 +4168,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>33</v>
       </c>
@@ -4130,14 +4182,14 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="6"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
     </row>
-    <row r="13" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="14" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="24" t="s">
         <v>34</v>
       </c>
@@ -4145,34 +4197,34 @@
       <c r="C14" s="25"/>
       <c r="D14" s="26"/>
     </row>
-    <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B15" s="31"/>
       <c r="C15" s="31"/>
       <c r="D15" s="32"/>
     </row>
-    <row r="16" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="33"/>
       <c r="B16" s="34"/>
       <c r="C16" s="34"/>
       <c r="D16" s="35"/>
     </row>
-    <row r="17" spans="1:5" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="33"/>
       <c r="B17" s="34"/>
       <c r="C17" s="34"/>
       <c r="D17" s="35"/>
     </row>
-    <row r="18" spans="1:5" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:5" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="36"/>
       <c r="B18" s="37"/>
       <c r="C18" s="37"/>
       <c r="D18" s="38"/>
     </row>
-    <row r="19" spans="1:5" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="20" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:5" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="27" t="s">
         <v>19</v>
       </c>
@@ -4182,7 +4234,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
         <v>0</v>
       </c>
@@ -4196,7 +4248,7 @@
         <v>45554</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:5" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>8</v>
       </c>
@@ -4208,7 +4260,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:5" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>9</v>
       </c>
@@ -4220,7 +4272,7 @@
         <v>0.69444444444444442</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:5" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>10</v>
       </c>
@@ -4232,7 +4284,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:5" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>11</v>
       </c>
@@ -4244,7 +4296,7 @@
         <v>0.70694444444444449</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:5" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>12</v>
       </c>
@@ -4256,7 +4308,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:5" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>13</v>
       </c>
@@ -4338,17 +4390,17 @@
       <selection activeCell="A14" sqref="A14:D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.453125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.08984375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.453125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.453125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.08984375" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.90625" style="1"/>
+    <col min="1" max="1" width="34.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>24</v>
       </c>
@@ -4356,8 +4408,8 @@
       <c r="C1" s="25"/>
       <c r="D1" s="26"/>
     </row>
-    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="24" t="s">
         <v>2</v>
       </c>
@@ -4369,7 +4421,7 @@
       <c r="H3"/>
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -4387,7 +4439,7 @@
       <c r="H4"/>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>28</v>
       </c>
@@ -4401,7 +4453,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>30</v>
       </c>
@@ -4415,7 +4467,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>31</v>
       </c>
@@ -4429,7 +4481,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>32</v>
       </c>
@@ -4443,7 +4495,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>33</v>
       </c>
@@ -4457,9 +4509,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B10" s="6">
         <v>45558</v>
@@ -4471,14 +4523,14 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="6"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
     </row>
-    <row r="12" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="13" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="24" t="s">
         <v>34</v>
       </c>
@@ -4486,34 +4538,34 @@
       <c r="C13" s="25"/>
       <c r="D13" s="26"/>
     </row>
-    <row r="14" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B14" s="31"/>
       <c r="C14" s="31"/>
       <c r="D14" s="32"/>
     </row>
-    <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="33"/>
       <c r="B15" s="34"/>
       <c r="C15" s="34"/>
       <c r="D15" s="35"/>
     </row>
-    <row r="16" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="33"/>
       <c r="B16" s="34"/>
       <c r="C16" s="34"/>
       <c r="D16" s="35"/>
     </row>
-    <row r="17" spans="1:5" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:5" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="36"/>
       <c r="B17" s="37"/>
       <c r="C17" s="37"/>
       <c r="D17" s="38"/>
     </row>
-    <row r="18" spans="1:5" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="19" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:5" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="27" t="s">
         <v>19</v>
       </c>
@@ -4523,7 +4575,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
         <v>0</v>
       </c>
@@ -4537,7 +4589,7 @@
         <v>45556</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:5" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>8</v>
       </c>
@@ -4549,7 +4601,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:5" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>9</v>
       </c>
@@ -4561,7 +4613,7 @@
         <v>0.41875000000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:5" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>10</v>
       </c>
@@ -4573,7 +4625,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:5" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>11</v>
       </c>
@@ -4585,7 +4637,7 @@
         <v>0.42499999999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:5" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>12</v>
       </c>
@@ -4597,7 +4649,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:5" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>13</v>
       </c>
@@ -4679,17 +4731,17 @@
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.453125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.08984375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.453125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.453125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.08984375" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.90625" style="1"/>
+    <col min="1" max="1" width="34.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>24</v>
       </c>
@@ -4697,8 +4749,8 @@
       <c r="C1" s="25"/>
       <c r="D1" s="26"/>
     </row>
-    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="24" t="s">
         <v>2</v>
       </c>
@@ -4710,7 +4762,7 @@
       <c r="H3"/>
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -4728,7 +4780,7 @@
       <c r="H4"/>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>28</v>
       </c>
@@ -4742,7 +4794,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>30</v>
       </c>
@@ -4756,7 +4808,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>31</v>
       </c>
@@ -4770,7 +4822,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>32</v>
       </c>
@@ -4784,7 +4836,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>33</v>
       </c>
@@ -4798,9 +4850,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B10" s="6">
         <v>45558</v>
@@ -4812,14 +4864,14 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="6"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
     </row>
-    <row r="12" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="13" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="24" t="s">
         <v>34</v>
       </c>
@@ -4827,34 +4879,34 @@
       <c r="C13" s="25"/>
       <c r="D13" s="26"/>
     </row>
-    <row r="14" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B14" s="31"/>
       <c r="C14" s="31"/>
       <c r="D14" s="32"/>
     </row>
-    <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="33"/>
       <c r="B15" s="34"/>
       <c r="C15" s="34"/>
       <c r="D15" s="35"/>
     </row>
-    <row r="16" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="33"/>
       <c r="B16" s="34"/>
       <c r="C16" s="34"/>
       <c r="D16" s="35"/>
     </row>
-    <row r="17" spans="1:5" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:5" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="36"/>
       <c r="B17" s="37"/>
       <c r="C17" s="37"/>
       <c r="D17" s="38"/>
     </row>
-    <row r="18" spans="1:5" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="19" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:5" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="27" t="s">
         <v>19</v>
       </c>
@@ -4864,7 +4916,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
         <v>0</v>
       </c>
@@ -4878,7 +4930,7 @@
         <v>45558</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:5" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>8</v>
       </c>
@@ -4890,7 +4942,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:5" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>9</v>
       </c>
@@ -4902,7 +4954,7 @@
         <v>0.6958333333333333</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:5" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>10</v>
       </c>
@@ -4914,7 +4966,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:5" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>11</v>
       </c>
@@ -4926,7 +4978,7 @@
         <v>0.70138888888888884</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:5" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>12</v>
       </c>
@@ -4938,7 +4990,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:5" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>13</v>
       </c>
@@ -5020,17 +5072,17 @@
       <selection activeCell="A14" sqref="A14:D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.453125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.08984375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.453125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.453125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.08984375" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.90625" style="1"/>
+    <col min="1" max="1" width="34.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>24</v>
       </c>
@@ -5038,8 +5090,8 @@
       <c r="C1" s="25"/>
       <c r="D1" s="26"/>
     </row>
-    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="24" t="s">
         <v>2</v>
       </c>
@@ -5051,7 +5103,7 @@
       <c r="H3"/>
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -5069,7 +5121,7 @@
       <c r="H4"/>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>28</v>
       </c>
@@ -5083,7 +5135,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>30</v>
       </c>
@@ -5097,7 +5149,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>31</v>
       </c>
@@ -5111,7 +5163,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>32</v>
       </c>
@@ -5125,7 +5177,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>33</v>
       </c>
@@ -5139,9 +5191,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B10" s="6">
         <v>45558</v>
@@ -5153,14 +5205,14 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="6"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
     </row>
-    <row r="12" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="13" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="24" t="s">
         <v>34</v>
       </c>
@@ -5168,34 +5220,34 @@
       <c r="C13" s="25"/>
       <c r="D13" s="26"/>
     </row>
-    <row r="14" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B14" s="31"/>
       <c r="C14" s="31"/>
       <c r="D14" s="32"/>
     </row>
-    <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="33"/>
       <c r="B15" s="34"/>
       <c r="C15" s="34"/>
       <c r="D15" s="35"/>
     </row>
-    <row r="16" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="33"/>
       <c r="B16" s="34"/>
       <c r="C16" s="34"/>
       <c r="D16" s="35"/>
     </row>
-    <row r="17" spans="1:5" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:5" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="36"/>
       <c r="B17" s="37"/>
       <c r="C17" s="37"/>
       <c r="D17" s="38"/>
     </row>
-    <row r="18" spans="1:5" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="19" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:5" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="27" t="s">
         <v>19</v>
       </c>
@@ -5205,7 +5257,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
         <v>0</v>
       </c>
@@ -5219,7 +5271,7 @@
         <v>45559</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:5" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>8</v>
       </c>
@@ -5231,7 +5283,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:5" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>9</v>
       </c>
@@ -5243,7 +5295,7 @@
         <v>0.68333333333333335</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:5" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>10</v>
       </c>
@@ -5255,7 +5307,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:5" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>11</v>
       </c>
@@ -5267,7 +5319,7 @@
         <v>0.69444444444444442</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:5" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>12</v>
       </c>
@@ -5279,7 +5331,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:5" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>13</v>
       </c>
@@ -5287,7 +5339,7 @@
         <v>15</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D26" s="3">
         <f>IF(D24="","",D24-D22)</f>
@@ -5363,17 +5415,17 @@
       <selection activeCell="A21" sqref="A21:A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.453125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.08984375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.453125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.453125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.08984375" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.90625" style="1"/>
+    <col min="1" max="1" width="34.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>24</v>
       </c>
@@ -5381,8 +5433,8 @@
       <c r="C1" s="25"/>
       <c r="D1" s="26"/>
     </row>
-    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="24" t="s">
         <v>2</v>
       </c>
@@ -5394,7 +5446,7 @@
       <c r="H3"/>
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -5412,7 +5464,7 @@
       <c r="H4"/>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>28</v>
       </c>
@@ -5426,7 +5478,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>30</v>
       </c>
@@ -5440,7 +5492,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>31</v>
       </c>
@@ -5454,7 +5506,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>32</v>
       </c>
@@ -5468,7 +5520,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>33</v>
       </c>
@@ -5482,9 +5534,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B10" s="6">
         <v>45558</v>
@@ -5496,14 +5548,14 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="6"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
     </row>
-    <row r="12" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="13" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="24" t="s">
         <v>34</v>
       </c>
@@ -5511,34 +5563,34 @@
       <c r="C13" s="25"/>
       <c r="D13" s="26"/>
     </row>
-    <row r="14" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="30" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B14" s="31"/>
       <c r="C14" s="31"/>
       <c r="D14" s="32"/>
     </row>
-    <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="33"/>
       <c r="B15" s="34"/>
       <c r="C15" s="34"/>
       <c r="D15" s="35"/>
     </row>
-    <row r="16" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="33"/>
       <c r="B16" s="34"/>
       <c r="C16" s="34"/>
       <c r="D16" s="35"/>
     </row>
-    <row r="17" spans="1:5" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:5" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="36"/>
       <c r="B17" s="37"/>
       <c r="C17" s="37"/>
       <c r="D17" s="38"/>
     </row>
-    <row r="18" spans="1:5" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="19" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:5" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="27" t="s">
         <v>19</v>
       </c>
@@ -5548,7 +5600,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
         <v>0</v>
       </c>
@@ -5562,7 +5614,7 @@
         <v>45560</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:5" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>8</v>
       </c>
@@ -5574,7 +5626,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:5" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>9</v>
       </c>
@@ -5586,7 +5638,7 @@
         <v>0.68194444444444446</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:5" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>10</v>
       </c>
@@ -5598,7 +5650,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:5" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>11</v>
       </c>
@@ -5610,7 +5662,7 @@
         <v>0.69444444444444442</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:5" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>12</v>
       </c>
@@ -5622,7 +5674,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:5" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>13</v>
       </c>
@@ -5707,23 +5759,23 @@
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.453125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.08984375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.453125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.453125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="6.453125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="34.453125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="31.08984375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="30.453125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="21.453125" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.90625" style="1"/>
+    <col min="1" max="1" width="34.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="6.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="34.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="31.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="30.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="21.42578125" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B1" s="25"/>
       <c r="C1" s="25"/>
@@ -5734,55 +5786,55 @@
       <c r="H1" s="25"/>
       <c r="I1" s="26"/>
     </row>
-    <row r="2" spans="1:9" customFormat="1" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="3" spans="1:9" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3" s="25"/>
       <c r="C3" s="25"/>
       <c r="D3" s="26"/>
       <c r="F3" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G3" s="25"/>
       <c r="H3" s="25"/>
       <c r="I3" s="26"/>
     </row>
-    <row r="4" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="50" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="50"/>
+      <c r="D4" s="51"/>
+      <c r="F4" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="G4" s="50"/>
+      <c r="H4" s="50"/>
+      <c r="I4" s="51"/>
+    </row>
+    <row r="5" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="B4" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="41"/>
-      <c r="D4" s="42"/>
-      <c r="F4" s="16" t="s">
+      <c r="B5" s="52" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="52"/>
+      <c r="D5" s="53"/>
+      <c r="F5" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="G4" s="41"/>
-      <c r="H4" s="41"/>
-      <c r="I4" s="42"/>
-    </row>
-    <row r="5" spans="1:9" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="B5" s="43" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="43"/>
-      <c r="D5" s="44"/>
-      <c r="F5" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="G5" s="43"/>
-      <c r="H5" s="43"/>
-      <c r="I5" s="44"/>
-    </row>
-    <row r="6" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="7" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G5" s="52"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="53"/>
+    </row>
+    <row r="6" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>3</v>
       </c>
@@ -5808,13 +5860,13 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="22"/>
       <c r="B8" s="6"/>
       <c r="C8" s="5"/>
       <c r="D8" s="23"/>
       <c r="F8" s="22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G8" s="6">
         <v>45567</v>
@@ -5826,7 +5878,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="22"/>
       <c r="B9" s="6"/>
       <c r="C9" s="5"/>
@@ -5844,13 +5896,13 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="22"/>
       <c r="B10" s="6"/>
       <c r="C10" s="5"/>
       <c r="D10" s="23"/>
       <c r="F10" s="22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G10" s="6">
         <v>45567</v>
@@ -5862,7 +5914,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="22"/>
       <c r="B11" s="6"/>
       <c r="C11" s="5"/>
@@ -5880,11 +5932,11 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="19"/>
       <c r="D12" s="18"/>
       <c r="F12" s="22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G12" s="6">
         <v>45567</v>
@@ -5896,15 +5948,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B13" s="25"/>
       <c r="C13" s="25"/>
       <c r="D13" s="26"/>
       <c r="F13" s="22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G13" s="6">
         <v>45567</v>
@@ -5916,13 +5968,13 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="30"/>
       <c r="B14" s="31"/>
       <c r="C14" s="31"/>
       <c r="D14" s="32"/>
       <c r="F14" s="22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G14" s="6">
         <v>45567</v>
@@ -5934,13 +5986,13 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="33"/>
       <c r="B15" s="34"/>
       <c r="C15" s="34"/>
       <c r="D15" s="35"/>
       <c r="F15" s="22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G15" s="6">
         <v>45567</v>
@@ -5952,13 +6004,13 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="33"/>
       <c r="B16" s="34"/>
       <c r="C16" s="34"/>
       <c r="D16" s="35"/>
       <c r="F16" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G16" s="6">
         <v>45567</v>
@@ -5970,13 +6022,13 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="36"/>
       <c r="B17" s="37"/>
       <c r="C17" s="37"/>
       <c r="D17" s="38"/>
       <c r="F17" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G17" s="6">
         <v>45567</v>
@@ -5988,106 +6040,98 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="14"/>
       <c r="B18"/>
       <c r="C18"/>
       <c r="D18" s="15"/>
     </row>
-    <row r="19" spans="1:9" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="45" t="s">
+    <row r="19" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="46"/>
-      <c r="C19" s="46"/>
-      <c r="D19" s="47"/>
+      <c r="B19" s="55"/>
+      <c r="C19" s="55"/>
+      <c r="D19" s="56"/>
       <c r="F19"/>
       <c r="G19"/>
     </row>
-    <row r="20" spans="1:9" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="52" t="s">
+    <row r="20" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="53"/>
-      <c r="C20" s="48" t="s">
-        <v>54</v>
-      </c>
-      <c r="D20" s="49"/>
+      <c r="B20" s="62"/>
+      <c r="C20" s="57" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" s="58"/>
       <c r="E20" s="13"/>
       <c r="F20"/>
       <c r="G20"/>
     </row>
-    <row r="21" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="54" t="s">
+    <row r="21" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="50"/>
-      <c r="C21" s="50" t="s">
+      <c r="B21" s="59"/>
+      <c r="C21" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" s="60"/>
+    </row>
+    <row r="22" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="64" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="48"/>
+      <c r="C22" s="48" t="s">
         <v>55</v>
       </c>
-      <c r="D21" s="51"/>
-    </row>
-    <row r="22" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="55" t="s">
-        <v>9</v>
-      </c>
-      <c r="B22" s="39"/>
-      <c r="C22" s="39" t="s">
+      <c r="D22" s="49"/>
+    </row>
+    <row r="23" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="39" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="40"/>
+      <c r="C23" s="40" t="s">
         <v>56</v>
       </c>
-      <c r="D22" s="40"/>
-    </row>
-    <row r="23" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="56" t="s">
-        <v>10</v>
-      </c>
-      <c r="B23" s="57"/>
-      <c r="C23" s="57" t="s">
+      <c r="D23" s="46"/>
+    </row>
+    <row r="24" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" s="42"/>
+      <c r="C24" s="42" t="s">
         <v>57</v>
       </c>
-      <c r="D23" s="63"/>
-    </row>
-    <row r="24" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="58" t="s">
-        <v>11</v>
-      </c>
-      <c r="B24" s="59"/>
-      <c r="C24" s="59" t="s">
+      <c r="D24" s="47"/>
+    </row>
+    <row r="25" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="40"/>
+      <c r="C25" s="40" t="s">
         <v>58</v>
       </c>
-      <c r="D24" s="64"/>
-    </row>
-    <row r="25" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="56" t="s">
-        <v>12</v>
-      </c>
-      <c r="B25" s="57"/>
-      <c r="C25" s="57" t="s">
+      <c r="D25" s="46"/>
+    </row>
+    <row r="26" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="44"/>
+      <c r="C26" s="44" t="s">
         <v>59</v>
       </c>
-      <c r="D25" s="63"/>
-    </row>
-    <row r="26" spans="1:9" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="60" t="s">
-        <v>13</v>
-      </c>
-      <c r="B26" s="61"/>
-      <c r="C26" s="61" t="s">
-        <v>60</v>
-      </c>
-      <c r="D26" s="62"/>
+      <c r="D26" s="45"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <mergeCells count="24">
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="A25:B25"/>
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="A13:D13"/>
     <mergeCell ref="A14:D17"/>
@@ -6104,6 +6148,14 @@
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="A25:B25"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="D8:D11 I8:I17">
@@ -6146,7 +6198,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CB2ECE66-384A-4231-9DE0-EE40A3A51602}">
           <x14:formula1>
-            <xm:f>Quinta!$A$22:$A$27</xm:f>
+            <xm:f>Quinta!$A$25:$A$30</xm:f>
           </x14:formula1>
           <xm:sqref>H8:H17</xm:sqref>
         </x14:dataValidation>

</xml_diff>

<commit_message>
ata de sábado 29/09
</commit_message>
<xml_diff>
--- a/ATAs_de_Reuniao/Sprint 2/Semana 2609/Grupo4_ATA_Semana2609.xlsx
+++ b/ATAs_de_Reuniao/Sprint 2/Semana 2609/Grupo4_ATA_Semana2609.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpfer\OneDrive\Documentos\SPTECH\PI\SPRINT\Sprint-SPTECH\ATAs_de_Reuniao\Sprint 2\Semana 2609\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f4fd29038e46714d/Área de Trabalho/SPTECH/Pesquisa e Inovação/Sprint-SPTECH/ATAs_de_Reuniao/Sprint 2/Semana 2609/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC84EBE2-A5B3-470A-94FF-5A84E71E7BEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="13_ncr:1_{DC84EBE2-A5B3-470A-94FF-5A84E71E7BEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F35C906D-421C-4D20-9113-1E35E52D248A}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="2" xr2:uid="{D70EAD62-B489-48DA-AED6-4403B2320B59}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" firstSheet="1" activeTab="3" xr2:uid="{D70EAD62-B489-48DA-AED6-4403B2320B59}"/>
   </bookViews>
   <sheets>
     <sheet name="BANCO DE DADOS" sheetId="2" state="hidden" r:id="rId1"/>
     <sheet name="Quinta" sheetId="1" r:id="rId2"/>
     <sheet name="Sexta" sheetId="11" r:id="rId3"/>
-    <sheet name="Sábado" sheetId="4" r:id="rId4"/>
+    <sheet name="Sábado" sheetId="12" r:id="rId4"/>
     <sheet name="Segunda" sheetId="5" r:id="rId5"/>
     <sheet name="Terça" sheetId="7" r:id="rId6"/>
     <sheet name="Quarta" sheetId="9" r:id="rId7"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="63">
   <si>
     <t>NOME</t>
   </si>
@@ -147,9 +147,6 @@
     <t>APRESENTAÇÃO DE TI</t>
   </si>
   <si>
-    <t>Ficou definida a parte de cada um dos integrantes na apresentação de TI: Introdução (Lucas Aiello), Ícones (Thiago), Diagrama (João Pedro e Lucas Pereira), Cálculo (Shelly) e Finalização (Miguel). Também combinamos uma data para treinarmos a apresentação pessoalente (Segunda-feira, 23/09).</t>
-  </si>
-  <si>
     <t>Foi falado que iremos adiantar as tarefas ainda nesse dia e acelerar o processo de Sprint Review o quanto antes.</t>
   </si>
   <si>
@@ -232,6 +229,9 @@
   </si>
   <si>
     <t>Discutimos sobre as atividades pendentes, ajustamos os prazos pendentes de algumas atividades para uma data mais próxima.</t>
+  </si>
+  <si>
+    <t>Definimos as tarefas semanais que poderão ser entregues até segunda-feira (30/09).</t>
   </si>
 </sst>
 </file>
@@ -879,6 +879,33 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -930,38 +957,341 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="8" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="8" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="8" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="8" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="8" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="8" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="125">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1210,336 +1540,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -3163,50 +3163,53 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{D0E7EA3C-BE91-4CD4-8D6B-11CF5253537E}" name="Tabela115" displayName="Tabela115" ref="A4:D15" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11" tableBorderDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{D0E7EA3C-BE91-4CD4-8D6B-11CF5253537E}" name="Tabela115" displayName="Tabela115" ref="A4:D15" totalsRowShown="0" headerRowDxfId="111" dataDxfId="110" tableBorderDxfId="109">
   <autoFilter ref="A4:D15" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{B6DB7E5E-011A-48D2-A976-ECEFE111C94E}" name="O QUE FAZER" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{C8C44900-7A4B-42F1-AAB5-3F3D22C68477}" name="PRAZOS DE ENTREGA" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{7D5CA6FE-4AAD-477F-AF2F-FCF9BB79F2A4}" name="RESPONSAVEL" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{C66C4879-8B2E-4E01-B450-94C2F9ACD3E6}" name="SITUAÇÃO" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{B6DB7E5E-011A-48D2-A976-ECEFE111C94E}" name="O QUE FAZER" dataDxfId="108"/>
+    <tableColumn id="2" xr3:uid="{C8C44900-7A4B-42F1-AAB5-3F3D22C68477}" name="PRAZOS DE ENTREGA" dataDxfId="107"/>
+    <tableColumn id="3" xr3:uid="{7D5CA6FE-4AAD-477F-AF2F-FCF9BB79F2A4}" name="RESPONSAVEL" dataDxfId="106"/>
+    <tableColumn id="4" xr3:uid="{C66C4879-8B2E-4E01-B450-94C2F9ACD3E6}" name="SITUAÇÃO" dataDxfId="105"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{7450B737-251D-4080-BADD-F4A96802C130}" name="Tabela216" displayName="Tabela216" ref="A24:C30" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4" tableBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{7450B737-251D-4080-BADD-F4A96802C130}" name="Tabela216" displayName="Tabela216" ref="A24:C30" totalsRowShown="0" headerRowDxfId="104" dataDxfId="103" tableBorderDxfId="102">
   <autoFilter ref="A24:C30" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{4F27162E-8CFA-4DAC-B500-6AABDBBE620A}" name="NOME" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{37D7277D-4E73-48C0-9519-8AD7D8FE33D8}" name="PARTICIPAÇÃO" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{496DFA61-9424-423D-B0E5-A7735AFDCAF4}" name="JUSTIFICATIVA" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{4F27162E-8CFA-4DAC-B500-6AABDBBE620A}" name="NOME" dataDxfId="101"/>
+    <tableColumn id="2" xr3:uid="{37D7277D-4E73-48C0-9519-8AD7D8FE33D8}" name="PARTICIPAÇÃO" dataDxfId="100"/>
+    <tableColumn id="3" xr3:uid="{496DFA61-9424-423D-B0E5-A7735AFDCAF4}" name="JUSTIFICATIVA" dataDxfId="99"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{0D24B965-B4D0-472F-8B6D-931251406FD0}" name="Tabela146" displayName="Tabela146" ref="A4:D11" totalsRowShown="0" headerRowDxfId="111" dataDxfId="110" tableBorderDxfId="109">
-  <autoFilter ref="A4:D11" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A2693141-5581-47AE-AA42-42593B3EBCC5}" name="Tabela1154" displayName="Tabela1154" ref="A4:D14" totalsRowShown="0" headerRowDxfId="45" dataDxfId="44" tableBorderDxfId="43">
+  <autoFilter ref="A4:D14" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:D14">
+    <sortCondition ref="B5:B14"/>
+  </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{4DB758E7-A5B8-4A9F-BCA4-563D8A6C3B6B}" name="O QUE FAZER" dataDxfId="108"/>
-    <tableColumn id="2" xr3:uid="{7EF6621B-1CC5-4635-882A-1B8E78882552}" name="PRAZOS DE ENTREGA" dataDxfId="107"/>
-    <tableColumn id="3" xr3:uid="{9F41E9D9-BCC0-44A3-9CEA-7746D12A0832}" name="RESPONSAVEL" dataDxfId="106"/>
-    <tableColumn id="4" xr3:uid="{C11A8EA2-A0AA-4B12-9B04-E8A9ADB179F1}" name="SITUAÇÃO" dataDxfId="105"/>
+    <tableColumn id="1" xr3:uid="{9F852A18-D2ED-4627-9A9F-5F87E825A023}" name="O QUE FAZER" dataDxfId="42"/>
+    <tableColumn id="2" xr3:uid="{47171A49-03A0-4FA7-9867-33A0B4CA3732}" name="PRAZOS DE ENTREGA" dataDxfId="41"/>
+    <tableColumn id="3" xr3:uid="{D64896FF-DF85-432A-AF0B-6A09292E6318}" name="RESPONSAVEL" dataDxfId="40"/>
+    <tableColumn id="4" xr3:uid="{3524D571-73DA-4A58-9780-D5CE262B5B8B}" name="SITUAÇÃO" dataDxfId="39"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{42551E1E-5CD7-4F6A-843E-1CBF547215BB}" name="Tabela257" displayName="Tabela257" ref="A20:C26" totalsRowShown="0" headerRowDxfId="104" dataDxfId="103" tableBorderDxfId="102">
-  <autoFilter ref="A20:C26" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{CA79F966-3FFA-418D-B80E-FC555E57811D}" name="Tabela2165" displayName="Tabela2165" ref="A23:C29" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37" tableBorderDxfId="36">
+  <autoFilter ref="A23:C29" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{8E8C9FBB-2737-4F1B-8662-DC7B8E05FE39}" name="NOME" dataDxfId="101"/>
-    <tableColumn id="2" xr3:uid="{5E83EC73-7E41-45E0-AF4D-68FC709F651A}" name="PARTICIPAÇÃO" dataDxfId="100"/>
-    <tableColumn id="3" xr3:uid="{87E32803-B844-4BA6-BF0A-17270B237D48}" name="JUSTIFICATIVA" dataDxfId="99"/>
+    <tableColumn id="1" xr3:uid="{6971728D-486F-404A-9A71-16C4D8DC9AA4}" name="NOME" dataDxfId="35"/>
+    <tableColumn id="2" xr3:uid="{C9BB7BC6-2734-4029-ACCA-3F1D8B884C14}" name="PARTICIPAÇÃO" dataDxfId="34"/>
+    <tableColumn id="3" xr3:uid="{D1D8705A-36D0-46DD-926C-E78547A7E649}" name="JUSTIFICATIVA" dataDxfId="33"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3573,12 +3576,12 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -3589,7 +3592,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -3600,7 +3603,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>18</v>
       </c>
@@ -3618,17 +3621,17 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.109375" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="34.453125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.08984375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.453125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.453125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.08984375" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="39.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="24" t="s">
         <v>24</v>
       </c>
@@ -3636,8 +3639,8 @@
       <c r="C1" s="25"/>
       <c r="D1" s="26"/>
     </row>
-    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="24" t="s">
         <v>2</v>
       </c>
@@ -3649,7 +3652,7 @@
       <c r="H3"/>
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -3667,9 +3670,9 @@
       <c r="H4"/>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B5" s="6">
         <v>45567</v>
@@ -3685,7 +3688,7 @@
       <c r="H5"/>
       <c r="I5"/>
     </row>
-    <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>30</v>
       </c>
@@ -3699,9 +3702,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B7" s="6">
         <v>45567</v>
@@ -3713,7 +3716,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>28</v>
       </c>
@@ -3727,9 +3730,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B9" s="6">
         <v>45567</v>
@@ -3741,7 +3744,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>28</v>
       </c>
@@ -3755,9 +3758,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B11" s="6">
         <v>45567</v>
@@ -3769,9 +3772,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B12" s="6">
         <v>45567</v>
@@ -3783,9 +3786,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B13" s="6">
         <v>45567</v>
@@ -3797,9 +3800,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B14" s="6">
         <v>45567</v>
@@ -3811,14 +3814,14 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="5"/>
       <c r="B15" s="6"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
     </row>
-    <row r="16" spans="1:9" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="17" spans="1:4" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="17" spans="1:4" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="24" t="s">
         <v>32</v>
       </c>
@@ -3826,34 +3829,34 @@
       <c r="C17" s="25"/>
       <c r="D17" s="26"/>
     </row>
-    <row r="18" spans="1:4" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="30" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B18" s="31"/>
       <c r="C18" s="31"/>
       <c r="D18" s="32"/>
     </row>
-    <row r="19" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="33"/>
       <c r="B19" s="34"/>
       <c r="C19" s="34"/>
       <c r="D19" s="35"/>
     </row>
-    <row r="20" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="33"/>
       <c r="B20" s="34"/>
       <c r="C20" s="34"/>
       <c r="D20" s="35"/>
     </row>
-    <row r="21" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="36"/>
       <c r="B21" s="37"/>
       <c r="C21" s="37"/>
       <c r="D21" s="38"/>
     </row>
-    <row r="22" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="23" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="23" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="27" t="s">
         <v>19</v>
       </c>
@@ -3863,7 +3866,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="10" t="s">
         <v>0</v>
       </c>
@@ -3877,7 +3880,7 @@
         <v>45561</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="2" t="s">
         <v>8</v>
       </c>
@@ -3889,7 +3892,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="2" t="s">
         <v>9</v>
       </c>
@@ -3901,7 +3904,7 @@
         <v>0.68819444444444444</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="2" t="s">
         <v>10</v>
       </c>
@@ -3913,7 +3916,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="2" t="s">
         <v>11</v>
       </c>
@@ -3925,7 +3928,7 @@
         <v>0.69930555555555551</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="2" t="s">
         <v>12</v>
       </c>
@@ -3937,7 +3940,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="2" t="s">
         <v>13</v>
       </c>
@@ -3964,21 +3967,21 @@
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="B25:B30">
-    <cfRule type="cellIs" dxfId="45" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="4" operator="equal">
       <formula>"AUSENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="5" operator="equal">
       <formula>"PRESENTE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D14">
-    <cfRule type="cellIs" dxfId="43" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="1" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="2" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="3" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4018,21 +4021,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA47C666-6B9B-4ED9-8062-81E393DBE6A0}">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:D21"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.109375" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="34.453125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.08984375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.453125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.453125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.08984375" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="39.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="24" t="s">
         <v>24</v>
       </c>
@@ -4040,8 +4043,8 @@
       <c r="C1" s="25"/>
       <c r="D1" s="26"/>
     </row>
-    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="24" t="s">
         <v>2</v>
       </c>
@@ -4053,7 +4056,7 @@
       <c r="H3"/>
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -4071,9 +4074,9 @@
       <c r="H4"/>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B5" s="6">
         <v>45567</v>
@@ -4089,7 +4092,7 @@
       <c r="H5"/>
       <c r="I5"/>
     </row>
-    <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>30</v>
       </c>
@@ -4103,9 +4106,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B7" s="6">
         <v>45565</v>
@@ -4117,7 +4120,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>28</v>
       </c>
@@ -4131,9 +4134,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B9" s="6">
         <v>45567</v>
@@ -4145,7 +4148,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>28</v>
       </c>
@@ -4159,12 +4162,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B11" s="6">
-        <v>45595</v>
+        <v>45565</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>12</v>
@@ -4173,12 +4176,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B12" s="6">
-        <v>45595</v>
+        <v>45565</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>12</v>
@@ -4187,12 +4190,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B13" s="6">
-        <v>45595</v>
+        <v>45565</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>13</v>
@@ -4201,9 +4204,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B14" s="6">
         <v>45567</v>
@@ -4215,14 +4218,14 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="5"/>
       <c r="B15" s="6"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
     </row>
-    <row r="16" spans="1:9" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="17" spans="1:4" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="17" spans="1:4" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="24" t="s">
         <v>32</v>
       </c>
@@ -4230,34 +4233,34 @@
       <c r="C17" s="25"/>
       <c r="D17" s="26"/>
     </row>
-    <row r="18" spans="1:4" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="30" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B18" s="31"/>
       <c r="C18" s="31"/>
       <c r="D18" s="32"/>
     </row>
-    <row r="19" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="33"/>
       <c r="B19" s="34"/>
       <c r="C19" s="34"/>
       <c r="D19" s="35"/>
     </row>
-    <row r="20" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="33"/>
       <c r="B20" s="34"/>
       <c r="C20" s="34"/>
       <c r="D20" s="35"/>
     </row>
-    <row r="21" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="36"/>
       <c r="B21" s="37"/>
       <c r="C21" s="37"/>
       <c r="D21" s="38"/>
     </row>
-    <row r="22" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="23" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="23" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="27" t="s">
         <v>19</v>
       </c>
@@ -4267,7 +4270,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="10" t="s">
         <v>0</v>
       </c>
@@ -4278,10 +4281,10 @@
         <v>7</v>
       </c>
       <c r="D24" s="4">
-        <v>45561</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>45562</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="2" t="s">
         <v>8</v>
       </c>
@@ -4293,7 +4296,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="2" t="s">
         <v>9</v>
       </c>
@@ -4305,7 +4308,7 @@
         <v>0.68541666666666667</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="2" t="s">
         <v>10</v>
       </c>
@@ -4317,7 +4320,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="2" t="s">
         <v>11</v>
       </c>
@@ -4329,7 +4332,7 @@
         <v>0.69930555555555551</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="2" t="s">
         <v>12</v>
       </c>
@@ -4341,7 +4344,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="2" t="s">
         <v>13</v>
       </c>
@@ -4364,21 +4367,21 @@
     <mergeCell ref="A23:C23"/>
   </mergeCells>
   <conditionalFormatting sqref="B25:B30">
-    <cfRule type="cellIs" dxfId="17" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="4" operator="equal">
       <formula>"AUSENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="5" operator="equal">
       <formula>"PRESENTE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D14">
-    <cfRule type="cellIs" dxfId="15" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="1" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="2" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="3" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4415,24 +4418,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E3CEB27-A829-4B68-B2D9-5D90AA774C8D}">
-  <dimension ref="A1:I26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25161DFF-344A-4C41-AE51-A14BEC6B2F7D}">
+  <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="66" zoomScaleNormal="46" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:D17"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.109375" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="34.453125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.08984375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.453125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.453125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.08984375" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="39.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="24" t="s">
         <v>24</v>
       </c>
@@ -4440,8 +4443,8 @@
       <c r="C1" s="25"/>
       <c r="D1" s="26"/>
     </row>
-    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="24" t="s">
         <v>2</v>
       </c>
@@ -4453,7 +4456,7 @@
       <c r="H3"/>
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -4471,12 +4474,12 @@
       <c r="H4"/>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="B5" s="6">
-        <v>45556</v>
+        <v>45565</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>9</v>
@@ -4484,248 +4487,293 @@
       <c r="D5" s="5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F5"/>
+      <c r="G5"/>
+      <c r="H5"/>
+      <c r="I5"/>
+    </row>
+    <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="B6" s="6">
-        <v>45559</v>
+        <v>45565</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>29</v>
+        <v>57</v>
       </c>
       <c r="B7" s="6">
-        <v>45556</v>
+        <v>45565</v>
       </c>
       <c r="C7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="6">
+        <v>45565</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D8" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
+    <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" s="6">
+        <v>45567</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="6">
-        <v>45559</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9" s="6">
-        <v>45555</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
-        <v>33</v>
-      </c>
       <c r="B10" s="6">
-        <v>45558</v>
+        <v>45567</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="5"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-    </row>
-    <row r="12" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="13" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="24" t="s">
+    <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="6">
+        <v>45567</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="6">
+        <v>45567</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" s="6">
+        <v>45567</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="5"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+    </row>
+    <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="16" spans="1:9" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="25"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="26"/>
-    </row>
-    <row r="14" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" s="31"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="32"/>
-    </row>
-    <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="33"/>
-      <c r="B15" s="34"/>
-      <c r="C15" s="34"/>
-      <c r="D15" s="35"/>
-    </row>
-    <row r="16" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="33"/>
-      <c r="B16" s="34"/>
-      <c r="C16" s="34"/>
-      <c r="D16" s="35"/>
-    </row>
-    <row r="17" spans="1:5" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="36"/>
-      <c r="B17" s="37"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="38"/>
-    </row>
-    <row r="18" spans="1:5" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="19" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="27" t="s">
+      <c r="B16" s="25"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="26"/>
+    </row>
+    <row r="17" spans="1:4" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="B17" s="31"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="32"/>
+    </row>
+    <row r="18" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="33"/>
+      <c r="B18" s="34"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="35"/>
+    </row>
+    <row r="19" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="33"/>
+      <c r="B19" s="34"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="35"/>
+    </row>
+    <row r="20" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="36"/>
+      <c r="B20" s="37"/>
+      <c r="C20" s="37"/>
+      <c r="D20" s="38"/>
+    </row>
+    <row r="21" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="22" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="28"/>
-      <c r="C19" s="29"/>
-      <c r="D19" s="12" t="s">
+      <c r="B22" s="28"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="10" t="s">
+    <row r="23" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B23" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C23" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="4">
-        <v>45556</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="2" t="s">
+      <c r="D23" s="4">
+        <v>45563</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C21" s="5"/>
-      <c r="D21" s="12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22" s="5"/>
-      <c r="D22" s="7">
-        <v>0.41875000000000001</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23" s="5"/>
-      <c r="D23" s="12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C24" s="5"/>
-      <c r="D24" s="8">
-        <v>0.42499999999999999</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D24" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C25" s="5"/>
-      <c r="D25" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D25" s="7">
+        <v>0.41875000000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C26" s="5"/>
-      <c r="D26" s="3">
-        <f>IF(D24="","",D24-D22)</f>
-        <v>6.2499999999999778E-3</v>
-      </c>
-      <c r="E26" s="13"/>
+      <c r="D26" s="12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" s="5"/>
+      <c r="D27" s="8">
+        <v>0.4284722222222222</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C28" s="5"/>
+      <c r="D28" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A29" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" s="5"/>
+      <c r="D29" s="3">
+        <f>IF(D27="","",D27-D25)</f>
+        <v>9.7222222222221877E-3</v>
+      </c>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <mergeCells count="5">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A13:D13"/>
-    <mergeCell ref="A14:D17"/>
-    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="A17:D20"/>
+    <mergeCell ref="A22:C22"/>
   </mergeCells>
-  <conditionalFormatting sqref="B21:B26">
-    <cfRule type="cellIs" dxfId="40" priority="4" operator="equal">
+  <conditionalFormatting sqref="B24:B29">
+    <cfRule type="cellIs" dxfId="22" priority="4" operator="equal">
       <formula>"AUSENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="5" operator="equal">
       <formula>"PRESENTE"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D5:D10">
-    <cfRule type="cellIs" dxfId="38" priority="1" operator="equal">
+  <conditionalFormatting sqref="D5:D13">
+    <cfRule type="cellIs" dxfId="20" priority="1" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="2" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="3" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C11" xr:uid="{CF602ED2-C5AB-4338-A760-E49F25957E9B}">
-      <formula1>$A$21:$A$26</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C14" xr:uid="{C8722A97-139C-4D2F-A9B1-4A10D3D568E3}">
+      <formula1>$A$24:$A$29</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -4737,17 +4785,17 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{595204DC-DCAA-4657-89BE-3A3637AA945B}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8E8C7061-5903-4F23-9649-F9812A833E92}">
           <x14:formula1>
             <xm:f>'BANCO DE DADOS'!$A$1:$A$2</xm:f>
           </x14:formula1>
-          <xm:sqref>B21:B26</xm:sqref>
+          <xm:sqref>B24:B29</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{514D41D0-19FB-4FBD-8072-BB9890C483E1}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1C28F55C-0601-423C-B6A5-BFFA9C259221}">
           <x14:formula1>
             <xm:f>'BANCO DE DADOS'!$B$1:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>D5:D11</xm:sqref>
+          <xm:sqref>D5:D14</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4763,17 +4811,17 @@
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.109375" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="34.453125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.08984375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.453125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.453125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.08984375" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="39.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="24" t="s">
         <v>24</v>
       </c>
@@ -4781,8 +4829,8 @@
       <c r="C1" s="25"/>
       <c r="D1" s="26"/>
     </row>
-    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="24" t="s">
         <v>2</v>
       </c>
@@ -4794,7 +4842,7 @@
       <c r="H3"/>
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -4812,7 +4860,7 @@
       <c r="H4"/>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>27</v>
       </c>
@@ -4826,7 +4874,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>28</v>
       </c>
@@ -4840,7 +4888,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>29</v>
       </c>
@@ -4854,7 +4902,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>30</v>
       </c>
@@ -4868,7 +4916,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>31</v>
       </c>
@@ -4882,7 +4930,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>33</v>
       </c>
@@ -4896,14 +4944,14 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5"/>
       <c r="B11" s="6"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
     </row>
-    <row r="12" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="13" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="13" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="24" t="s">
         <v>32</v>
       </c>
@@ -4911,34 +4959,34 @@
       <c r="C13" s="25"/>
       <c r="D13" s="26"/>
     </row>
-    <row r="14" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B14" s="31"/>
       <c r="C14" s="31"/>
       <c r="D14" s="32"/>
     </row>
-    <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="33"/>
       <c r="B15" s="34"/>
       <c r="C15" s="34"/>
       <c r="D15" s="35"/>
     </row>
-    <row r="16" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="33"/>
       <c r="B16" s="34"/>
       <c r="C16" s="34"/>
       <c r="D16" s="35"/>
     </row>
-    <row r="17" spans="1:5" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="36"/>
       <c r="B17" s="37"/>
       <c r="C17" s="37"/>
       <c r="D17" s="38"/>
     </row>
-    <row r="18" spans="1:5" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="19" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="19" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="27" t="s">
         <v>19</v>
       </c>
@@ -4948,7 +4996,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="10" t="s">
         <v>0</v>
       </c>
@@ -4962,7 +5010,7 @@
         <v>45558</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="2" t="s">
         <v>8</v>
       </c>
@@ -4974,7 +5022,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="2" t="s">
         <v>9</v>
       </c>
@@ -4986,7 +5034,7 @@
         <v>0.6958333333333333</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="2" t="s">
         <v>10</v>
       </c>
@@ -4998,7 +5046,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="2" t="s">
         <v>11</v>
       </c>
@@ -5010,7 +5058,7 @@
         <v>0.70138888888888884</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="2" t="s">
         <v>12</v>
       </c>
@@ -5022,7 +5070,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="2" t="s">
         <v>13</v>
       </c>
@@ -5046,21 +5094,21 @@
     <mergeCell ref="A19:C19"/>
   </mergeCells>
   <conditionalFormatting sqref="B21:B26">
-    <cfRule type="cellIs" dxfId="35" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="4" operator="equal">
       <formula>"AUSENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="5" operator="equal">
       <formula>"PRESENTE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D10">
-    <cfRule type="cellIs" dxfId="33" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="1" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="2" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="3" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5104,17 +5152,17 @@
       <selection activeCell="A14" sqref="A14:D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.109375" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="34.453125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.08984375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.453125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.453125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.08984375" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="39.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="24" t="s">
         <v>24</v>
       </c>
@@ -5122,8 +5170,8 @@
       <c r="C1" s="25"/>
       <c r="D1" s="26"/>
     </row>
-    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="24" t="s">
         <v>2</v>
       </c>
@@ -5135,7 +5183,7 @@
       <c r="H3"/>
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -5153,7 +5201,7 @@
       <c r="H4"/>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>27</v>
       </c>
@@ -5167,7 +5215,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>28</v>
       </c>
@@ -5181,7 +5229,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>29</v>
       </c>
@@ -5195,7 +5243,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>30</v>
       </c>
@@ -5209,7 +5257,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>31</v>
       </c>
@@ -5223,7 +5271,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>33</v>
       </c>
@@ -5237,14 +5285,14 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5"/>
       <c r="B11" s="6"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
     </row>
-    <row r="12" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="13" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="13" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="24" t="s">
         <v>32</v>
       </c>
@@ -5252,34 +5300,34 @@
       <c r="C13" s="25"/>
       <c r="D13" s="26"/>
     </row>
-    <row r="14" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B14" s="31"/>
       <c r="C14" s="31"/>
       <c r="D14" s="32"/>
     </row>
-    <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="33"/>
       <c r="B15" s="34"/>
       <c r="C15" s="34"/>
       <c r="D15" s="35"/>
     </row>
-    <row r="16" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="33"/>
       <c r="B16" s="34"/>
       <c r="C16" s="34"/>
       <c r="D16" s="35"/>
     </row>
-    <row r="17" spans="1:5" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="36"/>
       <c r="B17" s="37"/>
       <c r="C17" s="37"/>
       <c r="D17" s="38"/>
     </row>
-    <row r="18" spans="1:5" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="19" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="19" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="27" t="s">
         <v>19</v>
       </c>
@@ -5289,7 +5337,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="10" t="s">
         <v>0</v>
       </c>
@@ -5303,7 +5351,7 @@
         <v>45559</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="2" t="s">
         <v>8</v>
       </c>
@@ -5315,7 +5363,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="2" t="s">
         <v>9</v>
       </c>
@@ -5327,7 +5375,7 @@
         <v>0.68333333333333335</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="2" t="s">
         <v>10</v>
       </c>
@@ -5339,7 +5387,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="2" t="s">
         <v>11</v>
       </c>
@@ -5351,7 +5399,7 @@
         <v>0.69444444444444442</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="2" t="s">
         <v>12</v>
       </c>
@@ -5363,7 +5411,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="2" t="s">
         <v>13</v>
       </c>
@@ -5371,7 +5419,7 @@
         <v>15</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D26" s="3">
         <f>IF(D24="","",D24-D22)</f>
@@ -5389,21 +5437,21 @@
     <mergeCell ref="A19:C19"/>
   </mergeCells>
   <conditionalFormatting sqref="B21:B26">
-    <cfRule type="cellIs" dxfId="30" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="4" operator="equal">
       <formula>"AUSENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
       <formula>"PRESENTE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D10">
-    <cfRule type="cellIs" dxfId="28" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5447,17 +5495,17 @@
       <selection activeCell="A21" sqref="A21:A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.109375" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="34.453125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.08984375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.453125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.453125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.08984375" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="39.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="24" t="s">
         <v>24</v>
       </c>
@@ -5465,8 +5513,8 @@
       <c r="C1" s="25"/>
       <c r="D1" s="26"/>
     </row>
-    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="24" t="s">
         <v>2</v>
       </c>
@@ -5478,7 +5526,7 @@
       <c r="H3"/>
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -5496,7 +5544,7 @@
       <c r="H4"/>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>27</v>
       </c>
@@ -5510,7 +5558,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>28</v>
       </c>
@@ -5524,7 +5572,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>29</v>
       </c>
@@ -5538,7 +5586,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>30</v>
       </c>
@@ -5552,7 +5600,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>31</v>
       </c>
@@ -5566,7 +5614,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>33</v>
       </c>
@@ -5580,14 +5628,14 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5"/>
       <c r="B11" s="6"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
     </row>
-    <row r="12" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="13" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="13" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="24" t="s">
         <v>32</v>
       </c>
@@ -5595,34 +5643,34 @@
       <c r="C13" s="25"/>
       <c r="D13" s="26"/>
     </row>
-    <row r="14" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B14" s="31"/>
       <c r="C14" s="31"/>
       <c r="D14" s="32"/>
     </row>
-    <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="33"/>
       <c r="B15" s="34"/>
       <c r="C15" s="34"/>
       <c r="D15" s="35"/>
     </row>
-    <row r="16" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="33"/>
       <c r="B16" s="34"/>
       <c r="C16" s="34"/>
       <c r="D16" s="35"/>
     </row>
-    <row r="17" spans="1:5" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="36"/>
       <c r="B17" s="37"/>
       <c r="C17" s="37"/>
       <c r="D17" s="38"/>
     </row>
-    <row r="18" spans="1:5" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="19" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="19" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="27" t="s">
         <v>19</v>
       </c>
@@ -5632,7 +5680,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="10" t="s">
         <v>0</v>
       </c>
@@ -5646,7 +5694,7 @@
         <v>45560</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="2" t="s">
         <v>8</v>
       </c>
@@ -5658,7 +5706,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="2" t="s">
         <v>9</v>
       </c>
@@ -5670,7 +5718,7 @@
         <v>0.68194444444444446</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="2" t="s">
         <v>10</v>
       </c>
@@ -5682,7 +5730,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="2" t="s">
         <v>11</v>
       </c>
@@ -5694,7 +5742,7 @@
         <v>0.69444444444444442</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="2" t="s">
         <v>12</v>
       </c>
@@ -5706,7 +5754,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="2" t="s">
         <v>13</v>
       </c>
@@ -5730,21 +5778,21 @@
     <mergeCell ref="A19:C19"/>
   </mergeCells>
   <conditionalFormatting sqref="B21:B26">
-    <cfRule type="cellIs" dxfId="25" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
       <formula>"AUSENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
       <formula>"PRESENTE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D10">
-    <cfRule type="cellIs" dxfId="23" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5788,26 +5836,26 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="I13" sqref="F13:I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="6.44140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="34.44140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="31.109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="30.44140625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="21.44140625" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="34.453125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.08984375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.453125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.453125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="6.453125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="34.453125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="31.08984375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="30.453125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="21.453125" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="39.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1" s="25"/>
       <c r="C1" s="25"/>
@@ -5818,55 +5866,55 @@
       <c r="H1" s="25"/>
       <c r="I1" s="26"/>
     </row>
-    <row r="2" spans="1:9" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" customFormat="1" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="1:9" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B3" s="25"/>
       <c r="C3" s="25"/>
       <c r="D3" s="26"/>
       <c r="F3" s="24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G3" s="25"/>
       <c r="H3" s="25"/>
       <c r="I3" s="26"/>
     </row>
-    <row r="4" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="50" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="50"/>
+      <c r="D4" s="51"/>
+      <c r="F4" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4" s="50"/>
+      <c r="H4" s="50"/>
+      <c r="I4" s="51"/>
+    </row>
+    <row r="5" spans="1:9" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="41"/>
-      <c r="D4" s="42"/>
-      <c r="F4" s="16" t="s">
+      <c r="B5" s="52" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="52"/>
+      <c r="D5" s="53"/>
+      <c r="F5" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="G4" s="41"/>
-      <c r="H4" s="41"/>
-      <c r="I4" s="42"/>
-    </row>
-    <row r="5" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="B5" s="43" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="43"/>
-      <c r="D5" s="44"/>
-      <c r="F5" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="G5" s="43"/>
-      <c r="H5" s="43"/>
-      <c r="I5" s="44"/>
-    </row>
-    <row r="6" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G5" s="52"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="53"/>
+    </row>
+    <row r="6" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="7" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="20" t="s">
         <v>3</v>
       </c>
@@ -5892,13 +5940,13 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="22"/>
       <c r="B8" s="6"/>
       <c r="C8" s="5"/>
       <c r="D8" s="23"/>
       <c r="F8" s="22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G8" s="6">
         <v>45567</v>
@@ -5907,10 +5955,10 @@
         <v>8</v>
       </c>
       <c r="I8" s="23" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="22"/>
       <c r="B9" s="6"/>
       <c r="C9" s="5"/>
@@ -5928,13 +5976,13 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="22"/>
       <c r="B10" s="6"/>
       <c r="C10" s="5"/>
       <c r="D10" s="23"/>
       <c r="F10" s="22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G10" s="6">
         <v>45567</v>
@@ -5946,7 +5994,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="22"/>
       <c r="B11" s="6"/>
       <c r="C11" s="5"/>
@@ -5964,11 +6012,11 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="19"/>
       <c r="D12" s="18"/>
       <c r="F12" s="22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G12" s="6">
         <v>45567</v>
@@ -5980,15 +6028,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B13" s="25"/>
       <c r="C13" s="25"/>
       <c r="D13" s="26"/>
       <c r="F13" s="22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G13" s="6">
         <v>45567</v>
@@ -6000,13 +6048,13 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="30"/>
       <c r="B14" s="31"/>
       <c r="C14" s="31"/>
       <c r="D14" s="32"/>
       <c r="F14" s="22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G14" s="6">
         <v>45567</v>
@@ -6018,13 +6066,13 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="33"/>
       <c r="B15" s="34"/>
       <c r="C15" s="34"/>
       <c r="D15" s="35"/>
       <c r="F15" s="22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G15" s="6">
         <v>45567</v>
@@ -6036,13 +6084,13 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="33"/>
       <c r="B16" s="34"/>
       <c r="C16" s="34"/>
       <c r="D16" s="35"/>
       <c r="F16" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G16" s="6">
         <v>45567</v>
@@ -6054,13 +6102,13 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="36"/>
       <c r="B17" s="37"/>
       <c r="C17" s="37"/>
       <c r="D17" s="38"/>
       <c r="F17" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G17" s="6">
         <v>45567</v>
@@ -6072,106 +6120,98 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="14"/>
       <c r="B18"/>
       <c r="C18"/>
       <c r="D18" s="15"/>
     </row>
-    <row r="19" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="45" t="s">
+    <row r="19" spans="1:9" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="46"/>
-      <c r="C19" s="46"/>
-      <c r="D19" s="47"/>
+      <c r="B19" s="55"/>
+      <c r="C19" s="55"/>
+      <c r="D19" s="56"/>
       <c r="F19"/>
       <c r="G19"/>
     </row>
-    <row r="20" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="52" t="s">
+    <row r="20" spans="1:9" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="53"/>
-      <c r="C20" s="48" t="s">
-        <v>50</v>
-      </c>
-      <c r="D20" s="49"/>
+      <c r="B20" s="62"/>
+      <c r="C20" s="57" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" s="58"/>
       <c r="E20" s="13"/>
       <c r="F20"/>
       <c r="G20"/>
     </row>
-    <row r="21" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="54" t="s">
+    <row r="21" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="50"/>
-      <c r="C21" s="50" t="s">
+      <c r="B21" s="59"/>
+      <c r="C21" s="59" t="s">
+        <v>50</v>
+      </c>
+      <c r="D21" s="60"/>
+    </row>
+    <row r="22" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="64" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="48"/>
+      <c r="C22" s="48" t="s">
         <v>51</v>
       </c>
-      <c r="D21" s="51"/>
-    </row>
-    <row r="22" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="55" t="s">
-        <v>9</v>
-      </c>
-      <c r="B22" s="39"/>
-      <c r="C22" s="39" t="s">
+      <c r="D22" s="49"/>
+    </row>
+    <row r="23" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="39" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="40"/>
+      <c r="C23" s="40" t="s">
         <v>52</v>
       </c>
-      <c r="D22" s="40"/>
-    </row>
-    <row r="23" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="56" t="s">
-        <v>10</v>
-      </c>
-      <c r="B23" s="57"/>
-      <c r="C23" s="57" t="s">
+      <c r="D23" s="46"/>
+    </row>
+    <row r="24" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" s="42"/>
+      <c r="C24" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="D23" s="63"/>
-    </row>
-    <row r="24" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="58" t="s">
-        <v>11</v>
-      </c>
-      <c r="B24" s="59"/>
-      <c r="C24" s="59" t="s">
+      <c r="D24" s="47"/>
+    </row>
+    <row r="25" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="40"/>
+      <c r="C25" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="D24" s="64"/>
-    </row>
-    <row r="25" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="56" t="s">
-        <v>12</v>
-      </c>
-      <c r="B25" s="57"/>
-      <c r="C25" s="57" t="s">
+      <c r="D25" s="46"/>
+    </row>
+    <row r="26" spans="1:9" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="44"/>
+      <c r="C26" s="44" t="s">
         <v>55</v>
       </c>
-      <c r="D25" s="63"/>
-    </row>
-    <row r="26" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="60" t="s">
-        <v>13</v>
-      </c>
-      <c r="B26" s="61"/>
-      <c r="C26" s="61" t="s">
-        <v>56</v>
-      </c>
-      <c r="D26" s="62"/>
+      <c r="D26" s="45"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <mergeCells count="24">
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="A25:B25"/>
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="A13:D13"/>
     <mergeCell ref="A14:D17"/>
@@ -6188,16 +6228,24 @@
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="A25:B25"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="D8:D11 I8:I17">
-    <cfRule type="cellIs" dxfId="20" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="7" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="8" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6218,7 +6266,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8EFBC24D-2650-46F5-BA77-660A84572B57}">
           <x14:formula1>
-            <xm:f>Sábado!$A$21:$A$26</xm:f>
+            <xm:f>#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>C8:C11</xm:sqref>
         </x14:dataValidation>

</xml_diff>

<commit_message>
Update da ATA de hoje
</commit_message>
<xml_diff>
--- a/ATAs_de_Reuniao/Sprint 2/Semana 2609/Grupo4_ATA_Semana2609.xlsx
+++ b/ATAs_de_Reuniao/Sprint 2/Semana 2609/Grupo4_ATA_Semana2609.xlsx
@@ -5,19 +5,19 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f4fd29038e46714d/Área de Trabalho/SPTECH/Pesquisa e Inovação/Sprint-SPTECH/ATAs_de_Reuniao/Sprint 2/Semana 2609/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Documents\Projeto_PI\sprint2\ATAs_de_Reuniao\Sprint 2\Semana 2609\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="29" documentId="13_ncr:1_{DC84EBE2-A5B3-470A-94FF-5A84E71E7BEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F35C906D-421C-4D20-9113-1E35E52D248A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B51C9FBF-A596-44BE-98D1-B224AB39501A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" firstSheet="1" activeTab="3" xr2:uid="{D70EAD62-B489-48DA-AED6-4403B2320B59}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="4" xr2:uid="{D70EAD62-B489-48DA-AED6-4403B2320B59}"/>
   </bookViews>
   <sheets>
     <sheet name="BANCO DE DADOS" sheetId="2" state="hidden" r:id="rId1"/>
     <sheet name="Quinta" sheetId="1" r:id="rId2"/>
     <sheet name="Sexta" sheetId="11" r:id="rId3"/>
     <sheet name="Sábado" sheetId="12" r:id="rId4"/>
-    <sheet name="Segunda" sheetId="5" r:id="rId5"/>
+    <sheet name="Segunda" sheetId="13" r:id="rId5"/>
     <sheet name="Terça" sheetId="7" r:id="rId6"/>
     <sheet name="Quarta" sheetId="9" r:id="rId7"/>
     <sheet name="SEMANAL" sheetId="10" r:id="rId8"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="62">
   <si>
     <t>NOME</t>
   </si>
@@ -145,9 +145,6 @@
   </si>
   <si>
     <t>APRESENTAÇÃO DE TI</t>
-  </si>
-  <si>
-    <t>Foi falado que iremos adiantar as tarefas ainda nesse dia e acelerar o processo de Sprint Review o quanto antes.</t>
   </si>
   <si>
     <t>Foi feito o treinamento da apresentação sobre a metodologia PERT</t>
@@ -879,33 +876,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="8" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="8" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="8" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="8" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="8" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="8" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -957,341 +927,38 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="125">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1540,6 +1207,336 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -3188,53 +3185,56 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A2693141-5581-47AE-AA42-42593B3EBCC5}" name="Tabela1154" displayName="Tabela1154" ref="A4:D14" totalsRowShown="0" headerRowDxfId="45" dataDxfId="44" tableBorderDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A2693141-5581-47AE-AA42-42593B3EBCC5}" name="Tabela1154" displayName="Tabela1154" ref="A4:D14" totalsRowShown="0" headerRowDxfId="98" dataDxfId="97" tableBorderDxfId="96">
   <autoFilter ref="A4:D14" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:D14">
     <sortCondition ref="B5:B14"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{9F852A18-D2ED-4627-9A9F-5F87E825A023}" name="O QUE FAZER" dataDxfId="42"/>
-    <tableColumn id="2" xr3:uid="{47171A49-03A0-4FA7-9867-33A0B4CA3732}" name="PRAZOS DE ENTREGA" dataDxfId="41"/>
-    <tableColumn id="3" xr3:uid="{D64896FF-DF85-432A-AF0B-6A09292E6318}" name="RESPONSAVEL" dataDxfId="40"/>
-    <tableColumn id="4" xr3:uid="{3524D571-73DA-4A58-9780-D5CE262B5B8B}" name="SITUAÇÃO" dataDxfId="39"/>
+    <tableColumn id="1" xr3:uid="{9F852A18-D2ED-4627-9A9F-5F87E825A023}" name="O QUE FAZER" dataDxfId="95"/>
+    <tableColumn id="2" xr3:uid="{47171A49-03A0-4FA7-9867-33A0B4CA3732}" name="PRAZOS DE ENTREGA" dataDxfId="94"/>
+    <tableColumn id="3" xr3:uid="{D64896FF-DF85-432A-AF0B-6A09292E6318}" name="RESPONSAVEL" dataDxfId="93"/>
+    <tableColumn id="4" xr3:uid="{3524D571-73DA-4A58-9780-D5CE262B5B8B}" name="SITUAÇÃO" dataDxfId="92"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{CA79F966-3FFA-418D-B80E-FC555E57811D}" name="Tabela2165" displayName="Tabela2165" ref="A23:C29" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37" tableBorderDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{CA79F966-3FFA-418D-B80E-FC555E57811D}" name="Tabela2165" displayName="Tabela2165" ref="A23:C29" totalsRowShown="0" headerRowDxfId="91" dataDxfId="90" tableBorderDxfId="89">
   <autoFilter ref="A23:C29" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{6971728D-486F-404A-9A71-16C4D8DC9AA4}" name="NOME" dataDxfId="35"/>
-    <tableColumn id="2" xr3:uid="{C9BB7BC6-2734-4029-ACCA-3F1D8B884C14}" name="PARTICIPAÇÃO" dataDxfId="34"/>
-    <tableColumn id="3" xr3:uid="{D1D8705A-36D0-46DD-926C-E78547A7E649}" name="JUSTIFICATIVA" dataDxfId="33"/>
+    <tableColumn id="1" xr3:uid="{6971728D-486F-404A-9A71-16C4D8DC9AA4}" name="NOME" dataDxfId="88"/>
+    <tableColumn id="2" xr3:uid="{C9BB7BC6-2734-4029-ACCA-3F1D8B884C14}" name="PARTICIPAÇÃO" dataDxfId="87"/>
+    <tableColumn id="3" xr3:uid="{D1D8705A-36D0-46DD-926C-E78547A7E649}" name="JUSTIFICATIVA" dataDxfId="86"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{2973F3F9-B8D9-4E9E-BA21-0F7855C23630}" name="Tabela1468" displayName="Tabela1468" ref="A4:D11" totalsRowShown="0" headerRowDxfId="98" dataDxfId="97" tableBorderDxfId="96">
-  <autoFilter ref="A4:D11" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{6C031CDA-53E0-45FD-9AE0-557E1E0765C8}" name="Tabela11546" displayName="Tabela11546" ref="A4:D14" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11" tableBorderDxfId="10">
+  <autoFilter ref="A4:D14" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:D14">
+    <sortCondition ref="B5:B14"/>
+  </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{11646B81-A121-4FA2-893E-362D3A1A52F0}" name="O QUE FAZER" dataDxfId="95"/>
-    <tableColumn id="2" xr3:uid="{4833C381-32BB-4B40-AD0C-A01805D370D5}" name="PRAZOS DE ENTREGA" dataDxfId="94"/>
-    <tableColumn id="3" xr3:uid="{B9FED99E-7EE5-453D-998F-758D676F139A}" name="RESPONSAVEL" dataDxfId="93"/>
-    <tableColumn id="4" xr3:uid="{C9B39C91-0344-4E7A-847B-74EBED4B2F53}" name="SITUAÇÃO" dataDxfId="92"/>
+    <tableColumn id="1" xr3:uid="{BB742C24-B969-47D8-BDF5-2D9DD9DE0453}" name="O QUE FAZER" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{08450859-D0AC-4147-80B0-0A2BE06A68E3}" name="PRAZOS DE ENTREGA" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{90CA058E-F8FF-4FF1-BD90-FA898BB69129}" name="RESPONSAVEL" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{4533BAE4-7102-4B9B-8C5E-D2327FE6E37B}" name="SITUAÇÃO" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{3C9D5C14-8487-4611-B27F-7F4ABC950782}" name="Tabela2579" displayName="Tabela2579" ref="A20:C26" totalsRowShown="0" headerRowDxfId="91" dataDxfId="90" tableBorderDxfId="89">
-  <autoFilter ref="A20:C26" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{34D2C419-0C8F-420E-9F09-51777412EA0C}" name="Tabela21657" displayName="Tabela21657" ref="A23:C29" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4" tableBorderDxfId="3">
+  <autoFilter ref="A23:C29" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{66272961-D89D-4DD2-807F-D10CF138519D}" name="NOME" dataDxfId="88"/>
-    <tableColumn id="2" xr3:uid="{9700B9DF-18DC-4FF9-B87F-CA8E809DFE18}" name="PARTICIPAÇÃO" dataDxfId="87"/>
-    <tableColumn id="3" xr3:uid="{336A4CF9-2C48-4740-BBCF-05EBC653EB59}" name="JUSTIFICATIVA" dataDxfId="86"/>
+    <tableColumn id="1" xr3:uid="{E570557C-2EE0-4811-A62D-094AB9B0C9BC}" name="NOME" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{89F08E2F-F9ED-4424-B655-EEE89E3DA5A7}" name="PARTICIPAÇÃO" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{DE6C6C5E-3892-42A9-B8A6-EDE8DE750751}" name="JUSTIFICATIVA" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3672,7 +3672,7 @@
     </row>
     <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B5" s="6">
         <v>45567</v>
@@ -3704,7 +3704,7 @@
     </row>
     <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B7" s="6">
         <v>45567</v>
@@ -3732,7 +3732,7 @@
     </row>
     <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B9" s="6">
         <v>45567</v>
@@ -3760,7 +3760,7 @@
     </row>
     <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B11" s="6">
         <v>45567</v>
@@ -3774,7 +3774,7 @@
     </row>
     <row r="12" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B12" s="6">
         <v>45567</v>
@@ -3788,7 +3788,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B13" s="6">
         <v>45567</v>
@@ -3802,7 +3802,7 @@
     </row>
     <row r="14" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B14" s="6">
         <v>45567</v>
@@ -3831,7 +3831,7 @@
     </row>
     <row r="18" spans="1:4" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B18" s="31"/>
       <c r="C18" s="31"/>
@@ -3967,21 +3967,21 @@
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="B25:B30">
-    <cfRule type="cellIs" dxfId="32" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="4" operator="equal">
       <formula>"AUSENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="5" operator="equal">
       <formula>"PRESENTE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D14">
-    <cfRule type="cellIs" dxfId="30" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="1" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="2" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="3" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4076,7 +4076,7 @@
     </row>
     <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B5" s="6">
         <v>45567</v>
@@ -4108,7 +4108,7 @@
     </row>
     <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B7" s="6">
         <v>45565</v>
@@ -4136,7 +4136,7 @@
     </row>
     <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B9" s="6">
         <v>45567</v>
@@ -4164,7 +4164,7 @@
     </row>
     <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B11" s="6">
         <v>45565</v>
@@ -4178,7 +4178,7 @@
     </row>
     <row r="12" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B12" s="6">
         <v>45565</v>
@@ -4192,7 +4192,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B13" s="6">
         <v>45565</v>
@@ -4206,7 +4206,7 @@
     </row>
     <row r="14" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B14" s="6">
         <v>45567</v>
@@ -4235,7 +4235,7 @@
     </row>
     <row r="18" spans="1:4" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="30" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B18" s="31"/>
       <c r="C18" s="31"/>
@@ -4367,21 +4367,21 @@
     <mergeCell ref="A23:C23"/>
   </mergeCells>
   <conditionalFormatting sqref="B25:B30">
-    <cfRule type="cellIs" dxfId="27" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="4" operator="equal">
       <formula>"AUSENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="5" operator="equal">
       <formula>"PRESENTE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D14">
-    <cfRule type="cellIs" dxfId="25" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="1" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="2" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="3" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4421,8 +4421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25161DFF-344A-4C41-AE51-A14BEC6B2F7D}">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:D20"/>
+    <sheetView showGridLines="0" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -4476,7 +4476,7 @@
     </row>
     <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B5" s="6">
         <v>45565</v>
@@ -4494,7 +4494,7 @@
     </row>
     <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6" s="6">
         <v>45565</v>
@@ -4508,7 +4508,7 @@
     </row>
     <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B7" s="6">
         <v>45565</v>
@@ -4522,7 +4522,7 @@
     </row>
     <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B8" s="6">
         <v>45565</v>
@@ -4536,7 +4536,7 @@
     </row>
     <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B9" s="6">
         <v>45567</v>
@@ -4578,7 +4578,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B12" s="6">
         <v>45567</v>
@@ -4592,7 +4592,7 @@
     </row>
     <row r="13" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B13" s="6">
         <v>45567</v>
@@ -4621,7 +4621,7 @@
     </row>
     <row r="17" spans="1:4" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="30" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B17" s="31"/>
       <c r="C17" s="31"/>
@@ -4753,21 +4753,21 @@
     <mergeCell ref="A22:C22"/>
   </mergeCells>
   <conditionalFormatting sqref="B24:B29">
-    <cfRule type="cellIs" dxfId="22" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="4" operator="equal">
       <formula>"AUSENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="5" operator="equal">
       <formula>"PRESENTE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D13">
-    <cfRule type="cellIs" dxfId="20" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="1" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="2" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="3" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4804,11 +4804,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D02FDE50-A72F-4C17-8A91-E281A42AFC5E}">
-  <dimension ref="A1:I26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19BF0B73-CACA-492F-8733-CCF61DB202E2}">
+  <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" zoomScale="66" zoomScaleNormal="46" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -4862,238 +4862,283 @@
     </row>
     <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="B5" s="6">
-        <v>45556</v>
+        <v>45565</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>16</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="F5"/>
+      <c r="G5"/>
+      <c r="H5"/>
+      <c r="I5"/>
     </row>
     <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="B6" s="6">
-        <v>45559</v>
+        <v>45565</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="B7" s="6">
-        <v>45556</v>
+        <v>45565</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="B8" s="6">
-        <v>45559</v>
+        <v>45565</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
       <c r="B9" s="6">
-        <v>45555</v>
+        <v>45567</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B10" s="6">
-        <v>45558</v>
+        <v>45567</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="5"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-    </row>
-    <row r="12" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="13" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="24" t="s">
+      <c r="A11" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="6">
+        <v>45567</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="6">
+        <v>45567</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" s="6">
+        <v>45567</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="5"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+    </row>
+    <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="16" spans="1:9" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="25"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="26"/>
-    </row>
-    <row r="14" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" s="31"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="32"/>
-    </row>
-    <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="33"/>
-      <c r="B15" s="34"/>
-      <c r="C15" s="34"/>
-      <c r="D15" s="35"/>
-    </row>
-    <row r="16" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="33"/>
-      <c r="B16" s="34"/>
-      <c r="C16" s="34"/>
-      <c r="D16" s="35"/>
-    </row>
-    <row r="17" spans="1:5" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="36"/>
-      <c r="B17" s="37"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="38"/>
-    </row>
-    <row r="18" spans="1:5" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="19" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="27" t="s">
+      <c r="B16" s="25"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="26"/>
+    </row>
+    <row r="17" spans="1:4" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" s="31"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="32"/>
+    </row>
+    <row r="18" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="33"/>
+      <c r="B18" s="34"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="35"/>
+    </row>
+    <row r="19" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="33"/>
+      <c r="B19" s="34"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="35"/>
+    </row>
+    <row r="20" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="36"/>
+      <c r="B20" s="37"/>
+      <c r="C20" s="37"/>
+      <c r="D20" s="38"/>
+    </row>
+    <row r="21" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="22" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="28"/>
-      <c r="C19" s="29"/>
-      <c r="D19" s="12" t="s">
+      <c r="B22" s="28"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="10" t="s">
+    <row r="23" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B23" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C23" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="4">
-        <v>45558</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="2" t="s">
+      <c r="D23" s="4">
+        <v>45565</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C21" s="5"/>
-      <c r="D21" s="12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22" s="5"/>
-      <c r="D22" s="7">
-        <v>0.6958333333333333</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23" s="5"/>
-      <c r="D23" s="12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C24" s="5"/>
-      <c r="D24" s="8">
-        <v>0.70138888888888884</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D24" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C25" s="5"/>
-      <c r="D25" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D25" s="7">
+        <v>0.68055555555555558</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C26" s="5"/>
-      <c r="D26" s="3">
-        <f>IF(D24="","",D24-D22)</f>
-        <v>5.5555555555555358E-3</v>
-      </c>
-      <c r="E26" s="13"/>
+      <c r="D26" s="12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" s="5"/>
+      <c r="D27" s="8">
+        <v>0.69513888888888886</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C28" s="5"/>
+      <c r="D28" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A29" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" s="5"/>
+      <c r="D29" s="3">
+        <f>IF(D27="","",D27-D25)</f>
+        <v>1.4583333333333282E-2</v>
+      </c>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <mergeCells count="5">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A13:D13"/>
-    <mergeCell ref="A14:D17"/>
-    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="A17:D20"/>
+    <mergeCell ref="A22:C22"/>
   </mergeCells>
-  <conditionalFormatting sqref="B21:B26">
+  <conditionalFormatting sqref="B24:B29">
     <cfRule type="cellIs" dxfId="17" priority="4" operator="equal">
       <formula>"AUSENTE"</formula>
     </cfRule>
@@ -5101,7 +5146,7 @@
       <formula>"PRESENTE"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D5:D10">
+  <conditionalFormatting sqref="D5:D13">
     <cfRule type="cellIs" dxfId="15" priority="1" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
@@ -5113,8 +5158,8 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C11" xr:uid="{FAF4B15F-74B3-47F5-8B43-50363D8DED82}">
-      <formula1>$A$21:$A$26</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C14" xr:uid="{60E3DDA1-5313-49D8-A931-D16E2F618759}">
+      <formula1>$A$24:$A$29</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -5126,17 +5171,17 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3CEAE7ED-D488-483E-8209-BAF021E091E9}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CE995811-7E4B-4AF5-BAA5-8633E95526C3}">
           <x14:formula1>
             <xm:f>'BANCO DE DADOS'!$B$1:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>D5:D11</xm:sqref>
+          <xm:sqref>D5:D14</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D3856752-E5AE-441F-B371-26D903C39A26}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4BEE6107-5995-4902-99D2-CB1B88A8E637}">
           <x14:formula1>
             <xm:f>'BANCO DE DADOS'!$A$1:$A$2</xm:f>
           </x14:formula1>
-          <xm:sqref>B21:B26</xm:sqref>
+          <xm:sqref>B24:B29</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -5302,7 +5347,7 @@
     </row>
     <row r="14" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B14" s="31"/>
       <c r="C14" s="31"/>
@@ -5419,7 +5464,7 @@
         <v>15</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D26" s="3">
         <f>IF(D24="","",D24-D22)</f>
@@ -5437,21 +5482,21 @@
     <mergeCell ref="A19:C19"/>
   </mergeCells>
   <conditionalFormatting sqref="B21:B26">
-    <cfRule type="cellIs" dxfId="12" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="4" operator="equal">
       <formula>"AUSENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="5" operator="equal">
       <formula>"PRESENTE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D10">
-    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="1" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="2" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="3" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5645,7 +5690,7 @@
     </row>
     <row r="14" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="30" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B14" s="31"/>
       <c r="C14" s="31"/>
@@ -5778,21 +5823,21 @@
     <mergeCell ref="A19:C19"/>
   </mergeCells>
   <conditionalFormatting sqref="B21:B26">
-    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="4" operator="equal">
       <formula>"AUSENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="5" operator="equal">
       <formula>"PRESENTE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D10">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="1" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="2" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="3" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5855,7 +5900,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="39.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B1" s="25"/>
       <c r="C1" s="25"/>
@@ -5869,13 +5914,13 @@
     <row r="2" spans="1:9" customFormat="1" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="3" spans="1:9" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B3" s="25"/>
       <c r="C3" s="25"/>
       <c r="D3" s="26"/>
       <c r="F3" s="24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G3" s="25"/>
       <c r="H3" s="25"/>
@@ -5883,35 +5928,35 @@
     </row>
     <row r="4" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4" s="50" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="50"/>
-      <c r="D4" s="51"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="42"/>
       <c r="F4" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="G4" s="50"/>
-      <c r="H4" s="50"/>
-      <c r="I4" s="51"/>
+        <v>39</v>
+      </c>
+      <c r="G4" s="41"/>
+      <c r="H4" s="41"/>
+      <c r="I4" s="42"/>
     </row>
     <row r="5" spans="1:9" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="B5" s="52" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="52"/>
-      <c r="D5" s="53"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="44"/>
       <c r="F5" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="G5" s="52"/>
-      <c r="H5" s="52"/>
-      <c r="I5" s="53"/>
+        <v>40</v>
+      </c>
+      <c r="G5" s="43"/>
+      <c r="H5" s="43"/>
+      <c r="I5" s="44"/>
     </row>
     <row r="6" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="7" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
@@ -5946,7 +5991,7 @@
       <c r="C8" s="5"/>
       <c r="D8" s="23"/>
       <c r="F8" s="22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G8" s="6">
         <v>45567</v>
@@ -5982,7 +6027,7 @@
       <c r="C10" s="5"/>
       <c r="D10" s="23"/>
       <c r="F10" s="22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G10" s="6">
         <v>45567</v>
@@ -6016,7 +6061,7 @@
       <c r="A12" s="19"/>
       <c r="D12" s="18"/>
       <c r="F12" s="22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G12" s="6">
         <v>45567</v>
@@ -6030,13 +6075,13 @@
     </row>
     <row r="13" spans="1:9" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B13" s="25"/>
       <c r="C13" s="25"/>
       <c r="D13" s="26"/>
       <c r="F13" s="22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G13" s="6">
         <v>45567</v>
@@ -6054,7 +6099,7 @@
       <c r="C14" s="31"/>
       <c r="D14" s="32"/>
       <c r="F14" s="22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G14" s="6">
         <v>45567</v>
@@ -6072,7 +6117,7 @@
       <c r="C15" s="34"/>
       <c r="D15" s="35"/>
       <c r="F15" s="22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G15" s="6">
         <v>45567</v>
@@ -6090,7 +6135,7 @@
       <c r="C16" s="34"/>
       <c r="D16" s="35"/>
       <c r="F16" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G16" s="6">
         <v>45567</v>
@@ -6108,7 +6153,7 @@
       <c r="C17" s="37"/>
       <c r="D17" s="38"/>
       <c r="F17" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G17" s="6">
         <v>45567</v>
@@ -6127,91 +6172,99 @@
       <c r="D18" s="15"/>
     </row>
     <row r="19" spans="1:9" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="54" t="s">
+      <c r="A19" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="55"/>
-      <c r="C19" s="55"/>
-      <c r="D19" s="56"/>
+      <c r="B19" s="46"/>
+      <c r="C19" s="46"/>
+      <c r="D19" s="47"/>
       <c r="F19"/>
       <c r="G19"/>
     </row>
     <row r="20" spans="1:9" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="61" t="s">
+      <c r="A20" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="62"/>
-      <c r="C20" s="57" t="s">
-        <v>49</v>
-      </c>
-      <c r="D20" s="58"/>
+      <c r="B20" s="53"/>
+      <c r="C20" s="48" t="s">
+        <v>48</v>
+      </c>
+      <c r="D20" s="49"/>
       <c r="E20" s="13"/>
       <c r="F20"/>
       <c r="G20"/>
     </row>
     <row r="21" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="63" t="s">
+      <c r="A21" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="59"/>
-      <c r="C21" s="59" t="s">
+      <c r="B21" s="50"/>
+      <c r="C21" s="50" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" s="51"/>
+    </row>
+    <row r="22" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="55" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="39"/>
+      <c r="C22" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="D21" s="60"/>
-    </row>
-    <row r="22" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="B22" s="48"/>
-      <c r="C22" s="48" t="s">
+      <c r="D22" s="40"/>
+    </row>
+    <row r="23" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="56" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="57"/>
+      <c r="C23" s="57" t="s">
         <v>51</v>
       </c>
-      <c r="D22" s="49"/>
-    </row>
-    <row r="23" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="39" t="s">
-        <v>10</v>
-      </c>
-      <c r="B23" s="40"/>
-      <c r="C23" s="40" t="s">
+      <c r="D23" s="63"/>
+    </row>
+    <row r="24" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="58" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" s="59"/>
+      <c r="C24" s="59" t="s">
         <v>52</v>
       </c>
-      <c r="D23" s="46"/>
-    </row>
-    <row r="24" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="41" t="s">
-        <v>11</v>
-      </c>
-      <c r="B24" s="42"/>
-      <c r="C24" s="42" t="s">
+      <c r="D24" s="64"/>
+    </row>
+    <row r="25" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="56" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="57"/>
+      <c r="C25" s="57" t="s">
         <v>53</v>
       </c>
-      <c r="D24" s="47"/>
-    </row>
-    <row r="25" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="B25" s="40"/>
-      <c r="C25" s="40" t="s">
+      <c r="D25" s="63"/>
+    </row>
+    <row r="26" spans="1:9" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="60" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="61"/>
+      <c r="C26" s="61" t="s">
         <v>54</v>
       </c>
-      <c r="D25" s="46"/>
-    </row>
-    <row r="26" spans="1:9" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="43" t="s">
-        <v>13</v>
-      </c>
-      <c r="B26" s="44"/>
-      <c r="C26" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="D26" s="45"/>
+      <c r="D26" s="62"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <mergeCells count="24">
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="A25:B25"/>
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="A13:D13"/>
     <mergeCell ref="A14:D17"/>
@@ -6228,27 +6281,24 @@
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="A25:B25"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="D8:D11 I8:I17">
-    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="6" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="7" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="8" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8:C11" xr:uid="{8EFBC24D-2650-46F5-BA77-660A84572B57}">
+      <formula1>#REF!</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" scale="56" orientation="landscape" r:id="rId1"/>
   <tableParts count="2">
@@ -6257,18 +6307,12 @@
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{170DC6ED-100C-48FE-A29D-3864A9024536}">
           <x14:formula1>
             <xm:f>'BANCO DE DADOS'!$B$1:$B$3</xm:f>
           </x14:formula1>
           <xm:sqref>D8:D11 I8:I17</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8EFBC24D-2650-46F5-BA77-660A84572B57}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>C8:C11</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2E14A627-A508-4036-9948-768B809E3863}">
           <x14:formula1>

</xml_diff>

<commit_message>
Adição da ATA do dia 01/10/2024
</commit_message>
<xml_diff>
--- a/ATAs_de_Reuniao/Sprint 2/Semana 2609/Grupo4_ATA_Semana2609.xlsx
+++ b/ATAs_de_Reuniao/Sprint 2/Semana 2609/Grupo4_ATA_Semana2609.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Documents\Projeto_PI\sprint2\ATAs_de_Reuniao\Sprint 2\Semana 2609\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SPTech\GitHub\Sprint-SPTECH\ATAs_de_Reuniao\Sprint 2\Semana 2609\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B51C9FBF-A596-44BE-98D1-B224AB39501A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D738B761-BB7D-455F-9946-4005A5D4C153}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="4" xr2:uid="{D70EAD62-B489-48DA-AED6-4403B2320B59}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="5" xr2:uid="{D70EAD62-B489-48DA-AED6-4403B2320B59}"/>
   </bookViews>
   <sheets>
     <sheet name="BANCO DE DADOS" sheetId="2" state="hidden" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Sexta" sheetId="11" r:id="rId3"/>
     <sheet name="Sábado" sheetId="12" r:id="rId4"/>
     <sheet name="Segunda" sheetId="13" r:id="rId5"/>
-    <sheet name="Terça" sheetId="7" r:id="rId6"/>
+    <sheet name="Terça" sheetId="14" r:id="rId6"/>
     <sheet name="Quarta" sheetId="9" r:id="rId7"/>
     <sheet name="SEMANAL" sheetId="10" r:id="rId8"/>
   </sheets>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="62">
   <si>
     <t>NOME</t>
   </si>
@@ -147,12 +147,6 @@
     <t>APRESENTAÇÃO DE TI</t>
   </si>
   <si>
-    <t>Foi feito o treinamento da apresentação sobre a metodologia PERT</t>
-  </si>
-  <si>
-    <t>Apresentação na junta militar</t>
-  </si>
-  <si>
     <t>Foi discutido sobre os próximos passos para o andamento da Sprint, onde ficou estabelecido que iremos validar com o Frizza(cliente) na próxima aula sobre o andamento do projeto.</t>
   </si>
   <si>
@@ -229,6 +223,12 @@
   </si>
   <si>
     <t>Definimos as tarefas semanais que poderão ser entregues até segunda-feira (30/09).</t>
+  </si>
+  <si>
+    <t>Foi apresentado o trabalho feito no final de semana por cada integrante do grupo e decidido como seria o novo protótipo do Site. Também definimos pontos acerca das tabelas que farão parte do banco de dados.</t>
+  </si>
+  <si>
+    <t>Foi discutido sobre o prazo da entrega das atividades, falado sobre o mySQL na VM local e por ultimo também realizamos um teste para a apresentação sobre a metodologia PERT</t>
   </si>
 </sst>
 </file>
@@ -876,6 +876,33 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -927,33 +954,6 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="8" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="8" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="8" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="8" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="8" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="8" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1129,7 +1129,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -1595,7 +1595,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -1731,7 +1731,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -1980,7 +1980,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -2229,7 +2229,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -2478,7 +2478,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -2727,7 +2727,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -2976,7 +2976,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -3082,12 +3082,12 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{5A356893-9A8B-4B13-8C28-51E182146249}" name="Tabela257911" displayName="Tabela257911" ref="A20:C26" totalsRowShown="0" headerRowDxfId="78" dataDxfId="77" tableBorderDxfId="76">
-  <autoFilter ref="A20:C26" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{1191F4CB-7F6D-485B-AC60-0502347DD05B}" name="Tabela216579" displayName="Tabela216579" ref="A23:C29" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4" tableBorderDxfId="3">
+  <autoFilter ref="A23:C29" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{139E8E28-282E-4954-A42E-FF13F888D8CB}" name="NOME" dataDxfId="75"/>
-    <tableColumn id="2" xr3:uid="{2D2F98D9-24BC-48E1-977F-50AADAAFFCD7}" name="PARTICIPAÇÃO" dataDxfId="74"/>
-    <tableColumn id="3" xr3:uid="{ECE86497-A781-4678-B780-5FE8694A399F}" name="JUSTIFICATIVA" dataDxfId="73"/>
+    <tableColumn id="1" xr3:uid="{8CE1CFB1-3B41-4ED3-8123-1F497AD0EBF4}" name="NOME" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{D65F61F3-2928-4DDE-B139-E3881CA88028}" name="PARTICIPAÇÃO" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{E75E5DBF-4EBF-4291-8B2C-1C27A0B29355}" name="JUSTIFICATIVA" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3213,41 +3213,44 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{6C031CDA-53E0-45FD-9AE0-557E1E0765C8}" name="Tabela11546" displayName="Tabela11546" ref="A4:D14" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11" tableBorderDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{6C031CDA-53E0-45FD-9AE0-557E1E0765C8}" name="Tabela11546" displayName="Tabela11546" ref="A4:D14" totalsRowShown="0" headerRowDxfId="85" dataDxfId="84" tableBorderDxfId="83">
   <autoFilter ref="A4:D14" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:D14">
     <sortCondition ref="B5:B14"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{BB742C24-B969-47D8-BDF5-2D9DD9DE0453}" name="O QUE FAZER" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{08450859-D0AC-4147-80B0-0A2BE06A68E3}" name="PRAZOS DE ENTREGA" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{90CA058E-F8FF-4FF1-BD90-FA898BB69129}" name="RESPONSAVEL" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{4533BAE4-7102-4B9B-8C5E-D2327FE6E37B}" name="SITUAÇÃO" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{BB742C24-B969-47D8-BDF5-2D9DD9DE0453}" name="O QUE FAZER" dataDxfId="82"/>
+    <tableColumn id="2" xr3:uid="{08450859-D0AC-4147-80B0-0A2BE06A68E3}" name="PRAZOS DE ENTREGA" dataDxfId="81"/>
+    <tableColumn id="3" xr3:uid="{90CA058E-F8FF-4FF1-BD90-FA898BB69129}" name="RESPONSAVEL" dataDxfId="80"/>
+    <tableColumn id="4" xr3:uid="{4533BAE4-7102-4B9B-8C5E-D2327FE6E37B}" name="SITUAÇÃO" dataDxfId="79"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{34D2C419-0C8F-420E-9F09-51777412EA0C}" name="Tabela21657" displayName="Tabela21657" ref="A23:C29" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4" tableBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{34D2C419-0C8F-420E-9F09-51777412EA0C}" name="Tabela21657" displayName="Tabela21657" ref="A23:C29" totalsRowShown="0" headerRowDxfId="78" dataDxfId="77" tableBorderDxfId="76">
   <autoFilter ref="A23:C29" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{E570557C-2EE0-4811-A62D-094AB9B0C9BC}" name="NOME" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{89F08E2F-F9ED-4424-B655-EEE89E3DA5A7}" name="PARTICIPAÇÃO" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{DE6C6C5E-3892-42A9-B8A6-EDE8DE750751}" name="JUSTIFICATIVA" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{E570557C-2EE0-4811-A62D-094AB9B0C9BC}" name="NOME" dataDxfId="75"/>
+    <tableColumn id="2" xr3:uid="{89F08E2F-F9ED-4424-B655-EEE89E3DA5A7}" name="PARTICIPAÇÃO" dataDxfId="74"/>
+    <tableColumn id="3" xr3:uid="{DE6C6C5E-3892-42A9-B8A6-EDE8DE750751}" name="JUSTIFICATIVA" dataDxfId="73"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{4239FFAB-7F81-4D5D-933C-45DFBF3605AD}" name="Tabela146810" displayName="Tabela146810" ref="A4:D11" totalsRowShown="0" headerRowDxfId="85" dataDxfId="84" tableBorderDxfId="83">
-  <autoFilter ref="A4:D11" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{433F7683-AF81-4BA7-9443-5B185A6FB802}" name="Tabela115468" displayName="Tabela115468" ref="A4:D14" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11" tableBorderDxfId="10">
+  <autoFilter ref="A4:D14" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:D14">
+    <sortCondition ref="B5:B14"/>
+  </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{04C4A5A4-6229-4505-8F11-B7E824AC1473}" name="O QUE FAZER" dataDxfId="82"/>
-    <tableColumn id="2" xr3:uid="{E21C73CF-DFCA-4323-8C97-CBB757FA2560}" name="PRAZOS DE ENTREGA" dataDxfId="81"/>
-    <tableColumn id="3" xr3:uid="{9A31040F-148F-42BE-8FBC-5FCB2398EFB4}" name="RESPONSAVEL" dataDxfId="80"/>
-    <tableColumn id="4" xr3:uid="{4756F678-1E57-4686-8D68-E8BB92990CAB}" name="SITUAÇÃO" dataDxfId="79"/>
+    <tableColumn id="1" xr3:uid="{9478A723-D368-432D-B04D-0CE3A8B04818}" name="O QUE FAZER" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{299E99A9-2BDD-4259-B821-126259D6061E}" name="PRAZOS DE ENTREGA" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{885DF8C6-2582-4A91-9775-AD5DDBFE5E62}" name="RESPONSAVEL" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{653F985A-2FB8-486B-BC74-444331BCE755}" name="SITUAÇÃO" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3576,12 +3579,12 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="18.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -3592,7 +3595,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -3603,7 +3606,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>18</v>
       </c>
@@ -3621,17 +3624,17 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.453125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.08984375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.453125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.453125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.08984375" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.90625" style="1"/>
+    <col min="1" max="1" width="34.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>24</v>
       </c>
@@ -3639,8 +3642,8 @@
       <c r="C1" s="25"/>
       <c r="D1" s="26"/>
     </row>
-    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="24" t="s">
         <v>2</v>
       </c>
@@ -3652,7 +3655,7 @@
       <c r="H3"/>
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -3670,9 +3673,9 @@
       <c r="H4"/>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B5" s="6">
         <v>45567</v>
@@ -3688,7 +3691,7 @@
       <c r="H5"/>
       <c r="I5"/>
     </row>
-    <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>30</v>
       </c>
@@ -3702,9 +3705,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B7" s="6">
         <v>45567</v>
@@ -3716,7 +3719,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>28</v>
       </c>
@@ -3730,9 +3733,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B9" s="6">
         <v>45567</v>
@@ -3744,7 +3747,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>28</v>
       </c>
@@ -3758,9 +3761,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B11" s="6">
         <v>45567</v>
@@ -3772,9 +3775,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B12" s="6">
         <v>45567</v>
@@ -3786,9 +3789,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B13" s="6">
         <v>45567</v>
@@ -3800,9 +3803,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B14" s="6">
         <v>45567</v>
@@ -3814,14 +3817,14 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="6"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
     </row>
-    <row r="16" spans="1:9" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="17" spans="1:4" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:9" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="1:4" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="24" t="s">
         <v>32</v>
       </c>
@@ -3829,34 +3832,34 @@
       <c r="C17" s="25"/>
       <c r="D17" s="26"/>
     </row>
-    <row r="18" spans="1:4" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="30" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B18" s="31"/>
       <c r="C18" s="31"/>
       <c r="D18" s="32"/>
     </row>
-    <row r="19" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="33"/>
       <c r="B19" s="34"/>
       <c r="C19" s="34"/>
       <c r="D19" s="35"/>
     </row>
-    <row r="20" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="33"/>
       <c r="B20" s="34"/>
       <c r="C20" s="34"/>
       <c r="D20" s="35"/>
     </row>
-    <row r="21" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="36"/>
       <c r="B21" s="37"/>
       <c r="C21" s="37"/>
       <c r="D21" s="38"/>
     </row>
-    <row r="22" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="23" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="27" t="s">
         <v>19</v>
       </c>
@@ -3866,7 +3869,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
         <v>0</v>
       </c>
@@ -3880,7 +3883,7 @@
         <v>45561</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>8</v>
       </c>
@@ -3892,7 +3895,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>9</v>
       </c>
@@ -3904,7 +3907,7 @@
         <v>0.68819444444444444</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>10</v>
       </c>
@@ -3916,7 +3919,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>11</v>
       </c>
@@ -3928,7 +3931,7 @@
         <v>0.69930555555555551</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>12</v>
       </c>
@@ -3940,7 +3943,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>13</v>
       </c>
@@ -4025,17 +4028,17 @@
       <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.453125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.08984375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.453125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.453125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.08984375" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.90625" style="1"/>
+    <col min="1" max="1" width="34.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>24</v>
       </c>
@@ -4043,8 +4046,8 @@
       <c r="C1" s="25"/>
       <c r="D1" s="26"/>
     </row>
-    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="24" t="s">
         <v>2</v>
       </c>
@@ -4056,7 +4059,7 @@
       <c r="H3"/>
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -4074,9 +4077,9 @@
       <c r="H4"/>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B5" s="6">
         <v>45567</v>
@@ -4092,7 +4095,7 @@
       <c r="H5"/>
       <c r="I5"/>
     </row>
-    <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>30</v>
       </c>
@@ -4106,9 +4109,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B7" s="6">
         <v>45565</v>
@@ -4120,7 +4123,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>28</v>
       </c>
@@ -4134,9 +4137,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B9" s="6">
         <v>45567</v>
@@ -4148,7 +4151,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>28</v>
       </c>
@@ -4162,9 +4165,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B11" s="6">
         <v>45565</v>
@@ -4176,9 +4179,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B12" s="6">
         <v>45565</v>
@@ -4190,9 +4193,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B13" s="6">
         <v>45565</v>
@@ -4204,9 +4207,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B14" s="6">
         <v>45567</v>
@@ -4218,14 +4221,14 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="6"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
     </row>
-    <row r="16" spans="1:9" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="17" spans="1:4" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:9" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="1:4" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="24" t="s">
         <v>32</v>
       </c>
@@ -4233,34 +4236,34 @@
       <c r="C17" s="25"/>
       <c r="D17" s="26"/>
     </row>
-    <row r="18" spans="1:4" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="30" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B18" s="31"/>
       <c r="C18" s="31"/>
       <c r="D18" s="32"/>
     </row>
-    <row r="19" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="33"/>
       <c r="B19" s="34"/>
       <c r="C19" s="34"/>
       <c r="D19" s="35"/>
     </row>
-    <row r="20" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="33"/>
       <c r="B20" s="34"/>
       <c r="C20" s="34"/>
       <c r="D20" s="35"/>
     </row>
-    <row r="21" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="36"/>
       <c r="B21" s="37"/>
       <c r="C21" s="37"/>
       <c r="D21" s="38"/>
     </row>
-    <row r="22" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="23" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="27" t="s">
         <v>19</v>
       </c>
@@ -4270,7 +4273,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
         <v>0</v>
       </c>
@@ -4284,7 +4287,7 @@
         <v>45562</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>8</v>
       </c>
@@ -4296,7 +4299,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>9</v>
       </c>
@@ -4308,7 +4311,7 @@
         <v>0.68541666666666667</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>10</v>
       </c>
@@ -4320,7 +4323,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>11</v>
       </c>
@@ -4332,7 +4335,7 @@
         <v>0.69930555555555551</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>12</v>
       </c>
@@ -4344,7 +4347,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>13</v>
       </c>
@@ -4425,17 +4428,17 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.453125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.08984375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.453125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.453125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.08984375" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.90625" style="1"/>
+    <col min="1" max="1" width="34.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>24</v>
       </c>
@@ -4443,8 +4446,8 @@
       <c r="C1" s="25"/>
       <c r="D1" s="26"/>
     </row>
-    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="24" t="s">
         <v>2</v>
       </c>
@@ -4456,7 +4459,7 @@
       <c r="H3"/>
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -4474,9 +4477,9 @@
       <c r="H4"/>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B5" s="6">
         <v>45565</v>
@@ -4492,9 +4495,9 @@
       <c r="H5"/>
       <c r="I5"/>
     </row>
-    <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B6" s="6">
         <v>45565</v>
@@ -4506,9 +4509,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B7" s="6">
         <v>45565</v>
@@ -4520,9 +4523,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B8" s="6">
         <v>45565</v>
@@ -4534,9 +4537,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B9" s="6">
         <v>45567</v>
@@ -4548,7 +4551,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>30</v>
       </c>
@@ -4562,7 +4565,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>28</v>
       </c>
@@ -4576,9 +4579,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B12" s="6">
         <v>45567</v>
@@ -4590,9 +4593,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B13" s="6">
         <v>45567</v>
@@ -4604,14 +4607,14 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="6"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
     </row>
-    <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="16" spans="1:9" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:9" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:9" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="24" t="s">
         <v>32</v>
       </c>
@@ -4619,34 +4622,34 @@
       <c r="C16" s="25"/>
       <c r="D16" s="26"/>
     </row>
-    <row r="17" spans="1:4" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="30" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B17" s="31"/>
       <c r="C17" s="31"/>
       <c r="D17" s="32"/>
     </row>
-    <row r="18" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="33"/>
       <c r="B18" s="34"/>
       <c r="C18" s="34"/>
       <c r="D18" s="35"/>
     </row>
-    <row r="19" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="33"/>
       <c r="B19" s="34"/>
       <c r="C19" s="34"/>
       <c r="D19" s="35"/>
     </row>
-    <row r="20" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="36"/>
       <c r="B20" s="37"/>
       <c r="C20" s="37"/>
       <c r="D20" s="38"/>
     </row>
-    <row r="21" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="22" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="27" t="s">
         <v>19</v>
       </c>
@@ -4656,7 +4659,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
         <v>0</v>
       </c>
@@ -4670,7 +4673,7 @@
         <v>45563</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>8</v>
       </c>
@@ -4682,7 +4685,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>9</v>
       </c>
@@ -4694,7 +4697,7 @@
         <v>0.41875000000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>10</v>
       </c>
@@ -4706,7 +4709,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>11</v>
       </c>
@@ -4718,7 +4721,7 @@
         <v>0.4284722222222222</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>12</v>
       </c>
@@ -4730,7 +4733,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>13</v>
       </c>
@@ -4807,21 +4810,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19BF0B73-CACA-492F-8733-CCF61DB202E2}">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.453125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.08984375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.453125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.453125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.08984375" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.90625" style="1"/>
+    <col min="1" max="1" width="34.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>24</v>
       </c>
@@ -4829,8 +4832,8 @@
       <c r="C1" s="25"/>
       <c r="D1" s="26"/>
     </row>
-    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="24" t="s">
         <v>2</v>
       </c>
@@ -4842,7 +4845,7 @@
       <c r="H3"/>
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -4860,12 +4863,12 @@
       <c r="H4"/>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B5" s="6">
-        <v>45565</v>
+        <v>45569</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>9</v>
@@ -4878,12 +4881,12 @@
       <c r="H5"/>
       <c r="I5"/>
     </row>
-    <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B6" s="6">
-        <v>45565</v>
+        <v>45568</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>12</v>
@@ -4892,12 +4895,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B7" s="6">
-        <v>45565</v>
+        <v>45569</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>12</v>
@@ -4906,12 +4909,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B8" s="6">
-        <v>45565</v>
+        <v>45568</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>13</v>
@@ -4920,9 +4923,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B9" s="6">
         <v>45567</v>
@@ -4934,7 +4937,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>30</v>
       </c>
@@ -4948,7 +4951,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>28</v>
       </c>
@@ -4962,9 +4965,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B12" s="6">
         <v>45567</v>
@@ -4976,9 +4979,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B13" s="6">
         <v>45567</v>
@@ -4990,14 +4993,14 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="6"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
     </row>
-    <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="16" spans="1:9" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:9" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:9" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="24" t="s">
         <v>32</v>
       </c>
@@ -5005,34 +5008,34 @@
       <c r="C16" s="25"/>
       <c r="D16" s="26"/>
     </row>
-    <row r="17" spans="1:4" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="30" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B17" s="31"/>
       <c r="C17" s="31"/>
       <c r="D17" s="32"/>
     </row>
-    <row r="18" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="33"/>
       <c r="B18" s="34"/>
       <c r="C18" s="34"/>
       <c r="D18" s="35"/>
     </row>
-    <row r="19" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="33"/>
       <c r="B19" s="34"/>
       <c r="C19" s="34"/>
       <c r="D19" s="35"/>
     </row>
-    <row r="20" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="36"/>
       <c r="B20" s="37"/>
       <c r="C20" s="37"/>
       <c r="D20" s="38"/>
     </row>
-    <row r="21" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="22" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="27" t="s">
         <v>19</v>
       </c>
@@ -5042,7 +5045,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
         <v>0</v>
       </c>
@@ -5056,7 +5059,7 @@
         <v>45565</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>8</v>
       </c>
@@ -5068,7 +5071,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>9</v>
       </c>
@@ -5080,7 +5083,7 @@
         <v>0.68055555555555558</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>10</v>
       </c>
@@ -5092,7 +5095,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>11</v>
       </c>
@@ -5104,7 +5107,7 @@
         <v>0.69513888888888886</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>12</v>
       </c>
@@ -5116,7 +5119,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>13</v>
       </c>
@@ -5139,21 +5142,21 @@
     <mergeCell ref="A22:C22"/>
   </mergeCells>
   <conditionalFormatting sqref="B24:B29">
-    <cfRule type="cellIs" dxfId="17" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="4" operator="equal">
       <formula>"AUSENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="5" operator="equal">
       <formula>"PRESENTE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D13">
-    <cfRule type="cellIs" dxfId="15" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="1" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="2" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="3" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5190,24 +5193,24 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F4FDFF8-372F-4860-BF40-AFBF460A6F78}">
-  <dimension ref="A1:I26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4588FE3E-D7A2-4335-AA32-FE123603ED1D}">
+  <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" zoomScale="66" zoomScaleNormal="46" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:D23"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.453125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.08984375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.453125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.453125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.08984375" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.90625" style="1"/>
+    <col min="1" max="1" width="34.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>24</v>
       </c>
@@ -5215,8 +5218,8 @@
       <c r="C1" s="25"/>
       <c r="D1" s="26"/>
     </row>
-    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="24" t="s">
         <v>2</v>
       </c>
@@ -5228,7 +5231,7 @@
       <c r="H3"/>
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -5246,263 +5249,306 @@
       <c r="H4"/>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="B5" s="6">
-        <v>45556</v>
+        <v>45569</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+      <c r="F5"/>
+      <c r="G5"/>
+      <c r="H5"/>
+      <c r="I5"/>
+    </row>
+    <row r="6" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="B6" s="6">
-        <v>45559</v>
+        <v>45568</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="B7" s="6">
-        <v>45556</v>
+        <v>45569</v>
       </c>
       <c r="C7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="6">
+        <v>45568</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D8" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="6">
+        <v>45567</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="5" t="s">
+    <row r="10" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="6">
-        <v>45559</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="5" t="s">
+      <c r="B10" s="6">
+        <v>45567</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="6">
+        <v>45567</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="6">
+        <v>45567</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9" s="6">
-        <v>45555</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="5" t="s">
+    <row r="13" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" s="6">
+        <v>45567</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B10" s="6">
-        <v>45558</v>
-      </c>
-      <c r="C10" s="5" t="s">
+    <row r="14" spans="1:9" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="5"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+    </row>
+    <row r="15" spans="1:9" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:9" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="25"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="26"/>
+    </row>
+    <row r="17" spans="1:4" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" s="31"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="32"/>
+    </row>
+    <row r="18" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="33"/>
+      <c r="B18" s="34"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="35"/>
+    </row>
+    <row r="19" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="33"/>
+      <c r="B19" s="34"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="35"/>
+    </row>
+    <row r="20" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="36"/>
+      <c r="B20" s="37"/>
+      <c r="C20" s="37"/>
+      <c r="D20" s="38"/>
+    </row>
+    <row r="21" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="28"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="4">
+        <v>45566</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="5"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-    </row>
-    <row r="12" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="13" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" s="25"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="26"/>
-    </row>
-    <row r="14" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" s="31"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="32"/>
-    </row>
-    <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="33"/>
-      <c r="B15" s="34"/>
-      <c r="C15" s="34"/>
-      <c r="D15" s="35"/>
-    </row>
-    <row r="16" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="33"/>
-      <c r="B16" s="34"/>
-      <c r="C16" s="34"/>
-      <c r="D16" s="35"/>
-    </row>
-    <row r="17" spans="1:5" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="36"/>
-      <c r="B17" s="37"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="38"/>
-    </row>
-    <row r="18" spans="1:5" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="19" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" s="28"/>
-      <c r="C19" s="29"/>
-      <c r="D19" s="12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D20" s="4">
-        <v>45559</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C21" s="5"/>
-      <c r="D21" s="12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22" s="5"/>
-      <c r="D22" s="7">
-        <v>0.68333333333333335</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23" s="5"/>
-      <c r="D23" s="12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C24" s="5"/>
-      <c r="D24" s="8">
-        <v>0.69444444444444442</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D24" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C25" s="5"/>
-      <c r="D25" s="12" t="s">
+      <c r="D25" s="7">
+        <v>0.68333333333333335</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="5"/>
+      <c r="D26" s="12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" s="5"/>
+      <c r="D27" s="8">
+        <v>0.69305555555555554</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C28" s="5"/>
+      <c r="D28" s="12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="2" t="s">
+    <row r="29" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D26" s="3">
-        <f>IF(D24="","",D24-D22)</f>
-        <v>1.1111111111111072E-2</v>
-      </c>
-      <c r="E26" s="13"/>
+      <c r="B29" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" s="5"/>
+      <c r="D29" s="3">
+        <f>IF(D27="","",D27-D25)</f>
+        <v>9.7222222222221877E-3</v>
+      </c>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <mergeCells count="5">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A13:D13"/>
-    <mergeCell ref="A14:D17"/>
-    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="A17:D20"/>
+    <mergeCell ref="A22:C22"/>
   </mergeCells>
-  <conditionalFormatting sqref="B21:B26">
-    <cfRule type="cellIs" dxfId="30" priority="4" operator="equal">
+  <conditionalFormatting sqref="B24:B29">
+    <cfRule type="cellIs" dxfId="17" priority="4" operator="equal">
       <formula>"AUSENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="5" operator="equal">
       <formula>"PRESENTE"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D5:D10">
-    <cfRule type="cellIs" dxfId="28" priority="1" operator="equal">
+  <conditionalFormatting sqref="D5:D13">
+    <cfRule type="cellIs" dxfId="15" priority="1" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="2" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="3" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C11" xr:uid="{246F7448-B3F1-42C5-B8EC-A053A9779E64}">
-      <formula1>$A$21:$A$26</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C14" xr:uid="{2915FD14-172A-47B4-A85D-63A71A474370}">
+      <formula1>$A$24:$A$29</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -5514,17 +5560,17 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5D12E808-99D3-4425-8C97-AEE8CB7B788E}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F897371B-825E-46C1-AE8C-F5A30A71FAE7}">
           <x14:formula1>
             <xm:f>'BANCO DE DADOS'!$A$1:$A$2</xm:f>
           </x14:formula1>
-          <xm:sqref>B21:B26</xm:sqref>
+          <xm:sqref>B24:B29</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6AD0849D-1BF5-420D-8141-480ABFF26CDB}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DF141593-0456-44A9-8FC5-DB7C1738BC4E}">
           <x14:formula1>
             <xm:f>'BANCO DE DADOS'!$B$1:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>D5:D11</xm:sqref>
+          <xm:sqref>D5:D14</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -5540,17 +5586,17 @@
       <selection activeCell="A21" sqref="A21:A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.453125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.08984375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.453125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.453125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.08984375" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.90625" style="1"/>
+    <col min="1" max="1" width="34.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>24</v>
       </c>
@@ -5558,8 +5604,8 @@
       <c r="C1" s="25"/>
       <c r="D1" s="26"/>
     </row>
-    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="24" t="s">
         <v>2</v>
       </c>
@@ -5571,7 +5617,7 @@
       <c r="H3"/>
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -5589,7 +5635,7 @@
       <c r="H4"/>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>27</v>
       </c>
@@ -5603,7 +5649,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>28</v>
       </c>
@@ -5617,7 +5663,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>29</v>
       </c>
@@ -5631,7 +5677,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>30</v>
       </c>
@@ -5645,7 +5691,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>31</v>
       </c>
@@ -5659,7 +5705,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>33</v>
       </c>
@@ -5673,14 +5719,14 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="6"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
     </row>
-    <row r="12" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="13" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="24" t="s">
         <v>32</v>
       </c>
@@ -5688,34 +5734,34 @@
       <c r="C13" s="25"/>
       <c r="D13" s="26"/>
     </row>
-    <row r="14" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="30" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B14" s="31"/>
       <c r="C14" s="31"/>
       <c r="D14" s="32"/>
     </row>
-    <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="33"/>
       <c r="B15" s="34"/>
       <c r="C15" s="34"/>
       <c r="D15" s="35"/>
     </row>
-    <row r="16" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="33"/>
       <c r="B16" s="34"/>
       <c r="C16" s="34"/>
       <c r="D16" s="35"/>
     </row>
-    <row r="17" spans="1:5" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:5" ht="16.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="36"/>
       <c r="B17" s="37"/>
       <c r="C17" s="37"/>
       <c r="D17" s="38"/>
     </row>
-    <row r="18" spans="1:5" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="19" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:5" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="27" t="s">
         <v>19</v>
       </c>
@@ -5725,7 +5771,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
         <v>0</v>
       </c>
@@ -5739,7 +5785,7 @@
         <v>45560</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:5" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>8</v>
       </c>
@@ -5751,7 +5797,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:5" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>9</v>
       </c>
@@ -5763,7 +5809,7 @@
         <v>0.68194444444444446</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:5" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>10</v>
       </c>
@@ -5775,7 +5821,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:5" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>11</v>
       </c>
@@ -5787,7 +5833,7 @@
         <v>0.69444444444444442</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:5" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>12</v>
       </c>
@@ -5799,7 +5845,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:5" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>13</v>
       </c>
@@ -5884,23 +5930,23 @@
       <selection activeCell="I13" sqref="F13:I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.453125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.08984375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.453125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.453125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="6.453125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="34.453125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="31.08984375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="30.453125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="21.453125" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.90625" style="1"/>
+    <col min="1" max="1" width="34.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="6.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="34.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="31.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="30.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="21.42578125" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B1" s="25"/>
       <c r="C1" s="25"/>
@@ -5911,55 +5957,55 @@
       <c r="H1" s="25"/>
       <c r="I1" s="26"/>
     </row>
-    <row r="2" spans="1:9" customFormat="1" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="3" spans="1:9" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="24" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B3" s="25"/>
       <c r="C3" s="25"/>
       <c r="D3" s="26"/>
       <c r="F3" s="24" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G3" s="25"/>
       <c r="H3" s="25"/>
       <c r="I3" s="26"/>
     </row>
-    <row r="4" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="B4" s="41" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="41"/>
-      <c r="D4" s="42"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="51"/>
       <c r="F4" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="G4" s="41"/>
-      <c r="H4" s="41"/>
-      <c r="I4" s="42"/>
-    </row>
-    <row r="5" spans="1:9" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>37</v>
+      </c>
+      <c r="G4" s="50"/>
+      <c r="H4" s="50"/>
+      <c r="I4" s="51"/>
+    </row>
+    <row r="5" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="B5" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="43"/>
-      <c r="D5" s="44"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="53"/>
       <c r="F5" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="G5" s="43"/>
-      <c r="H5" s="43"/>
-      <c r="I5" s="44"/>
-    </row>
-    <row r="6" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="7" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+        <v>38</v>
+      </c>
+      <c r="G5" s="52"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="53"/>
+    </row>
+    <row r="6" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>3</v>
       </c>
@@ -5985,13 +6031,13 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="22"/>
       <c r="B8" s="6"/>
       <c r="C8" s="5"/>
       <c r="D8" s="23"/>
       <c r="F8" s="22" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G8" s="6">
         <v>45567</v>
@@ -6003,7 +6049,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="22"/>
       <c r="B9" s="6"/>
       <c r="C9" s="5"/>
@@ -6021,13 +6067,13 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="22"/>
       <c r="B10" s="6"/>
       <c r="C10" s="5"/>
       <c r="D10" s="23"/>
       <c r="F10" s="22" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G10" s="6">
         <v>45567</v>
@@ -6039,7 +6085,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="22"/>
       <c r="B11" s="6"/>
       <c r="C11" s="5"/>
@@ -6057,11 +6103,11 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="19"/>
       <c r="D12" s="18"/>
       <c r="F12" s="22" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G12" s="6">
         <v>45567</v>
@@ -6073,15 +6119,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="24" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B13" s="25"/>
       <c r="C13" s="25"/>
       <c r="D13" s="26"/>
       <c r="F13" s="22" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G13" s="6">
         <v>45567</v>
@@ -6093,13 +6139,13 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="30"/>
       <c r="B14" s="31"/>
       <c r="C14" s="31"/>
       <c r="D14" s="32"/>
       <c r="F14" s="22" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G14" s="6">
         <v>45567</v>
@@ -6111,13 +6157,13 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="33"/>
       <c r="B15" s="34"/>
       <c r="C15" s="34"/>
       <c r="D15" s="35"/>
       <c r="F15" s="22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G15" s="6">
         <v>45567</v>
@@ -6129,13 +6175,13 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="33"/>
       <c r="B16" s="34"/>
       <c r="C16" s="34"/>
       <c r="D16" s="35"/>
       <c r="F16" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G16" s="6">
         <v>45567</v>
@@ -6147,13 +6193,13 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="36"/>
       <c r="B17" s="37"/>
       <c r="C17" s="37"/>
       <c r="D17" s="38"/>
       <c r="F17" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G17" s="6">
         <v>45567</v>
@@ -6165,106 +6211,98 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="14"/>
       <c r="B18"/>
       <c r="C18"/>
       <c r="D18" s="15"/>
     </row>
-    <row r="19" spans="1:9" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="45" t="s">
+    <row r="19" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="46"/>
-      <c r="C19" s="46"/>
-      <c r="D19" s="47"/>
+      <c r="B19" s="55"/>
+      <c r="C19" s="55"/>
+      <c r="D19" s="56"/>
       <c r="F19"/>
       <c r="G19"/>
     </row>
-    <row r="20" spans="1:9" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="52" t="s">
+    <row r="20" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="53"/>
-      <c r="C20" s="48" t="s">
-        <v>48</v>
-      </c>
-      <c r="D20" s="49"/>
+      <c r="B20" s="62"/>
+      <c r="C20" s="57" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" s="58"/>
       <c r="E20" s="13"/>
       <c r="F20"/>
       <c r="G20"/>
     </row>
-    <row r="21" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="54" t="s">
+    <row r="21" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="50"/>
-      <c r="C21" s="50" t="s">
+      <c r="B21" s="59"/>
+      <c r="C21" s="59" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21" s="60"/>
+    </row>
+    <row r="22" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="64" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="48"/>
+      <c r="C22" s="48" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" s="49"/>
+    </row>
+    <row r="23" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="39" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="40"/>
+      <c r="C23" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="D21" s="51"/>
-    </row>
-    <row r="22" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="55" t="s">
-        <v>9</v>
-      </c>
-      <c r="B22" s="39"/>
-      <c r="C22" s="39" t="s">
+      <c r="D23" s="46"/>
+    </row>
+    <row r="24" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" s="42"/>
+      <c r="C24" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="D22" s="40"/>
-    </row>
-    <row r="23" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="56" t="s">
-        <v>10</v>
-      </c>
-      <c r="B23" s="57"/>
-      <c r="C23" s="57" t="s">
+      <c r="D24" s="47"/>
+    </row>
+    <row r="25" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="40"/>
+      <c r="C25" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="D23" s="63"/>
-    </row>
-    <row r="24" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="58" t="s">
-        <v>11</v>
-      </c>
-      <c r="B24" s="59"/>
-      <c r="C24" s="59" t="s">
+      <c r="D25" s="46"/>
+    </row>
+    <row r="26" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="44"/>
+      <c r="C26" s="44" t="s">
         <v>52</v>
       </c>
-      <c r="D24" s="64"/>
-    </row>
-    <row r="25" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="56" t="s">
-        <v>12</v>
-      </c>
-      <c r="B25" s="57"/>
-      <c r="C25" s="57" t="s">
-        <v>53</v>
-      </c>
-      <c r="D25" s="63"/>
-    </row>
-    <row r="26" spans="1:9" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="60" t="s">
-        <v>13</v>
-      </c>
-      <c r="B26" s="61"/>
-      <c r="C26" s="61" t="s">
-        <v>54</v>
-      </c>
-      <c r="D26" s="62"/>
+      <c r="D26" s="45"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <mergeCells count="24">
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="A25:B25"/>
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="A13:D13"/>
     <mergeCell ref="A14:D17"/>
@@ -6281,6 +6319,14 @@
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="A25:B25"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="D8:D11 I8:I17">

</xml_diff>

<commit_message>
Subindo a ATA Semanal que será enviada ao cliente e adição de Requisitos ao Backlog
</commit_message>
<xml_diff>
--- a/ATAs_de_Reuniao/Sprint 2/Semana 2609/Grupo4_ATA_Semana2609.xlsx
+++ b/ATAs_de_Reuniao/Sprint 2/Semana 2609/Grupo4_ATA_Semana2609.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpfer\OneDrive\Documentos\SPTECH\PI\SPRINT\Sprint-SPTECH\ATAs_de_Reuniao\Sprint 2\Semana 2609\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Documents\Projeto_PI\sprint2\ATAs_de_Reuniao\Sprint 2\Semana 2609\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2C07F55-631C-434C-9A68-B477C9254942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6F518FD-4945-4C35-9346-D14FF8571FDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="6" xr2:uid="{D70EAD62-B489-48DA-AED6-4403B2320B59}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="7" xr2:uid="{D70EAD62-B489-48DA-AED6-4403B2320B59}"/>
   </bookViews>
   <sheets>
     <sheet name="BANCO DE DADOS" sheetId="2" state="hidden" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="65">
   <si>
     <t>NOME</t>
   </si>
@@ -218,6 +218,27 @@
   <si>
     <t>Foi discutido sobre o prazo da entrega das atividades, falado sobre as tabelas e sua modelação no MySQL, atualização do Backlog e os próximos passos para o projeto.</t>
   </si>
+  <si>
+    <t>CALCULADORA</t>
+  </si>
+  <si>
+    <t>SITE ESTÁTICO (HTML+CSS)</t>
+  </si>
+  <si>
+    <t>VALIDAR SOLUÇÃO TÉCNICA</t>
+  </si>
+  <si>
+    <t>PLANILHA DE RISCO</t>
+  </si>
+  <si>
+    <t>ESPECIFICAÇÃO DA DASHBOARD</t>
+  </si>
+  <si>
+    <t>Percebemos que houve um maior entrosamento entre os integrantes do grupo e atingimos maior produtividade nas tarefas. Planejamos entregar todos os requisitos essenciais faltantes até a semana do dia 09/10.</t>
+  </si>
+  <si>
+    <t>PLANEJAMENTO SEMANA 03/10</t>
+  </si>
 </sst>
 </file>
 
@@ -744,7 +765,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -790,19 +811,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -818,6 +831,7 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -872,84 +886,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="8" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="8" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="8" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="8" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="8" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="8" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -986,12 +922,419 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="125">
+  <dxfs count="124">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1009,7 +1352,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -1029,12 +1372,12 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <font>
-        <b/>
+        <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -1049,7 +1392,29 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
@@ -1084,7 +1449,8 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1122,7 +1488,17 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -1142,7 +1518,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -1163,7 +1539,7 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -1183,7 +1559,17 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -1204,26 +1590,6 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -1243,336 +1609,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -1588,7 +1624,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -1608,12 +1644,12 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
+        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -1628,29 +1664,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
@@ -1685,8 +1699,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -3102,191 +3115,191 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}" name="Tabela1" displayName="Tabela1" ref="A4:D15" totalsRowShown="0" headerRowDxfId="124" dataDxfId="123" tableBorderDxfId="122">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}" name="Tabela1" displayName="Tabela1" ref="A4:D15" totalsRowShown="0" headerRowDxfId="123" dataDxfId="122" tableBorderDxfId="121">
   <autoFilter ref="A4:D15" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{304AA193-8246-42D6-B1C9-59B7CDC154B3}" name="O QUE FAZER" dataDxfId="121"/>
-    <tableColumn id="2" xr3:uid="{78AA6BC8-76A1-4FBB-8FD3-BCC5150E3A32}" name="PRAZOS DE ENTREGA" dataDxfId="120"/>
-    <tableColumn id="3" xr3:uid="{2F5C5138-DE27-4C39-AB08-9838AABC1D77}" name="RESPONSAVEL" dataDxfId="119"/>
-    <tableColumn id="4" xr3:uid="{D7517C3D-D3B1-4731-934F-9B5B368C5317}" name="SITUAÇÃO" dataDxfId="118"/>
+    <tableColumn id="1" xr3:uid="{304AA193-8246-42D6-B1C9-59B7CDC154B3}" name="O QUE FAZER" dataDxfId="120"/>
+    <tableColumn id="2" xr3:uid="{78AA6BC8-76A1-4FBB-8FD3-BCC5150E3A32}" name="PRAZOS DE ENTREGA" dataDxfId="119"/>
+    <tableColumn id="3" xr3:uid="{2F5C5138-DE27-4C39-AB08-9838AABC1D77}" name="RESPONSAVEL" dataDxfId="118"/>
+    <tableColumn id="4" xr3:uid="{D7517C3D-D3B1-4731-934F-9B5B368C5317}" name="SITUAÇÃO" dataDxfId="117"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{1191F4CB-7F6D-485B-AC60-0502347DD05B}" name="Tabela216579" displayName="Tabela216579" ref="A23:C29" totalsRowShown="0" headerRowDxfId="65" dataDxfId="64" tableBorderDxfId="63">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{1191F4CB-7F6D-485B-AC60-0502347DD05B}" name="Tabela216579" displayName="Tabela216579" ref="A23:C29" totalsRowShown="0" headerRowDxfId="64" dataDxfId="63" tableBorderDxfId="62">
   <autoFilter ref="A23:C29" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{8CE1CFB1-3B41-4ED3-8123-1F497AD0EBF4}" name="NOME" dataDxfId="62"/>
-    <tableColumn id="2" xr3:uid="{D65F61F3-2928-4DDE-B139-E3881CA88028}" name="PARTICIPAÇÃO" dataDxfId="61"/>
-    <tableColumn id="3" xr3:uid="{E75E5DBF-4EBF-4291-8B2C-1C27A0B29355}" name="JUSTIFICATIVA" dataDxfId="60"/>
+    <tableColumn id="1" xr3:uid="{8CE1CFB1-3B41-4ED3-8123-1F497AD0EBF4}" name="NOME" dataDxfId="61"/>
+    <tableColumn id="2" xr3:uid="{D65F61F3-2928-4DDE-B139-E3881CA88028}" name="PARTICIPAÇÃO" dataDxfId="60"/>
+    <tableColumn id="3" xr3:uid="{E75E5DBF-4EBF-4291-8B2C-1C27A0B29355}" name="JUSTIFICATIVA" dataDxfId="59"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{F391C4DF-42DB-4953-AF20-457CABC56FEC}" name="Tabela11546810" displayName="Tabela11546810" ref="A4:D14" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11" tableBorderDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{F391C4DF-42DB-4953-AF20-457CABC56FEC}" name="Tabela11546810" displayName="Tabela11546810" ref="A4:D14" totalsRowShown="0" headerRowDxfId="58" dataDxfId="57" tableBorderDxfId="56">
   <autoFilter ref="A4:D14" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:D14">
     <sortCondition ref="B5:B14"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{858C7998-D092-476C-BA38-00BFDD03CAC8}" name="O QUE FAZER" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{359F04F9-B255-453C-964F-60CE7A43531F}" name="PRAZOS DE ENTREGA" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{85B08382-C992-4A73-A20C-88A4AEFF9181}" name="RESPONSAVEL" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{00B398DB-E5DD-46C9-A85D-A0F1A41304EF}" name="SITUAÇÃO" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{858C7998-D092-476C-BA38-00BFDD03CAC8}" name="O QUE FAZER" dataDxfId="55"/>
+    <tableColumn id="2" xr3:uid="{359F04F9-B255-453C-964F-60CE7A43531F}" name="PRAZOS DE ENTREGA" dataDxfId="54"/>
+    <tableColumn id="3" xr3:uid="{85B08382-C992-4A73-A20C-88A4AEFF9181}" name="RESPONSAVEL" dataDxfId="53"/>
+    <tableColumn id="4" xr3:uid="{00B398DB-E5DD-46C9-A85D-A0F1A41304EF}" name="SITUAÇÃO" dataDxfId="52"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{857DC006-90BB-4A21-8363-6711FF969141}" name="Tabela21657911" displayName="Tabela21657911" ref="A23:C29" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4" tableBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{857DC006-90BB-4A21-8363-6711FF969141}" name="Tabela21657911" displayName="Tabela21657911" ref="A23:C29" totalsRowShown="0" headerRowDxfId="51" dataDxfId="50" tableBorderDxfId="49">
   <autoFilter ref="A23:C29" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{0EC888F5-FDA9-40C2-9479-76175354E904}" name="NOME" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{ECFC391D-EC26-474E-A50A-574A03222BAF}" name="PARTICIPAÇÃO" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{7BC4BFBF-9DCA-4173-BB6D-824380DCF690}" name="JUSTIFICATIVA" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{0EC888F5-FDA9-40C2-9479-76175354E904}" name="NOME" dataDxfId="48"/>
+    <tableColumn id="2" xr3:uid="{ECFC391D-EC26-474E-A50A-574A03222BAF}" name="PARTICIPAÇÃO" dataDxfId="47"/>
+    <tableColumn id="3" xr3:uid="{7BC4BFBF-9DCA-4173-BB6D-824380DCF690}" name="JUSTIFICATIVA" dataDxfId="46"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{5D051227-CD21-44B9-B384-BB058BE2415C}" name="Tabela1468101214" displayName="Tabela1468101214" ref="A7:D11" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58" tableBorderDxfId="57">
-  <autoFilter ref="A7:D11" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{5D051227-CD21-44B9-B384-BB058BE2415C}" name="Tabela1468101214" displayName="Tabela1468101214" ref="A7:D17" totalsRowShown="0" headerRowDxfId="45" tableBorderDxfId="44">
+  <autoFilter ref="A7:D17" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{60DF006F-DEC1-44B4-B650-77AA681BD053}" name="O QUE FAZER" dataDxfId="56"/>
-    <tableColumn id="2" xr3:uid="{B1C8A4D2-1A12-4627-B02D-C93638B8E22A}" name="PRAZOS DE ENTREGA" dataDxfId="55"/>
-    <tableColumn id="3" xr3:uid="{F9358C8C-A26D-4EC1-88FC-FC7F9E7F7126}" name="RESPONSAVEL" dataDxfId="54"/>
-    <tableColumn id="4" xr3:uid="{4EFF508D-FF9C-4340-8D19-B4DDBABBA711}" name="SITUAÇÃO" dataDxfId="53"/>
+    <tableColumn id="1" xr3:uid="{60DF006F-DEC1-44B4-B650-77AA681BD053}" name="O QUE FAZER" dataDxfId="43"/>
+    <tableColumn id="2" xr3:uid="{B1C8A4D2-1A12-4627-B02D-C93638B8E22A}" name="PRAZOS DE ENTREGA" dataDxfId="42"/>
+    <tableColumn id="3" xr3:uid="{F9358C8C-A26D-4EC1-88FC-FC7F9E7F7126}" name="RESPONSAVEL" dataDxfId="41"/>
+    <tableColumn id="4" xr3:uid="{4EFF508D-FF9C-4340-8D19-B4DDBABBA711}" name="SITUAÇÃO" dataDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{3230F418-B85A-4611-A179-37FFDCA32F80}" name="Tabela146810121418" displayName="Tabela146810121418" ref="F7:I17" totalsRowShown="0" headerRowDxfId="52" dataDxfId="51" tableBorderDxfId="50">
-  <autoFilter ref="F7:I17" xr:uid="{3230F418-B85A-4611-A179-37FFDCA32F80}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="F8:I17">
-    <sortCondition ref="H7:H17"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{3230F418-B85A-4611-A179-37FFDCA32F80}" name="Tabela146810121418" displayName="Tabela146810121418" ref="F7:I14" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38" tableBorderDxfId="37">
+  <autoFilter ref="F7:I14" xr:uid="{3230F418-B85A-4611-A179-37FFDCA32F80}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="F8:I10">
+    <sortCondition ref="H7:H10"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{8C9AFF73-6E6E-4E4C-A377-C37849BB14F7}" name="O QUE FAZER" dataDxfId="49"/>
-    <tableColumn id="2" xr3:uid="{591F032C-5225-4191-A54B-DEF3830ED570}" name="PRAZOS DE ENTREGA" dataDxfId="48"/>
-    <tableColumn id="3" xr3:uid="{E796F4BB-4BEF-4028-8B36-D1E4B9650852}" name="RESPONSAVEL" dataDxfId="47"/>
-    <tableColumn id="4" xr3:uid="{D6A8EF5F-93E1-4C3A-A560-545F459C0602}" name="SITUAÇÃO" dataDxfId="46"/>
+    <tableColumn id="1" xr3:uid="{8C9AFF73-6E6E-4E4C-A377-C37849BB14F7}" name="O QUE FAZER" dataDxfId="36"/>
+    <tableColumn id="2" xr3:uid="{591F032C-5225-4191-A54B-DEF3830ED570}" name="PRAZOS DE ENTREGA" dataDxfId="35"/>
+    <tableColumn id="3" xr3:uid="{E796F4BB-4BEF-4028-8B36-D1E4B9650852}" name="RESPONSAVEL" dataDxfId="34"/>
+    <tableColumn id="4" xr3:uid="{D6A8EF5F-93E1-4C3A-A560-545F459C0602}" name="SITUAÇÃO" dataDxfId="33"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}" name="Tabela2" displayName="Tabela2" ref="A24:C30" totalsRowShown="0" headerRowDxfId="117" dataDxfId="116" tableBorderDxfId="115">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}" name="Tabela2" displayName="Tabela2" ref="A24:C30" totalsRowShown="0" headerRowDxfId="116" dataDxfId="115" tableBorderDxfId="114">
   <autoFilter ref="A24:C30" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{EE178185-CFC7-4789-A834-552542FE9234}" name="NOME" dataDxfId="114"/>
-    <tableColumn id="2" xr3:uid="{441E3B93-F7D3-4DEA-9A31-B2AAF98FF93F}" name="PARTICIPAÇÃO" dataDxfId="113"/>
-    <tableColumn id="3" xr3:uid="{63718DE3-E919-4841-AE71-A3377F141C19}" name="JUSTIFICATIVA" dataDxfId="112"/>
+    <tableColumn id="1" xr3:uid="{EE178185-CFC7-4789-A834-552542FE9234}" name="NOME" dataDxfId="113"/>
+    <tableColumn id="2" xr3:uid="{441E3B93-F7D3-4DEA-9A31-B2AAF98FF93F}" name="PARTICIPAÇÃO" dataDxfId="112"/>
+    <tableColumn id="3" xr3:uid="{63718DE3-E919-4841-AE71-A3377F141C19}" name="JUSTIFICATIVA" dataDxfId="111"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{D0E7EA3C-BE91-4CD4-8D6B-11CF5253537E}" name="Tabela115" displayName="Tabela115" ref="A4:D15" totalsRowShown="0" headerRowDxfId="111" dataDxfId="110" tableBorderDxfId="109">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{D0E7EA3C-BE91-4CD4-8D6B-11CF5253537E}" name="Tabela115" displayName="Tabela115" ref="A4:D15" totalsRowShown="0" headerRowDxfId="110" dataDxfId="109" tableBorderDxfId="108">
   <autoFilter ref="A4:D15" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{B6DB7E5E-011A-48D2-A976-ECEFE111C94E}" name="O QUE FAZER" dataDxfId="108"/>
-    <tableColumn id="2" xr3:uid="{C8C44900-7A4B-42F1-AAB5-3F3D22C68477}" name="PRAZOS DE ENTREGA" dataDxfId="107"/>
-    <tableColumn id="3" xr3:uid="{7D5CA6FE-4AAD-477F-AF2F-FCF9BB79F2A4}" name="RESPONSAVEL" dataDxfId="106"/>
-    <tableColumn id="4" xr3:uid="{C66C4879-8B2E-4E01-B450-94C2F9ACD3E6}" name="SITUAÇÃO" dataDxfId="105"/>
+    <tableColumn id="1" xr3:uid="{B6DB7E5E-011A-48D2-A976-ECEFE111C94E}" name="O QUE FAZER" dataDxfId="107"/>
+    <tableColumn id="2" xr3:uid="{C8C44900-7A4B-42F1-AAB5-3F3D22C68477}" name="PRAZOS DE ENTREGA" dataDxfId="106"/>
+    <tableColumn id="3" xr3:uid="{7D5CA6FE-4AAD-477F-AF2F-FCF9BB79F2A4}" name="RESPONSAVEL" dataDxfId="105"/>
+    <tableColumn id="4" xr3:uid="{C66C4879-8B2E-4E01-B450-94C2F9ACD3E6}" name="SITUAÇÃO" dataDxfId="104"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{7450B737-251D-4080-BADD-F4A96802C130}" name="Tabela216" displayName="Tabela216" ref="A24:C30" totalsRowShown="0" headerRowDxfId="104" dataDxfId="103" tableBorderDxfId="102">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{7450B737-251D-4080-BADD-F4A96802C130}" name="Tabela216" displayName="Tabela216" ref="A24:C30" totalsRowShown="0" headerRowDxfId="103" dataDxfId="102" tableBorderDxfId="101">
   <autoFilter ref="A24:C30" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{4F27162E-8CFA-4DAC-B500-6AABDBBE620A}" name="NOME" dataDxfId="101"/>
-    <tableColumn id="2" xr3:uid="{37D7277D-4E73-48C0-9519-8AD7D8FE33D8}" name="PARTICIPAÇÃO" dataDxfId="100"/>
-    <tableColumn id="3" xr3:uid="{496DFA61-9424-423D-B0E5-A7735AFDCAF4}" name="JUSTIFICATIVA" dataDxfId="99"/>
+    <tableColumn id="1" xr3:uid="{4F27162E-8CFA-4DAC-B500-6AABDBBE620A}" name="NOME" dataDxfId="100"/>
+    <tableColumn id="2" xr3:uid="{37D7277D-4E73-48C0-9519-8AD7D8FE33D8}" name="PARTICIPAÇÃO" dataDxfId="99"/>
+    <tableColumn id="3" xr3:uid="{496DFA61-9424-423D-B0E5-A7735AFDCAF4}" name="JUSTIFICATIVA" dataDxfId="98"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A2693141-5581-47AE-AA42-42593B3EBCC5}" name="Tabela1154" displayName="Tabela1154" ref="A4:D14" totalsRowShown="0" headerRowDxfId="98" dataDxfId="97" tableBorderDxfId="96">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A2693141-5581-47AE-AA42-42593B3EBCC5}" name="Tabela1154" displayName="Tabela1154" ref="A4:D14" totalsRowShown="0" headerRowDxfId="97" dataDxfId="96" tableBorderDxfId="95">
   <autoFilter ref="A4:D14" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:D14">
     <sortCondition ref="B5:B14"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{9F852A18-D2ED-4627-9A9F-5F87E825A023}" name="O QUE FAZER" dataDxfId="95"/>
-    <tableColumn id="2" xr3:uid="{47171A49-03A0-4FA7-9867-33A0B4CA3732}" name="PRAZOS DE ENTREGA" dataDxfId="94"/>
-    <tableColumn id="3" xr3:uid="{D64896FF-DF85-432A-AF0B-6A09292E6318}" name="RESPONSAVEL" dataDxfId="93"/>
-    <tableColumn id="4" xr3:uid="{3524D571-73DA-4A58-9780-D5CE262B5B8B}" name="SITUAÇÃO" dataDxfId="92"/>
+    <tableColumn id="1" xr3:uid="{9F852A18-D2ED-4627-9A9F-5F87E825A023}" name="O QUE FAZER" dataDxfId="94"/>
+    <tableColumn id="2" xr3:uid="{47171A49-03A0-4FA7-9867-33A0B4CA3732}" name="PRAZOS DE ENTREGA" dataDxfId="93"/>
+    <tableColumn id="3" xr3:uid="{D64896FF-DF85-432A-AF0B-6A09292E6318}" name="RESPONSAVEL" dataDxfId="92"/>
+    <tableColumn id="4" xr3:uid="{3524D571-73DA-4A58-9780-D5CE262B5B8B}" name="SITUAÇÃO" dataDxfId="91"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{CA79F966-3FFA-418D-B80E-FC555E57811D}" name="Tabela2165" displayName="Tabela2165" ref="A23:C29" totalsRowShown="0" headerRowDxfId="91" dataDxfId="90" tableBorderDxfId="89">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{CA79F966-3FFA-418D-B80E-FC555E57811D}" name="Tabela2165" displayName="Tabela2165" ref="A23:C29" totalsRowShown="0" headerRowDxfId="90" dataDxfId="89" tableBorderDxfId="88">
   <autoFilter ref="A23:C29" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{6971728D-486F-404A-9A71-16C4D8DC9AA4}" name="NOME" dataDxfId="88"/>
-    <tableColumn id="2" xr3:uid="{C9BB7BC6-2734-4029-ACCA-3F1D8B884C14}" name="PARTICIPAÇÃO" dataDxfId="87"/>
-    <tableColumn id="3" xr3:uid="{D1D8705A-36D0-46DD-926C-E78547A7E649}" name="JUSTIFICATIVA" dataDxfId="86"/>
+    <tableColumn id="1" xr3:uid="{6971728D-486F-404A-9A71-16C4D8DC9AA4}" name="NOME" dataDxfId="87"/>
+    <tableColumn id="2" xr3:uid="{C9BB7BC6-2734-4029-ACCA-3F1D8B884C14}" name="PARTICIPAÇÃO" dataDxfId="86"/>
+    <tableColumn id="3" xr3:uid="{D1D8705A-36D0-46DD-926C-E78547A7E649}" name="JUSTIFICATIVA" dataDxfId="85"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{6C031CDA-53E0-45FD-9AE0-557E1E0765C8}" name="Tabela11546" displayName="Tabela11546" ref="A4:D14" totalsRowShown="0" headerRowDxfId="85" dataDxfId="84" tableBorderDxfId="83">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{6C031CDA-53E0-45FD-9AE0-557E1E0765C8}" name="Tabela11546" displayName="Tabela11546" ref="A4:D14" totalsRowShown="0" headerRowDxfId="84" dataDxfId="83" tableBorderDxfId="82">
   <autoFilter ref="A4:D14" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:D14">
     <sortCondition ref="B5:B14"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{BB742C24-B969-47D8-BDF5-2D9DD9DE0453}" name="O QUE FAZER" dataDxfId="82"/>
-    <tableColumn id="2" xr3:uid="{08450859-D0AC-4147-80B0-0A2BE06A68E3}" name="PRAZOS DE ENTREGA" dataDxfId="81"/>
-    <tableColumn id="3" xr3:uid="{90CA058E-F8FF-4FF1-BD90-FA898BB69129}" name="RESPONSAVEL" dataDxfId="80"/>
-    <tableColumn id="4" xr3:uid="{4533BAE4-7102-4B9B-8C5E-D2327FE6E37B}" name="SITUAÇÃO" dataDxfId="79"/>
+    <tableColumn id="1" xr3:uid="{BB742C24-B969-47D8-BDF5-2D9DD9DE0453}" name="O QUE FAZER" dataDxfId="81"/>
+    <tableColumn id="2" xr3:uid="{08450859-D0AC-4147-80B0-0A2BE06A68E3}" name="PRAZOS DE ENTREGA" dataDxfId="80"/>
+    <tableColumn id="3" xr3:uid="{90CA058E-F8FF-4FF1-BD90-FA898BB69129}" name="RESPONSAVEL" dataDxfId="79"/>
+    <tableColumn id="4" xr3:uid="{4533BAE4-7102-4B9B-8C5E-D2327FE6E37B}" name="SITUAÇÃO" dataDxfId="78"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{34D2C419-0C8F-420E-9F09-51777412EA0C}" name="Tabela21657" displayName="Tabela21657" ref="A23:C29" totalsRowShown="0" headerRowDxfId="78" dataDxfId="77" tableBorderDxfId="76">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{34D2C419-0C8F-420E-9F09-51777412EA0C}" name="Tabela21657" displayName="Tabela21657" ref="A23:C29" totalsRowShown="0" headerRowDxfId="77" dataDxfId="76" tableBorderDxfId="75">
   <autoFilter ref="A23:C29" xr:uid="{0DE2F4A7-28E2-496F-A24F-1236B78FA213}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{E570557C-2EE0-4811-A62D-094AB9B0C9BC}" name="NOME" dataDxfId="75"/>
-    <tableColumn id="2" xr3:uid="{89F08E2F-F9ED-4424-B655-EEE89E3DA5A7}" name="PARTICIPAÇÃO" dataDxfId="74"/>
-    <tableColumn id="3" xr3:uid="{DE6C6C5E-3892-42A9-B8A6-EDE8DE750751}" name="JUSTIFICATIVA" dataDxfId="73"/>
+    <tableColumn id="1" xr3:uid="{E570557C-2EE0-4811-A62D-094AB9B0C9BC}" name="NOME" dataDxfId="74"/>
+    <tableColumn id="2" xr3:uid="{89F08E2F-F9ED-4424-B655-EEE89E3DA5A7}" name="PARTICIPAÇÃO" dataDxfId="73"/>
+    <tableColumn id="3" xr3:uid="{DE6C6C5E-3892-42A9-B8A6-EDE8DE750751}" name="JUSTIFICATIVA" dataDxfId="72"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{433F7683-AF81-4BA7-9443-5B185A6FB802}" name="Tabela115468" displayName="Tabela115468" ref="A4:D14" totalsRowShown="0" headerRowDxfId="72" dataDxfId="71" tableBorderDxfId="70">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{433F7683-AF81-4BA7-9443-5B185A6FB802}" name="Tabela115468" displayName="Tabela115468" ref="A4:D14" totalsRowShown="0" headerRowDxfId="71" dataDxfId="70" tableBorderDxfId="69">
   <autoFilter ref="A4:D14" xr:uid="{2A6FFF7A-C2A8-4229-AD8A-85BF792BC551}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:D14">
     <sortCondition ref="B5:B14"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{9478A723-D368-432D-B04D-0CE3A8B04818}" name="O QUE FAZER" dataDxfId="69"/>
-    <tableColumn id="2" xr3:uid="{299E99A9-2BDD-4259-B821-126259D6061E}" name="PRAZOS DE ENTREGA" dataDxfId="68"/>
-    <tableColumn id="3" xr3:uid="{885DF8C6-2582-4A91-9775-AD5DDBFE5E62}" name="RESPONSAVEL" dataDxfId="67"/>
-    <tableColumn id="4" xr3:uid="{653F985A-2FB8-486B-BC74-444331BCE755}" name="SITUAÇÃO" dataDxfId="66"/>
+    <tableColumn id="1" xr3:uid="{9478A723-D368-432D-B04D-0CE3A8B04818}" name="O QUE FAZER" dataDxfId="68"/>
+    <tableColumn id="2" xr3:uid="{299E99A9-2BDD-4259-B821-126259D6061E}" name="PRAZOS DE ENTREGA" dataDxfId="67"/>
+    <tableColumn id="3" xr3:uid="{885DF8C6-2582-4A91-9775-AD5DDBFE5E62}" name="RESPONSAVEL" dataDxfId="66"/>
+    <tableColumn id="4" xr3:uid="{653F985A-2FB8-486B-BC74-444331BCE755}" name="SITUAÇÃO" dataDxfId="65"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3615,12 +3628,12 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -3631,7 +3644,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -3642,7 +3655,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>18</v>
       </c>
@@ -3656,42 +3669,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{440FA3E8-7F0D-4287-A3E8-76B61D68049B}">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A20" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.109375" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="34.453125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.08984375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.453125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.453125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.08984375" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:9" ht="39.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="26"/>
-    </row>
-    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="24" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="23"/>
+    </row>
+    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="26"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="23"/>
       <c r="F3"/>
       <c r="G3"/>
       <c r="H3"/>
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -3709,7 +3722,7 @@
       <c r="H4"/>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>48</v>
       </c>
@@ -3727,7 +3740,7 @@
       <c r="H5"/>
       <c r="I5"/>
     </row>
-    <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>28</v>
       </c>
@@ -3741,7 +3754,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>37</v>
       </c>
@@ -3755,7 +3768,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>27</v>
       </c>
@@ -3769,7 +3782,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>36</v>
       </c>
@@ -3783,7 +3796,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>27</v>
       </c>
@@ -3797,7 +3810,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>34</v>
       </c>
@@ -3811,7 +3824,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>50</v>
       </c>
@@ -3825,7 +3838,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>38</v>
       </c>
@@ -3839,7 +3852,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>51</v>
       </c>
@@ -3853,59 +3866,59 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="5"/>
       <c r="B15" s="6"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
     </row>
-    <row r="16" spans="1:9" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="17" spans="1:4" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="24" t="s">
+    <row r="16" spans="1:9" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="17" spans="1:4" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="25"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="26"/>
-    </row>
-    <row r="18" spans="1:4" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="30" t="s">
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="23"/>
+    </row>
+    <row r="18" spans="1:4" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="B18" s="31"/>
-      <c r="C18" s="31"/>
-      <c r="D18" s="32"/>
-    </row>
-    <row r="19" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="33"/>
-      <c r="B19" s="34"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="35"/>
-    </row>
-    <row r="20" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="33"/>
-      <c r="B20" s="34"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="35"/>
-    </row>
-    <row r="21" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="36"/>
-      <c r="B21" s="37"/>
-      <c r="C21" s="37"/>
-      <c r="D21" s="38"/>
-    </row>
-    <row r="22" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="23" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="27" t="s">
+      <c r="B18" s="28"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="29"/>
+    </row>
+    <row r="19" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="30"/>
+      <c r="B19" s="31"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="32"/>
+    </row>
+    <row r="20" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="30"/>
+      <c r="B20" s="31"/>
+      <c r="C20" s="31"/>
+      <c r="D20" s="32"/>
+    </row>
+    <row r="21" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="33"/>
+      <c r="B21" s="34"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="35"/>
+    </row>
+    <row r="22" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="23" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="B23" s="28"/>
-      <c r="C23" s="29"/>
+      <c r="B23" s="25"/>
+      <c r="C23" s="26"/>
       <c r="D23" s="12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="10" t="s">
         <v>0</v>
       </c>
@@ -3919,7 +3932,7 @@
         <v>45561</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="2" t="s">
         <v>8</v>
       </c>
@@ -3931,7 +3944,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="2" t="s">
         <v>9</v>
       </c>
@@ -3943,7 +3956,7 @@
         <v>0.68819444444444444</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="2" t="s">
         <v>10</v>
       </c>
@@ -3955,7 +3968,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="2" t="s">
         <v>11</v>
       </c>
@@ -3967,7 +3980,7 @@
         <v>0.69930555555555551</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="2" t="s">
         <v>12</v>
       </c>
@@ -3979,7 +3992,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="2" t="s">
         <v>13</v>
       </c>
@@ -4006,21 +4019,21 @@
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="B25:B30">
-    <cfRule type="cellIs" dxfId="45" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="4" operator="equal">
       <formula>"AUSENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="5" operator="equal">
       <formula>"PRESENTE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D14">
-    <cfRule type="cellIs" dxfId="43" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="1" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="2" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="3" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4064,38 +4077,38 @@
       <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.109375" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="34.453125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.08984375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.453125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.453125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.08984375" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:9" ht="39.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="26"/>
-    </row>
-    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="24" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="23"/>
+    </row>
+    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="26"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="23"/>
       <c r="F3"/>
       <c r="G3"/>
       <c r="H3"/>
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -4113,7 +4126,7 @@
       <c r="H4"/>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>48</v>
       </c>
@@ -4131,7 +4144,7 @@
       <c r="H5"/>
       <c r="I5"/>
     </row>
-    <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>28</v>
       </c>
@@ -4145,7 +4158,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>37</v>
       </c>
@@ -4159,7 +4172,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>27</v>
       </c>
@@ -4173,7 +4186,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>36</v>
       </c>
@@ -4187,7 +4200,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>27</v>
       </c>
@@ -4201,7 +4214,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>34</v>
       </c>
@@ -4215,7 +4228,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>49</v>
       </c>
@@ -4229,7 +4242,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>38</v>
       </c>
@@ -4243,7 +4256,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>51</v>
       </c>
@@ -4257,59 +4270,59 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="5"/>
       <c r="B15" s="6"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
     </row>
-    <row r="16" spans="1:9" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="17" spans="1:4" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="24" t="s">
+    <row r="16" spans="1:9" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="17" spans="1:4" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="25"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="26"/>
-    </row>
-    <row r="18" spans="1:4" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="30" t="s">
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="23"/>
+    </row>
+    <row r="18" spans="1:4" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="B18" s="31"/>
-      <c r="C18" s="31"/>
-      <c r="D18" s="32"/>
-    </row>
-    <row r="19" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="33"/>
-      <c r="B19" s="34"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="35"/>
-    </row>
-    <row r="20" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="33"/>
-      <c r="B20" s="34"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="35"/>
-    </row>
-    <row r="21" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="36"/>
-      <c r="B21" s="37"/>
-      <c r="C21" s="37"/>
-      <c r="D21" s="38"/>
-    </row>
-    <row r="22" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="23" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="27" t="s">
+      <c r="B18" s="28"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="29"/>
+    </row>
+    <row r="19" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="30"/>
+      <c r="B19" s="31"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="32"/>
+    </row>
+    <row r="20" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="30"/>
+      <c r="B20" s="31"/>
+      <c r="C20" s="31"/>
+      <c r="D20" s="32"/>
+    </row>
+    <row r="21" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="33"/>
+      <c r="B21" s="34"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="35"/>
+    </row>
+    <row r="22" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="23" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="B23" s="28"/>
-      <c r="C23" s="29"/>
+      <c r="B23" s="25"/>
+      <c r="C23" s="26"/>
       <c r="D23" s="12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="10" t="s">
         <v>0</v>
       </c>
@@ -4323,7 +4336,7 @@
         <v>45562</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="2" t="s">
         <v>8</v>
       </c>
@@ -4335,7 +4348,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="2" t="s">
         <v>9</v>
       </c>
@@ -4347,7 +4360,7 @@
         <v>0.68541666666666667</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="2" t="s">
         <v>10</v>
       </c>
@@ -4359,7 +4372,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="2" t="s">
         <v>11</v>
       </c>
@@ -4371,7 +4384,7 @@
         <v>0.69930555555555551</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="2" t="s">
         <v>12</v>
       </c>
@@ -4383,7 +4396,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="2" t="s">
         <v>13</v>
       </c>
@@ -4406,21 +4419,21 @@
     <mergeCell ref="A23:C23"/>
   </mergeCells>
   <conditionalFormatting sqref="B25:B30">
-    <cfRule type="cellIs" dxfId="40" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="4" operator="equal">
       <formula>"AUSENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="5" operator="equal">
       <formula>"PRESENTE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D14">
-    <cfRule type="cellIs" dxfId="38" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="1" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="2" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="3" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4464,38 +4477,38 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.109375" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="34.453125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.08984375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.453125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.453125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.08984375" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:9" ht="39.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="26"/>
-    </row>
-    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="24" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="23"/>
+    </row>
+    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="26"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="23"/>
       <c r="F3"/>
       <c r="G3"/>
       <c r="H3"/>
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -4513,7 +4526,7 @@
       <c r="H4"/>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>37</v>
       </c>
@@ -4531,7 +4544,7 @@
       <c r="H5"/>
       <c r="I5"/>
     </row>
-    <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>34</v>
       </c>
@@ -4545,7 +4558,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>49</v>
       </c>
@@ -4559,7 +4572,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>38</v>
       </c>
@@ -4573,7 +4586,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>48</v>
       </c>
@@ -4587,7 +4600,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>28</v>
       </c>
@@ -4601,7 +4614,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>27</v>
       </c>
@@ -4615,7 +4628,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>36</v>
       </c>
@@ -4629,7 +4642,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>51</v>
       </c>
@@ -4643,59 +4656,59 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="5"/>
       <c r="B14" s="6"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
     </row>
-    <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="16" spans="1:9" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="24" t="s">
+    <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="16" spans="1:9" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="25"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="26"/>
-    </row>
-    <row r="17" spans="1:4" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="30" t="s">
+      <c r="B16" s="22"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="23"/>
+    </row>
+    <row r="17" spans="1:4" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="B17" s="31"/>
-      <c r="C17" s="31"/>
-      <c r="D17" s="32"/>
-    </row>
-    <row r="18" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="33"/>
-      <c r="B18" s="34"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="35"/>
-    </row>
-    <row r="19" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="33"/>
-      <c r="B19" s="34"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="35"/>
-    </row>
-    <row r="20" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="36"/>
-      <c r="B20" s="37"/>
-      <c r="C20" s="37"/>
-      <c r="D20" s="38"/>
-    </row>
-    <row r="21" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="22" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="27" t="s">
+      <c r="B17" s="28"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="29"/>
+    </row>
+    <row r="18" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="30"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="32"/>
+    </row>
+    <row r="19" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="30"/>
+      <c r="B19" s="31"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="32"/>
+    </row>
+    <row r="20" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="33"/>
+      <c r="B20" s="34"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="35"/>
+    </row>
+    <row r="21" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="22" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="28"/>
-      <c r="C22" s="29"/>
+      <c r="B22" s="25"/>
+      <c r="C22" s="26"/>
       <c r="D22" s="12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="10" t="s">
         <v>0</v>
       </c>
@@ -4709,7 +4722,7 @@
         <v>45563</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="2" t="s">
         <v>8</v>
       </c>
@@ -4721,7 +4734,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="2" t="s">
         <v>9</v>
       </c>
@@ -4733,7 +4746,7 @@
         <v>0.41875000000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="2" t="s">
         <v>10</v>
       </c>
@@ -4745,7 +4758,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="2" t="s">
         <v>11</v>
       </c>
@@ -4757,7 +4770,7 @@
         <v>0.4284722222222222</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="2" t="s">
         <v>12</v>
       </c>
@@ -4769,7 +4782,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="2" t="s">
         <v>13</v>
       </c>
@@ -4792,21 +4805,21 @@
     <mergeCell ref="A22:C22"/>
   </mergeCells>
   <conditionalFormatting sqref="B24:B29">
-    <cfRule type="cellIs" dxfId="35" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="4" operator="equal">
       <formula>"AUSENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="5" operator="equal">
       <formula>"PRESENTE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D13">
-    <cfRule type="cellIs" dxfId="33" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="1" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="2" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="3" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4846,42 +4859,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19BF0B73-CACA-492F-8733-CCF61DB202E2}">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B5" sqref="B5:B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.109375" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="34.453125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.08984375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.453125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.453125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.08984375" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:9" ht="39.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="26"/>
-    </row>
-    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="24" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="23"/>
+    </row>
+    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="26"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="23"/>
       <c r="F3"/>
       <c r="G3"/>
       <c r="H3"/>
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -4899,7 +4912,7 @@
       <c r="H4"/>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>37</v>
       </c>
@@ -4917,7 +4930,7 @@
       <c r="H5"/>
       <c r="I5"/>
     </row>
-    <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>34</v>
       </c>
@@ -4931,7 +4944,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>49</v>
       </c>
@@ -4945,7 +4958,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>38</v>
       </c>
@@ -4959,7 +4972,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>48</v>
       </c>
@@ -4973,7 +4986,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>28</v>
       </c>
@@ -4987,7 +5000,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>27</v>
       </c>
@@ -5001,7 +5014,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>36</v>
       </c>
@@ -5015,7 +5028,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>51</v>
       </c>
@@ -5029,59 +5042,59 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="5"/>
       <c r="B14" s="6"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
     </row>
-    <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="16" spans="1:9" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="24" t="s">
+    <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="16" spans="1:9" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="25"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="26"/>
-    </row>
-    <row r="17" spans="1:4" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="30" t="s">
+      <c r="B16" s="22"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="23"/>
+    </row>
+    <row r="17" spans="1:4" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="B17" s="31"/>
-      <c r="C17" s="31"/>
-      <c r="D17" s="32"/>
-    </row>
-    <row r="18" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="33"/>
-      <c r="B18" s="34"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="35"/>
-    </row>
-    <row r="19" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="33"/>
-      <c r="B19" s="34"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="35"/>
-    </row>
-    <row r="20" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="36"/>
-      <c r="B20" s="37"/>
-      <c r="C20" s="37"/>
-      <c r="D20" s="38"/>
-    </row>
-    <row r="21" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="22" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="27" t="s">
+      <c r="B17" s="28"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="29"/>
+    </row>
+    <row r="18" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="30"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="32"/>
+    </row>
+    <row r="19" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="30"/>
+      <c r="B19" s="31"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="32"/>
+    </row>
+    <row r="20" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="33"/>
+      <c r="B20" s="34"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="35"/>
+    </row>
+    <row r="21" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="22" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="28"/>
-      <c r="C22" s="29"/>
+      <c r="B22" s="25"/>
+      <c r="C22" s="26"/>
       <c r="D22" s="12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="10" t="s">
         <v>0</v>
       </c>
@@ -5095,7 +5108,7 @@
         <v>45565</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="2" t="s">
         <v>8</v>
       </c>
@@ -5107,7 +5120,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="2" t="s">
         <v>9</v>
       </c>
@@ -5119,7 +5132,7 @@
         <v>0.68055555555555558</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="2" t="s">
         <v>10</v>
       </c>
@@ -5131,7 +5144,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="2" t="s">
         <v>11</v>
       </c>
@@ -5143,7 +5156,7 @@
         <v>0.69513888888888886</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="2" t="s">
         <v>12</v>
       </c>
@@ -5155,7 +5168,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="2" t="s">
         <v>13</v>
       </c>
@@ -5178,21 +5191,21 @@
     <mergeCell ref="A22:C22"/>
   </mergeCells>
   <conditionalFormatting sqref="B24:B29">
-    <cfRule type="cellIs" dxfId="30" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="4" operator="equal">
       <formula>"AUSENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="5" operator="equal">
       <formula>"PRESENTE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D13">
-    <cfRule type="cellIs" dxfId="28" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="1" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="2" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="3" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5236,38 +5249,38 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.109375" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="34.453125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.08984375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.453125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.453125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.08984375" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:9" ht="39.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="26"/>
-    </row>
-    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="24" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="23"/>
+    </row>
+    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="26"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="23"/>
       <c r="F3"/>
       <c r="G3"/>
       <c r="H3"/>
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -5285,7 +5298,7 @@
       <c r="H4"/>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>37</v>
       </c>
@@ -5303,7 +5316,7 @@
       <c r="H5"/>
       <c r="I5"/>
     </row>
-    <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>34</v>
       </c>
@@ -5317,7 +5330,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>49</v>
       </c>
@@ -5331,7 +5344,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>38</v>
       </c>
@@ -5345,7 +5358,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>48</v>
       </c>
@@ -5359,7 +5372,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>28</v>
       </c>
@@ -5373,7 +5386,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>27</v>
       </c>
@@ -5387,7 +5400,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>36</v>
       </c>
@@ -5401,7 +5414,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>51</v>
       </c>
@@ -5415,59 +5428,59 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="5"/>
       <c r="B14" s="6"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
     </row>
-    <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="16" spans="1:9" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="24" t="s">
+    <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="16" spans="1:9" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="25"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="26"/>
-    </row>
-    <row r="17" spans="1:4" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="30" t="s">
+      <c r="B16" s="22"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="23"/>
+    </row>
+    <row r="17" spans="1:4" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="B17" s="31"/>
-      <c r="C17" s="31"/>
-      <c r="D17" s="32"/>
-    </row>
-    <row r="18" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="33"/>
-      <c r="B18" s="34"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="35"/>
-    </row>
-    <row r="19" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="33"/>
-      <c r="B19" s="34"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="35"/>
-    </row>
-    <row r="20" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="36"/>
-      <c r="B20" s="37"/>
-      <c r="C20" s="37"/>
-      <c r="D20" s="38"/>
-    </row>
-    <row r="21" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="22" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="27" t="s">
+      <c r="B17" s="28"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="29"/>
+    </row>
+    <row r="18" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="30"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="32"/>
+    </row>
+    <row r="19" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="30"/>
+      <c r="B19" s="31"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="32"/>
+    </row>
+    <row r="20" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="33"/>
+      <c r="B20" s="34"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="35"/>
+    </row>
+    <row r="21" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="22" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="28"/>
-      <c r="C22" s="29"/>
+      <c r="B22" s="25"/>
+      <c r="C22" s="26"/>
       <c r="D22" s="12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="10" t="s">
         <v>0</v>
       </c>
@@ -5481,7 +5494,7 @@
         <v>45566</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="2" t="s">
         <v>8</v>
       </c>
@@ -5493,7 +5506,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="2" t="s">
         <v>9</v>
       </c>
@@ -5505,7 +5518,7 @@
         <v>0.68333333333333335</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="2" t="s">
         <v>10</v>
       </c>
@@ -5517,7 +5530,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="2" t="s">
         <v>11</v>
       </c>
@@ -5529,7 +5542,7 @@
         <v>0.69305555555555554</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="2" t="s">
         <v>12</v>
       </c>
@@ -5541,7 +5554,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="2" t="s">
         <v>13</v>
       </c>
@@ -5564,21 +5577,21 @@
     <mergeCell ref="A22:C22"/>
   </mergeCells>
   <conditionalFormatting sqref="B24:B29">
-    <cfRule type="cellIs" dxfId="25" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="4" operator="equal">
       <formula>"AUSENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
       <formula>"PRESENTE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D13">
-    <cfRule type="cellIs" dxfId="23" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5618,42 +5631,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEA814AF-35E5-4596-923E-E8BF36EBF589}">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.109375" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="34.453125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.08984375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.453125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.453125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.08984375" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:9" ht="39.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="26"/>
-    </row>
-    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="24" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="23"/>
+    </row>
+    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="26"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="23"/>
       <c r="F3"/>
       <c r="G3"/>
       <c r="H3"/>
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -5671,7 +5684,7 @@
       <c r="H4"/>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>37</v>
       </c>
@@ -5686,10 +5699,10 @@
       </c>
       <c r="F5"/>
       <c r="G5"/>
-      <c r="H5" s="74"/>
+      <c r="H5" s="20"/>
       <c r="I5"/>
     </row>
-    <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>34</v>
       </c>
@@ -5703,7 +5716,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>49</v>
       </c>
@@ -5717,7 +5730,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>38</v>
       </c>
@@ -5731,7 +5744,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>48</v>
       </c>
@@ -5745,7 +5758,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>28</v>
       </c>
@@ -5759,7 +5772,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>27</v>
       </c>
@@ -5773,7 +5786,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>36</v>
       </c>
@@ -5787,7 +5800,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>51</v>
       </c>
@@ -5801,59 +5814,59 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="5"/>
       <c r="B14" s="6"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
     </row>
-    <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="16" spans="1:9" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="24" t="s">
+    <row r="15" spans="1:9" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="16" spans="1:9" ht="16.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="25"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="26"/>
-    </row>
-    <row r="17" spans="1:4" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="65" t="s">
+      <c r="B16" s="22"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="23"/>
+    </row>
+    <row r="17" spans="1:4" ht="16.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="B17" s="66"/>
-      <c r="C17" s="66"/>
-      <c r="D17" s="67"/>
-    </row>
-    <row r="18" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="68"/>
-      <c r="B18" s="69"/>
-      <c r="C18" s="69"/>
-      <c r="D18" s="70"/>
-    </row>
-    <row r="19" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="68"/>
-      <c r="B19" s="69"/>
-      <c r="C19" s="69"/>
-      <c r="D19" s="70"/>
-    </row>
-    <row r="20" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="71"/>
-      <c r="B20" s="72"/>
-      <c r="C20" s="72"/>
-      <c r="D20" s="73"/>
-    </row>
-    <row r="21" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="22" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="27" t="s">
+      <c r="B17" s="37"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="38"/>
+    </row>
+    <row r="18" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="39"/>
+      <c r="B18" s="40"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="41"/>
+    </row>
+    <row r="19" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="39"/>
+      <c r="B19" s="40"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="41"/>
+    </row>
+    <row r="20" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="42"/>
+      <c r="B20" s="43"/>
+      <c r="C20" s="43"/>
+      <c r="D20" s="44"/>
+    </row>
+    <row r="21" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="22" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="28"/>
-      <c r="C22" s="29"/>
+      <c r="B22" s="25"/>
+      <c r="C22" s="26"/>
       <c r="D22" s="12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="10" t="s">
         <v>0</v>
       </c>
@@ -5867,7 +5880,7 @@
         <v>45567</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="2" t="s">
         <v>8</v>
       </c>
@@ -5879,7 +5892,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="2" t="s">
         <v>9</v>
       </c>
@@ -5891,7 +5904,7 @@
         <v>0.68194444444444446</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="2" t="s">
         <v>10</v>
       </c>
@@ -5903,7 +5916,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="2" t="s">
         <v>11</v>
       </c>
@@ -5915,7 +5928,7 @@
         <v>0.6958333333333333</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="2" t="s">
         <v>12</v>
       </c>
@@ -5927,7 +5940,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="2" t="s">
         <v>13</v>
       </c>
@@ -5950,21 +5963,21 @@
     <mergeCell ref="A22:C22"/>
   </mergeCells>
   <conditionalFormatting sqref="B24:B29">
-    <cfRule type="cellIs" dxfId="17" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
       <formula>"AUSENTE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
       <formula>"PRESENTE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D13">
-    <cfRule type="cellIs" dxfId="15" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6005,89 +6018,93 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I13" sqref="F13:I13"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="6.44140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="34.44140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="31.109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="30.44140625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="21.44140625" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="34.453125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.08984375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.453125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.453125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="6.453125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="37" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.08984375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="30.453125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="21.453125" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:9" ht="39.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="26"/>
-    </row>
-    <row r="2" spans="1:9" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="24" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="23"/>
+    </row>
+    <row r="2" spans="1:9" customFormat="1" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="1:9" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="26"/>
-      <c r="F3" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="26"/>
-    </row>
-    <row r="4" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="16" t="s">
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="23"/>
+      <c r="F3" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="23"/>
+    </row>
+    <row r="4" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="41"/>
-      <c r="D4" s="42"/>
-      <c r="F4" s="16" t="s">
+      <c r="C4" s="47"/>
+      <c r="D4" s="48"/>
+      <c r="F4" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="G4" s="41"/>
-      <c r="H4" s="41"/>
-      <c r="I4" s="42"/>
-    </row>
-    <row r="5" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="17" t="s">
+      <c r="G4" s="47" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="47"/>
+      <c r="I4" s="48"/>
+    </row>
+    <row r="5" spans="1:9" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="43" t="s">
+      <c r="B5" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="43"/>
-      <c r="D5" s="44"/>
-      <c r="F5" s="17" t="s">
+      <c r="C5" s="49"/>
+      <c r="D5" s="50"/>
+      <c r="F5" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="G5" s="43"/>
-      <c r="H5" s="43"/>
-      <c r="I5" s="44"/>
-    </row>
-    <row r="6" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="20" t="s">
+      <c r="G5" s="49" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="49"/>
+      <c r="I5" s="50"/>
+    </row>
+    <row r="6" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="7" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="16" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="9" t="s">
@@ -6096,10 +6113,10 @@
       <c r="C7" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="21" t="s">
+      <c r="D7" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="F7" s="16" t="s">
         <v>3</v>
       </c>
       <c r="G7" s="9" t="s">
@@ -6108,293 +6125,373 @@
       <c r="H7" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="I7" s="21" t="s">
+      <c r="I7" s="17" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="22"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="23"/>
-      <c r="F8" s="22" t="s">
+    <row r="8" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="18" t="s">
         <v>48</v>
       </c>
+      <c r="B8" s="6">
+        <v>45567</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="18" t="s">
+        <v>58</v>
+      </c>
       <c r="G8" s="6">
+        <v>45574</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I8" s="19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9" s="6">
         <v>45567</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="C9" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="6">
+        <v>45574</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I9" s="19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="6">
+        <v>45567</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" s="6">
+        <v>45574</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I10" s="19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="6">
+        <v>45567</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G11" s="6">
+        <v>45574</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="6">
+        <v>45567</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="G12" s="6">
+        <v>45574</v>
+      </c>
+      <c r="H12" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I8" s="23" t="s">
+      <c r="I12" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="6">
+        <v>45567</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="19" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="22"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="23"/>
-      <c r="F9" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="G9" s="6">
-        <v>45567</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="I9" s="23" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="22"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="23"/>
-      <c r="F10" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="G10" s="6">
-        <v>45567</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="I10" s="23" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="22"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="23"/>
-      <c r="F11" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="G11" s="6">
-        <v>45567</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I11" s="23" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="19"/>
-      <c r="D12" s="18"/>
-      <c r="F12" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="G12" s="6">
-        <v>45567</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I12" s="23" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" s="25"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="26"/>
-      <c r="F13" s="22" t="s">
-        <v>35</v>
+      <c r="F13" s="5" t="s">
+        <v>61</v>
       </c>
       <c r="G13" s="6">
-        <v>45567</v>
+        <v>45574</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="I13" s="23" t="s">
+      <c r="I13" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="30"/>
-      <c r="B14" s="31"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="32"/>
-      <c r="F14" s="22" t="s">
+    <row r="14" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="18" t="s">
         <v>34</v>
       </c>
+      <c r="B14" s="6">
+        <v>45567</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>62</v>
+      </c>
       <c r="G14" s="6">
+        <v>45574</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" s="6">
         <v>45567</v>
       </c>
-      <c r="H14" s="5" t="s">
+      <c r="C15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="I14" s="23" t="s">
+      <c r="D15" s="19" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="33"/>
-      <c r="B15" s="34"/>
-      <c r="C15" s="34"/>
-      <c r="D15" s="35"/>
-      <c r="F15" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="G15" s="6">
+    <row r="16" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="6">
         <v>45567</v>
       </c>
-      <c r="H15" s="5" t="s">
+      <c r="C16" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="6">
+        <v>45567</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="5"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+    </row>
+    <row r="19" spans="1:5" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="23"/>
+    </row>
+    <row r="20" spans="1:5" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" s="28"/>
+      <c r="C20" s="28"/>
+      <c r="D20" s="29"/>
+    </row>
+    <row r="21" spans="1:5" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="30"/>
+      <c r="B21" s="31"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="13"/>
+    </row>
+    <row r="22" spans="1:5" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="30"/>
+      <c r="B22" s="31"/>
+      <c r="C22" s="31"/>
+      <c r="D22" s="32"/>
+    </row>
+    <row r="23" spans="1:5" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="33"/>
+      <c r="B23" s="34"/>
+      <c r="C23" s="34"/>
+      <c r="D23" s="35"/>
+    </row>
+    <row r="24" spans="1:5" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A24"/>
+      <c r="B24"/>
+      <c r="C24"/>
+      <c r="D24"/>
+    </row>
+    <row r="25" spans="1:5" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="51" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" s="52"/>
+      <c r="C25" s="52"/>
+      <c r="D25" s="53"/>
+    </row>
+    <row r="26" spans="1:5" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" s="59"/>
+      <c r="C26" s="54" t="s">
+        <v>41</v>
+      </c>
+      <c r="D26" s="55"/>
+    </row>
+    <row r="27" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="60" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" s="56"/>
+      <c r="C27" s="56" t="s">
+        <v>42</v>
+      </c>
+      <c r="D27" s="57"/>
+    </row>
+    <row r="28" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="61" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28" s="45"/>
+      <c r="C28" s="45" t="s">
+        <v>43</v>
+      </c>
+      <c r="D28" s="46"/>
+    </row>
+    <row r="29" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="62" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" s="63"/>
+      <c r="C29" s="63" t="s">
+        <v>44</v>
+      </c>
+      <c r="D29" s="69"/>
+    </row>
+    <row r="30" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="64" t="s">
+        <v>11</v>
+      </c>
+      <c r="B30" s="65"/>
+      <c r="C30" s="65" t="s">
+        <v>45</v>
+      </c>
+      <c r="D30" s="70"/>
+    </row>
+    <row r="31" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="I15" s="23" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="33"/>
-      <c r="B16" s="34"/>
-      <c r="C16" s="34"/>
-      <c r="D16" s="35"/>
-      <c r="F16" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="G16" s="6">
-        <v>45567</v>
-      </c>
-      <c r="H16" s="5" t="s">
+      <c r="B31" s="63"/>
+      <c r="C31" s="63" t="s">
+        <v>46</v>
+      </c>
+      <c r="D31" s="69"/>
+    </row>
+    <row r="32" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A32" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="I16" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="36"/>
-      <c r="B17" s="37"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="38"/>
-      <c r="F17" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="G17" s="6">
-        <v>45567</v>
-      </c>
-      <c r="H17" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="I17" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="14"/>
-      <c r="B18"/>
-      <c r="C18"/>
-      <c r="D18" s="15"/>
-    </row>
-    <row r="19" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="45" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" s="46"/>
-      <c r="C19" s="46"/>
-      <c r="D19" s="47"/>
-      <c r="F19"/>
-      <c r="G19"/>
-    </row>
-    <row r="20" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="52" t="s">
-        <v>0</v>
-      </c>
-      <c r="B20" s="53"/>
-      <c r="C20" s="48" t="s">
-        <v>41</v>
-      </c>
-      <c r="D20" s="49"/>
-      <c r="E20" s="13"/>
-      <c r="F20"/>
-      <c r="G20"/>
-    </row>
-    <row r="21" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="54" t="s">
-        <v>8</v>
-      </c>
-      <c r="B21" s="50"/>
-      <c r="C21" s="50" t="s">
-        <v>42</v>
-      </c>
-      <c r="D21" s="51"/>
-    </row>
-    <row r="22" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="55" t="s">
-        <v>9</v>
-      </c>
-      <c r="B22" s="39"/>
-      <c r="C22" s="39" t="s">
-        <v>43</v>
-      </c>
-      <c r="D22" s="40"/>
-    </row>
-    <row r="23" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="56" t="s">
-        <v>10</v>
-      </c>
-      <c r="B23" s="57"/>
-      <c r="C23" s="57" t="s">
-        <v>44</v>
-      </c>
-      <c r="D23" s="63"/>
-    </row>
-    <row r="24" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="58" t="s">
-        <v>11</v>
-      </c>
-      <c r="B24" s="59"/>
-      <c r="C24" s="59" t="s">
-        <v>45</v>
-      </c>
-      <c r="D24" s="64"/>
-    </row>
-    <row r="25" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="56" t="s">
-        <v>12</v>
-      </c>
-      <c r="B25" s="57"/>
-      <c r="C25" s="57" t="s">
-        <v>46</v>
-      </c>
-      <c r="D25" s="63"/>
-    </row>
-    <row r="26" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="60" t="s">
-        <v>13</v>
-      </c>
-      <c r="B26" s="61"/>
-      <c r="C26" s="61" t="s">
+      <c r="B32" s="67"/>
+      <c r="C32" s="67" t="s">
         <v>47</v>
       </c>
-      <c r="D26" s="62"/>
+      <c r="D32" s="68"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <mergeCells count="24">
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="A13:D13"/>
-    <mergeCell ref="A14:D17"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A20:D23"/>
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="B4:D4"/>
@@ -6402,56 +6499,50 @@
     <mergeCell ref="G4:I4"/>
     <mergeCell ref="G5:I5"/>
     <mergeCell ref="F3:I3"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
-  <conditionalFormatting sqref="D8:D11 I8:I17">
-    <cfRule type="cellIs" dxfId="20" priority="6" operator="equal">
+  <conditionalFormatting sqref="I8:I14 D8:D18">
+    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="7" operator="equal">
       <formula>"Em Andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="8" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8:C11" xr:uid="{8EFBC24D-2650-46F5-BA77-660A84572B57}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B5" xr:uid="{2E14A627-A508-4036-9948-768B809E3863}">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" scale="56" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="55" orientation="landscape" r:id="rId1"/>
   <tableParts count="2">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{170DC6ED-100C-48FE-A29D-3864A9024536}">
           <x14:formula1>
             <xm:f>'BANCO DE DADOS'!$B$1:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>D8:D11 I8:I17</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2E14A627-A508-4036-9948-768B809E3863}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>B4:B5 G4:G5 G20</xm:sqref>
+          <xm:sqref>D8:D18 I8:I14</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CB2ECE66-384A-4231-9DE0-EE40A3A51602}">
           <x14:formula1>
             <xm:f>Quinta!$A$25:$A$30</xm:f>
           </x14:formula1>
-          <xm:sqref>H8:H17</xm:sqref>
+          <xm:sqref>G4:I5 C8:C18 H8:H14</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Alterações no Backlog e na API
</commit_message>
<xml_diff>
--- a/ATAs_de_Reuniao/Sprint 2/Semana 2609/Grupo4_ATA_Semana2609.xlsx
+++ b/ATAs_de_Reuniao/Sprint 2/Semana 2609/Grupo4_ATA_Semana2609.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Documents\Projeto_PI\sprint2\ATAs_de_Reuniao\Sprint 2\Semana 2609\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6F518FD-4945-4C35-9346-D14FF8571FDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32C806C3-B041-4C8A-892E-FDC3C27CB3AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="7" xr2:uid="{D70EAD62-B489-48DA-AED6-4403B2320B59}"/>
   </bookViews>
@@ -922,6 +922,33 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -971,33 +998,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="8" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="8" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="8" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="8" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="8" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="8" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -6020,8 +6020,8 @@
   </sheetPr>
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -6070,37 +6070,37 @@
       <c r="A4" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="47" t="s">
+      <c r="B4" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="47"/>
-      <c r="D4" s="48"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="57"/>
       <c r="F4" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="G4" s="47" t="s">
+      <c r="G4" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="47"/>
-      <c r="I4" s="48"/>
+      <c r="H4" s="56"/>
+      <c r="I4" s="57"/>
     </row>
     <row r="5" spans="1:9" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="49" t="s">
+      <c r="B5" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="49"/>
-      <c r="D5" s="50"/>
+      <c r="C5" s="58"/>
+      <c r="D5" s="59"/>
       <c r="F5" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="G5" s="49" t="s">
+      <c r="G5" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="49"/>
-      <c r="I5" s="50"/>
+      <c r="H5" s="58"/>
+      <c r="I5" s="59"/>
     </row>
     <row r="6" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="7" spans="1:9" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
@@ -6401,94 +6401,86 @@
       <c r="D24"/>
     </row>
     <row r="25" spans="1:5" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="51" t="s">
+      <c r="A25" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="52"/>
-      <c r="C25" s="52"/>
-      <c r="D25" s="53"/>
+      <c r="B25" s="61"/>
+      <c r="C25" s="61"/>
+      <c r="D25" s="62"/>
     </row>
     <row r="26" spans="1:5" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="58" t="s">
+      <c r="A26" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="B26" s="59"/>
-      <c r="C26" s="54" t="s">
+      <c r="B26" s="68"/>
+      <c r="C26" s="63" t="s">
         <v>41</v>
       </c>
-      <c r="D26" s="55"/>
+      <c r="D26" s="64"/>
     </row>
     <row r="27" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="60" t="s">
+      <c r="A27" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="B27" s="56"/>
-      <c r="C27" s="56" t="s">
+      <c r="B27" s="65"/>
+      <c r="C27" s="65" t="s">
         <v>42</v>
       </c>
-      <c r="D27" s="57"/>
+      <c r="D27" s="66"/>
     </row>
     <row r="28" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="61" t="s">
+      <c r="A28" s="70" t="s">
         <v>9</v>
       </c>
-      <c r="B28" s="45"/>
-      <c r="C28" s="45" t="s">
+      <c r="B28" s="54"/>
+      <c r="C28" s="54" t="s">
         <v>43</v>
       </c>
-      <c r="D28" s="46"/>
+      <c r="D28" s="55"/>
     </row>
     <row r="29" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="62" t="s">
+      <c r="A29" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="B29" s="63"/>
-      <c r="C29" s="63" t="s">
+      <c r="B29" s="46"/>
+      <c r="C29" s="46" t="s">
         <v>44</v>
       </c>
-      <c r="D29" s="69"/>
+      <c r="D29" s="52"/>
     </row>
     <row r="30" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="64" t="s">
+      <c r="A30" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="B30" s="65"/>
-      <c r="C30" s="65" t="s">
+      <c r="B30" s="48"/>
+      <c r="C30" s="48" t="s">
         <v>45</v>
       </c>
-      <c r="D30" s="70"/>
+      <c r="D30" s="53"/>
     </row>
     <row r="31" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="62" t="s">
+      <c r="A31" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="B31" s="63"/>
-      <c r="C31" s="63" t="s">
+      <c r="B31" s="46"/>
+      <c r="C31" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="D31" s="69"/>
+      <c r="D31" s="52"/>
     </row>
     <row r="32" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="66" t="s">
+      <c r="A32" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="B32" s="67"/>
-      <c r="C32" s="67" t="s">
+      <c r="B32" s="50"/>
+      <c r="C32" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="D32" s="68"/>
+      <c r="D32" s="51"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <mergeCells count="24">
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="A31:B31"/>
     <mergeCell ref="C28:D28"/>
     <mergeCell ref="A19:D19"/>
     <mergeCell ref="A20:D23"/>
@@ -6505,6 +6497,14 @@
     <mergeCell ref="A26:B26"/>
     <mergeCell ref="A27:B27"/>
     <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="A31:B31"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="I8:I14 D8:D18">

</xml_diff>